<commit_message>
asset methods to buy, sell, update porfolios and values, and functions for RSI and sma,ema,wma
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\OneDrive\PET PROJECTS\Al-the-Trader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{0F1EDEEF-C5AC-42F7-94BD-610EF81928D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{4E0D7944-E2F1-4312-897C-7709F46D0244}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{0F1EDEEF-C5AC-42F7-94BD-610EF81928D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{FEE645C1-E02D-4059-9FAA-B33B73156C66}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{1F250315-142D-43F1-84A9-3B10F3F4598B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{1F250315-142D-43F1-84A9-3B10F3F4598B}"/>
   </bookViews>
   <sheets>
     <sheet name="watchlist" sheetId="1" r:id="rId1"/>
-    <sheet name="portfolio" sheetId="2" r:id="rId2"/>
+    <sheet name="stocks" sheetId="2" r:id="rId2"/>
+    <sheet name="portfolio" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>MSFT</t>
   </si>
@@ -62,6 +63,15 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>CASH</t>
+  </si>
+  <si>
+    <t>asset</t>
+  </si>
+  <si>
+    <t>STOCKS</t>
   </si>
 </sst>
 </file>
@@ -416,7 +426,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,27 +470,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3993D2E-37EB-47A1-AD85-39D7337DC3A7}">
   <dimension ref="A1:E1"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF103F3-2CB5-4F30-9120-6766BA818176}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initialize trade testing via RSI, 1 share
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\OneDrive\PET PROJECTS\Al-the-Trader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{0F1EDEEF-C5AC-42F7-94BD-610EF81928D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{FEE645C1-E02D-4059-9FAA-B33B73156C66}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{0F1EDEEF-C5AC-42F7-94BD-610EF81928D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{C502F530-19FA-47D1-9F3B-8122F789F101}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{1F250315-142D-43F1-84A9-3B10F3F4598B}"/>
+    <workbookView xWindow="22932" yWindow="2784" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{1F250315-142D-43F1-84A9-3B10F3F4598B}"/>
   </bookViews>
   <sheets>
     <sheet name="watchlist" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>AAPL</t>
   </si>
   <si>
-    <t>GOOG</t>
-  </si>
-  <si>
     <t>NVDA</t>
   </si>
   <si>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>STOCKS</t>
+  </si>
+  <si>
+    <t>GOOGL</t>
   </si>
 </sst>
 </file>
@@ -425,15 +425,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194368C9-511D-45B6-9535-A3EACA883C9F}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -448,17 +448,17 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -470,7 +470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3993D2E-37EB-47A1-AD85-39D7337DC3A7}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -479,19 +479,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -503,23 +503,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF103F3-2CB5-4F30-9120-6766BA818176}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>10000</v>
@@ -527,7 +527,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added trades history sheet and asset method
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -10,6 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="watchlist" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="stocks" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="portfolio" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="trades" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -520,4 +521,50 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ticker</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>buy_sell</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>shares</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
trasferred trades history logic to main script, fixed workbook updating
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -1,40 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\OneDrive\PET PROJECTS\Al-the-Trader\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_7EBCB87E1082D1F7837DEA47725D37B3577E973D" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D7DB0AA3-FB57-41AA-B76A-321B442DE5AE}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="watchlist" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="stocks" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="portfolio" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="trades" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="portfolio" sheetId="3" r:id="rId1"/>
+    <sheet name="watchlist" sheetId="1" r:id="rId2"/>
+    <sheet name="stocks" sheetId="2" r:id="rId3"/>
+    <sheet name="trades" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+  <si>
+    <t>ticker</t>
+  </si>
+  <si>
+    <t>MSFT</t>
+  </si>
+  <si>
+    <t>AAPL</t>
+  </si>
+  <si>
+    <t>GOOGL</t>
+  </si>
+  <si>
+    <t>ZM</t>
+  </si>
+  <si>
+    <t>current_price</t>
+  </si>
+  <si>
+    <t>shares</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>current_rsi</t>
+  </si>
+  <si>
+    <t>last_activity</t>
+  </si>
+  <si>
+    <t>asset</t>
+  </si>
+  <si>
+    <t>CASH</t>
+  </si>
+  <si>
+    <t>STOCKS</t>
+  </si>
+  <si>
+    <t>buy_sell</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,10 +105,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -60,15 +124,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -356,64 +429,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>ticker</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
         <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>MSFT</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>AAPL</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>GOOGL</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>ZM</t>
-        </is>
       </c>
     </row>
   </sheetData>
@@ -422,49 +466,83 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ticker</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>current_price</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>shares</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>current_rsi</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>last_activity</t>
-        </is>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -472,99 +550,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8779B27A-E9EE-4629-A1FD-2006C4D58462}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>asset</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>CASH</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>STOCKS</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="B1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>ticker</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>buy_sell</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>shares</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
complete new trade mechanics
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -474,16 +474,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>172.15</v>
+        <v>177.36</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>172.15</v>
+        <v>177.36</v>
       </c>
       <c r="E2" t="n">
-        <v>45.77932342712615</v>
+        <v>54.94932666944332</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -498,16 +498,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>278.98</v>
+        <v>295.7</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>278.98</v>
+        <v>295.7</v>
       </c>
       <c r="E3" t="n">
-        <v>56.93602034826844</v>
+        <v>53.4112618592753</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -522,16 +522,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1252.31</v>
+        <v>1334.05</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>1252.31</v>
+        <v>1334.05</v>
       </c>
       <c r="E4" t="n">
-        <v>55.25249561928622</v>
+        <v>57.45291685806153</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -587,7 +587,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1703</v>
+        <v>1807</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed portfolio total summing
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -786,7 +786,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -824,16 +824,6 @@
       </c>
       <c r="B3" t="n">
         <v>137</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>9998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
simple formula for number of shares per trade
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -737,10 +737,10 @@
         <v>96.05</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>96.05</v>
+        <v>960.5</v>
       </c>
       <c r="E2" t="n">
         <v>24.71111111111112</v>
@@ -761,10 +761,10 @@
         <v>41.66</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D3" t="n">
-        <v>41.66</v>
+        <v>999.8399999999999</v>
       </c>
       <c r="E3" t="n">
         <v>28.55110749847591</v>
@@ -813,7 +813,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9861</v>
+        <v>8039.66</v>
       </c>
     </row>
     <row r="3">
@@ -823,7 +823,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>137</v>
+        <v>1960.34</v>
       </c>
     </row>
   </sheetData>
@@ -878,7 +878,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>01/05/2020 16:42:28</t>
+          <t>01/05/2020 17:43:50</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -892,10 +892,10 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>96.05</v>
+        <v>960.5</v>
       </c>
     </row>
     <row r="3">
@@ -904,7 +904,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>01/05/2020 16:42:30</t>
+          <t>01/05/2020 17:43:52</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -918,10 +918,10 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F3" t="n">
-        <v>41.66</v>
+        <v>999.8399999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor adjustment and notes
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -395,65 +395,65 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>TRV</t>
+          <t>WBA</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>97.17</v>
+        <v>42.02</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2683</v>
+        <v>-1.013</v>
       </c>
       <c r="D2" t="n">
-        <v>22.80341880341881</v>
+        <v>25.58558558558559</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>WBA</t>
+          <t>RTX</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>42.03</v>
+        <v>59</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.9893999999999999</v>
+        <v>0.2549</v>
       </c>
       <c r="D3" t="n">
-        <v>25.6317689530686</v>
+        <v>29.25180519280995</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>RTX</t>
+          <t>CAT</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>59.05</v>
+        <v>108.91</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3398</v>
+        <v>1.1047</v>
       </c>
       <c r="D4" t="n">
-        <v>29.46852504211977</v>
+        <v>30.06517427033153</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>CAT</t>
+          <t>TRV</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>109.31</v>
+        <v>96.84999999999999</v>
       </c>
       <c r="C5" t="n">
-        <v>1.476</v>
+        <v>-0.0619</v>
       </c>
       <c r="D5" t="n">
-        <v>30.8489773045671</v>
+        <v>31.12028158757131</v>
       </c>
     </row>
     <row r="6">
@@ -463,13 +463,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>124.84</v>
+        <v>124.73</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9216</v>
+        <v>0.8327</v>
       </c>
       <c r="D6" t="n">
-        <v>32.40740740740742</v>
+        <v>31.82879377431907</v>
       </c>
     </row>
     <row r="7">
@@ -479,13 +479,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>56.58</v>
+        <v>56.51</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6046</v>
+        <v>0.4801</v>
       </c>
       <c r="D7" t="n">
-        <v>34.02061855670104</v>
+        <v>32.3943661971831</v>
       </c>
     </row>
     <row r="8">
@@ -495,13 +495,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>116.11</v>
+        <v>116.01</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2937</v>
+        <v>0.2073</v>
       </c>
       <c r="D8" t="n">
-        <v>36.39185926181442</v>
+        <v>35.27553527553528</v>
       </c>
     </row>
     <row r="9">
@@ -511,13 +511,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>180.1</v>
+        <v>179.24</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.9732</v>
+        <v>-1.4461</v>
       </c>
       <c r="D9" t="n">
-        <v>37.27108589115296</v>
+        <v>35.68782415411212</v>
       </c>
     </row>
     <row r="10">
@@ -527,13 +527,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>58.71</v>
+        <v>58.75</v>
       </c>
       <c r="C10" t="n">
-        <v>1.2416</v>
+        <v>1.3106</v>
       </c>
       <c r="D10" t="n">
-        <v>38.195427877807</v>
+        <v>38.39483766888486</v>
       </c>
     </row>
     <row r="11">
@@ -543,13 +543,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>33.34</v>
+        <v>33.37</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8469</v>
+        <v>0.9377</v>
       </c>
       <c r="D11" t="n">
-        <v>40.12219959266803</v>
+        <v>40.2439024390244</v>
       </c>
     </row>
     <row r="12">
@@ -559,13 +559,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>41.54</v>
+        <v>41.46</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4595</v>
+        <v>0.266</v>
       </c>
       <c r="D12" t="n">
-        <v>42.65298644192012</v>
+        <v>41.97256210604376</v>
       </c>
     </row>
     <row r="13">
@@ -575,13 +575,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>122.81</v>
+        <v>122.58</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9287</v>
+        <v>0.7396</v>
       </c>
       <c r="D13" t="n">
-        <v>42.84549531186302</v>
+        <v>42.30452674897119</v>
       </c>
     </row>
     <row r="14">
@@ -591,13 +591,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>93.20999999999999</v>
+        <v>92.89</v>
       </c>
       <c r="C14" t="n">
-        <v>1.9357</v>
+        <v>1.5857</v>
       </c>
       <c r="D14" t="n">
-        <v>43.48503740648379</v>
+        <v>42.91561712846347</v>
       </c>
     </row>
     <row r="15">
@@ -607,125 +607,125 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>125.86</v>
+        <v>125.4</v>
       </c>
       <c r="C15" t="n">
-        <v>-4.2599</v>
+        <v>-4.6098</v>
       </c>
       <c r="D15" t="n">
-        <v>43.8148814011483</v>
+        <v>43.35226946691915</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>XOM</t>
+          <t>DIS</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>44.86</v>
+        <v>101.06</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.0446</v>
+        <v>-2.0547</v>
       </c>
       <c r="D16" t="n">
-        <v>44.88888888888889</v>
+        <v>44.59847509654421</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>DIS</t>
+          <t>XOM</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>101.27</v>
+        <v>44.83</v>
       </c>
       <c r="C17" t="n">
-        <v>-1.8511</v>
+        <v>-0.1114</v>
       </c>
       <c r="D17" t="n">
-        <v>45.06704022413448</v>
+        <v>44.71853257432005</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>JPM</t>
+          <t>NKE</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>92.14</v>
+        <v>87.2</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>1.691</v>
       </c>
       <c r="D18" t="n">
-        <v>47.19350073855244</v>
+        <v>46.7005076142132</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>NKE</t>
+          <t>MRK</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>87.40000000000001</v>
+        <v>78.01000000000001</v>
       </c>
       <c r="C19" t="n">
-        <v>1.9242</v>
+        <v>1.4962</v>
       </c>
       <c r="D19" t="n">
-        <v>48.01980198019802</v>
+        <v>47.48294302046838</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>MRK</t>
+          <t>GS</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>78.18000000000001</v>
+        <v>178.3</v>
       </c>
       <c r="C20" t="n">
-        <v>1.7174</v>
+        <v>1.2896</v>
       </c>
       <c r="D20" t="n">
-        <v>48.29339143064634</v>
+        <v>48.03341454925166</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>GS</t>
+          <t>UNH</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>179.75</v>
+        <v>293.04</v>
       </c>
       <c r="C21" t="n">
-        <v>2.1133</v>
+        <v>1.9128</v>
       </c>
       <c r="D21" t="n">
-        <v>50.05018400802943</v>
+        <v>51.46884021056208</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>UNH</t>
+          <t>KO</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>293.16</v>
+        <v>45.4</v>
       </c>
       <c r="C22" t="n">
-        <v>1.9545</v>
+        <v>0.576</v>
       </c>
       <c r="D22" t="n">
-        <v>51.56753092696155</v>
+        <v>52.76156264032331</v>
       </c>
     </row>
     <row r="23">
@@ -735,29 +735,29 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>86.54000000000001</v>
+        <v>86.73999999999999</v>
       </c>
       <c r="C23" t="n">
-        <v>0.1852</v>
+        <v>0.4168</v>
       </c>
       <c r="D23" t="n">
-        <v>52.96033722935429</v>
+        <v>53.31812131583951</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>KO</t>
+          <t>JPM</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>45.58</v>
+        <v>92</v>
       </c>
       <c r="C24" t="n">
-        <v>0.9747</v>
+        <v>-0.1519</v>
       </c>
       <c r="D24" t="n">
-        <v>54.59646094087181</v>
+        <v>53.77090564846955</v>
       </c>
     </row>
     <row r="25">
@@ -767,13 +767,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>180.59</v>
+        <v>180.76</v>
       </c>
       <c r="C25" t="n">
-        <v>0.9785</v>
+        <v>1.0736</v>
       </c>
       <c r="D25" t="n">
-        <v>56.38297872340425</v>
+        <v>56.60719685515573</v>
       </c>
     </row>
     <row r="26">
@@ -783,13 +783,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>38.57</v>
+        <v>38.51</v>
       </c>
       <c r="C26" t="n">
-        <v>2.5253</v>
+        <v>2.3658</v>
       </c>
       <c r="D26" t="n">
-        <v>60</v>
+        <v>59.58188153310105</v>
       </c>
     </row>
     <row r="27">
@@ -799,13 +799,13 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>297.93</v>
+        <v>297.56</v>
       </c>
       <c r="C27" t="n">
-        <v>1.6271</v>
+        <v>1.5009</v>
       </c>
       <c r="D27" t="n">
-        <v>60.79245283018868</v>
+        <v>60.51681550446514</v>
       </c>
     </row>
     <row r="28">
@@ -815,13 +815,13 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>147.37</v>
+        <v>147.43</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.6941000000000001</v>
+        <v>-0.6536</v>
       </c>
       <c r="D28" t="n">
-        <v>63.08579668348955</v>
+        <v>63.22254335260115</v>
       </c>
     </row>
     <row r="29">
@@ -831,13 +831,13 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>149.91</v>
+        <v>149.5</v>
       </c>
       <c r="C29" t="n">
-        <v>1.1061</v>
+        <v>0.8296</v>
       </c>
       <c r="D29" t="n">
-        <v>66.78899082568807</v>
+        <v>64.44880923152468</v>
       </c>
     </row>
     <row r="30">
@@ -847,13 +847,13 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>179.05</v>
+        <v>178.44</v>
       </c>
       <c r="C30" t="n">
-        <v>1.6463</v>
+        <v>1.3</v>
       </c>
       <c r="D30" t="n">
-        <v>69.1006233303651</v>
+        <v>68.4143455306754</v>
       </c>
     </row>
     <row r="31">
@@ -863,13 +863,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>226.13</v>
+        <v>225.61</v>
       </c>
       <c r="C31" t="n">
-        <v>1.9338</v>
+        <v>1.6994</v>
       </c>
       <c r="D31" t="n">
-        <v>80.64085447263017</v>
+        <v>80.33750188338104</v>
       </c>
     </row>
   </sheetData>
@@ -943,19 +943,19 @@
         <v>96.05</v>
       </c>
       <c r="C2" t="n">
-        <v>97.17</v>
+        <v>96.84999999999999</v>
       </c>
       <c r="D2" t="n">
         <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>971.7</v>
+        <v>968.5</v>
       </c>
       <c r="F2" t="n">
-        <v>1.1661</v>
+        <v>0.8329</v>
       </c>
       <c r="G2" t="n">
-        <v>22.80341880341881</v>
+        <v>31.12028158757131</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -973,19 +973,19 @@
         <v>41.66</v>
       </c>
       <c r="C3" t="n">
-        <v>42.03</v>
+        <v>42.02</v>
       </c>
       <c r="D3" t="n">
         <v>24</v>
       </c>
       <c r="E3" t="n">
-        <v>1008.72</v>
+        <v>1008.48</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8881</v>
+        <v>0.8641</v>
       </c>
       <c r="G3" t="n">
-        <v>25.6317689530686</v>
+        <v>25.58558558558559</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1003,19 +1003,19 @@
         <v>110.2</v>
       </c>
       <c r="C4" t="n">
-        <v>109.31</v>
+        <v>108.91</v>
       </c>
       <c r="D4" t="n">
         <v>7</v>
       </c>
       <c r="E4" t="n">
-        <v>765.1700000000001</v>
+        <v>762.37</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.8076</v>
+        <v>-1.1706</v>
       </c>
       <c r="G4" t="n">
-        <v>30.8489773045671</v>
+        <v>30.06517427033153</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1029,27 +1029,23 @@
           <t>RTX</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
+      <c r="B5" t="n">
+        <v>59.04999999999999</v>
       </c>
       <c r="C5" t="n">
-        <v>59.05</v>
+        <v>59</v>
       </c>
       <c r="D5" t="n">
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>708.5999999999999</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
+        <v>708</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-0.0847</v>
       </c>
       <c r="G5" t="n">
-        <v>29.46852504211977</v>
+        <v>29.25180519280995</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1105,7 +1101,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3454.19</v>
+        <v>3447.35</v>
       </c>
     </row>
     <row r="4">
@@ -1115,7 +1111,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10013.85</v>
+        <v>10007.01</v>
       </c>
     </row>
   </sheetData>
@@ -1279,7 +1275,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1360,49 +1356,33 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>05/05/2020 14:07:43</t>
+          <t>05/05/2020 16:35:30</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7268.26</v>
+        <v>6559.66</v>
       </c>
       <c r="C5" t="n">
-        <v>2767.62</v>
+        <v>3447.35</v>
       </c>
       <c r="D5" t="n">
-        <v>10035.88</v>
+        <v>10007.01</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>05/05/2020 14:35:31</t>
+          <t>06/05/2020 06:20:52</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7268.26</v>
+        <v>6559.66</v>
       </c>
       <c r="C6" t="n">
-        <v>2762.52</v>
+        <v>3447.35</v>
       </c>
       <c r="D6" t="n">
-        <v>10030.78</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>05/05/2020 15:35:29</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>6559.66</v>
-      </c>
-      <c r="C7" t="n">
-        <v>3454.19</v>
-      </c>
-      <c r="D7" t="n">
-        <v>10013.85</v>
+        <v>10007.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comment GS for temp fix
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -395,129 +395,129 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>MMM</t>
+          <t>VZ</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>135.99</v>
+        <v>54.1</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.0955</v>
+        <v>0.2409</v>
       </c>
       <c r="D2" t="n">
-        <v>12.90172333488584</v>
+        <v>22.64150943396223</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>RTX</t>
+          <t>JNJ</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>53.86</v>
+        <v>144.37</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4476</v>
+        <v>-0.9127999999999999</v>
       </c>
       <c r="D3" t="n">
-        <v>14.05817174515236</v>
+        <v>34.71837488457984</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>TRV</t>
+          <t>PG</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>90.22</v>
+        <v>112.6</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4006</v>
+        <v>0.878</v>
       </c>
       <c r="D4" t="n">
-        <v>24.47747329307943</v>
+        <v>35.79304495335023</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>WBA</t>
+          <t>IBM</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>38.85</v>
+        <v>118.39</v>
       </c>
       <c r="C5" t="n">
-        <v>1.3038</v>
+        <v>-0.6128</v>
       </c>
       <c r="D5" t="n">
-        <v>25.65789473684217</v>
+        <v>37.52711496746203</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MCD</t>
+          <t>WBA</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>175.41</v>
+        <v>39.6</v>
       </c>
       <c r="C6" t="n">
-        <v>1.4987</v>
+        <v>-0.3774</v>
       </c>
       <c r="D6" t="n">
-        <v>26.49903288201159</v>
+        <v>40.31476997578689</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>IBM</t>
+          <t>CVX</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>116.95</v>
+        <v>90.28</v>
       </c>
       <c r="C7" t="n">
-        <v>1.0542</v>
+        <v>-1.9122</v>
       </c>
       <c r="D7" t="n">
-        <v>28.07570977917982</v>
+        <v>41.56706507304116</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>KO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>122.52</v>
+        <v>45.03</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8395</v>
+        <v>-0.3099</v>
       </c>
       <c r="D8" t="n">
-        <v>28.83295194508008</v>
+        <v>42.50000000000002</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>VZ</t>
+          <t>GS</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>54.91</v>
+        <v>179.93</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1094</v>
+        <v>-0.0944</v>
       </c>
       <c r="D9" t="n">
-        <v>28.97350993377476</v>
+        <v>42.81578947368421</v>
       </c>
     </row>
     <row r="10">
@@ -527,349 +527,349 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>87.52</v>
+        <v>89.47</v>
       </c>
       <c r="C10" t="n">
-        <v>4.1533</v>
+        <v>-0.7763</v>
       </c>
       <c r="D10" t="n">
-        <v>29.48207171314741</v>
+        <v>43.44295574502638</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>CAT</t>
+          <t>XOM</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>106.19</v>
+        <v>44.6</v>
       </c>
       <c r="C11" t="n">
-        <v>1.6367</v>
+        <v>0.0898</v>
       </c>
       <c r="D11" t="n">
-        <v>30.120952009364</v>
+        <v>46.83544303797471</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>KO</t>
+          <t>MSFT</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>43.7</v>
+        <v>183.51</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.5462</v>
+        <v>0.0436</v>
       </c>
       <c r="D12" t="n">
-        <v>30.89005235602093</v>
+        <v>48.37438423645321</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>PG</t>
+          <t>MMM</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>113.81</v>
+        <v>146.44</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.09660000000000001</v>
+        <v>0.4321</v>
       </c>
       <c r="D13" t="n">
-        <v>33.22314049586778</v>
+        <v>49.00813008130079</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>DOW</t>
+          <t>AXP</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>33.51</v>
+        <v>89.33</v>
       </c>
       <c r="C14" t="n">
-        <v>3.5858</v>
+        <v>-0.5566</v>
       </c>
       <c r="D14" t="n">
-        <v>35.35911602209943</v>
+        <v>49.72624798711755</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>XOM</t>
+          <t>MRK</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>42.3</v>
+        <v>76.37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8824</v>
+        <v>-0.2351</v>
       </c>
       <c r="D15" t="n">
-        <v>35.99999999999997</v>
+        <v>49.82896237172177</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>JNJ</t>
+          <t>CAT</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>147.64</v>
+        <v>112.47</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3466</v>
+        <v>-1.394</v>
       </c>
       <c r="D16" t="n">
-        <v>36.54708520179367</v>
+        <v>50.64423765211167</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>GS</t>
+          <t>PFE</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>174.45</v>
+        <v>37.5</v>
       </c>
       <c r="C17" t="n">
-        <v>1.5425</v>
+        <v>0.6441</v>
       </c>
       <c r="D17" t="n">
-        <v>37.45454545454545</v>
+        <v>53.24074074074074</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>AXP</t>
+          <t>UNH</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>83.81</v>
+        <v>289.94</v>
       </c>
       <c r="C18" t="n">
-        <v>7.4074</v>
+        <v>1.0561</v>
       </c>
       <c r="D18" t="n">
-        <v>37.890625</v>
+        <v>53.94948952176249</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>DIS</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>105.91</v>
+        <v>137.53</v>
       </c>
       <c r="C19" t="n">
-        <v>2.9052</v>
+        <v>-1.0576</v>
       </c>
       <c r="D19" t="n">
-        <v>45.48022598870055</v>
+        <v>54.45048966267682</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>CVX</t>
+          <t>TRV</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>90.05</v>
+        <v>100.1</v>
       </c>
       <c r="C20" t="n">
-        <v>1.522</v>
+        <v>0.9378</v>
       </c>
       <c r="D20" t="n">
-        <v>45.64537740062528</v>
+        <v>56.33608815426995</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>INTC</t>
+          <t>MCD</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>59.08</v>
+        <v>184.41</v>
       </c>
       <c r="C21" t="n">
-        <v>2.3207</v>
+        <v>-0.362</v>
       </c>
       <c r="D21" t="n">
-        <v>46.96312364425162</v>
+        <v>56.34477254588986</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>NKE</t>
+          <t>RTX</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>86.55</v>
+        <v>60</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6161</v>
+        <v>-0.1664</v>
       </c>
       <c r="D22" t="n">
-        <v>47.47393744987968</v>
+        <v>56.77655677655678</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>UNH</t>
+          <t>WMT</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>290.61</v>
+        <v>124.33</v>
       </c>
       <c r="C23" t="n">
-        <v>4.536</v>
+        <v>-0.528</v>
       </c>
       <c r="D23" t="n">
-        <v>48.19487577639751</v>
+        <v>57.11361310133061</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>PFE</t>
+          <t>V</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>37.92</v>
+        <v>190.86</v>
       </c>
       <c r="C24" t="n">
-        <v>2.3482</v>
+        <v>0.1259</v>
       </c>
       <c r="D24" t="n">
-        <v>49.48630136986306</v>
+        <v>59.50594121325831</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>DOW</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>180.53</v>
+        <v>36.12</v>
       </c>
       <c r="C25" t="n">
-        <v>0.4339</v>
+        <v>0.8375</v>
       </c>
       <c r="D25" t="n">
-        <v>52.68510984540275</v>
+        <v>60.32295271049597</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>MRK</t>
+          <t>HD</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>80.05</v>
+        <v>241.88</v>
       </c>
       <c r="C26" t="n">
-        <v>2.7731</v>
+        <v>0.4151</v>
       </c>
       <c r="D26" t="n">
-        <v>52.975691533948</v>
+        <v>60.68253513048464</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>INTC</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>180.9</v>
+        <v>62.26</v>
       </c>
       <c r="C27" t="n">
-        <v>2.1514</v>
+        <v>0.4518</v>
       </c>
       <c r="D27" t="n">
-        <v>55.13670256835133</v>
+        <v>61.55218554861729</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>CSCO</t>
+          <t>NKE</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>43.85</v>
+        <v>93.75</v>
       </c>
       <c r="C28" t="n">
-        <v>4.5292</v>
+        <v>-0.5411</v>
       </c>
       <c r="D28" t="n">
-        <v>59.48387096774193</v>
+        <v>61.64189667374379</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>WMT</t>
+          <t>AAPL</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>123.42</v>
+        <v>318.89</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.2344</v>
+        <v>0.6438</v>
       </c>
       <c r="D29" t="n">
-        <v>65.58441558441558</v>
+        <v>62.32414181204273</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>CSCO</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>309.54</v>
+        <v>44.9</v>
       </c>
       <c r="C30" t="n">
-        <v>0.6143</v>
+        <v>0.5824</v>
       </c>
       <c r="D30" t="n">
-        <v>70.312115999017</v>
+        <v>63.35664335664335</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>HD</t>
+          <t>DIS</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>234.48</v>
+        <v>118.02</v>
       </c>
       <c r="C31" t="n">
-        <v>1.9035</v>
+        <v>0.1612</v>
       </c>
       <c r="D31" t="n">
-        <v>71.8852703913952</v>
+        <v>64.53412073490814</v>
       </c>
     </row>
   </sheetData>
@@ -943,19 +943,19 @@
         <v>96.05</v>
       </c>
       <c r="C2" t="n">
-        <v>90.22</v>
+        <v>100.1</v>
       </c>
       <c r="D2" t="n">
         <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>902.2</v>
+        <v>1001</v>
       </c>
       <c r="F2" t="n">
-        <v>-6.0698</v>
+        <v>4.2166</v>
       </c>
       <c r="G2" t="n">
-        <v>24.47747329307943</v>
+        <v>56.33608815426995</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -973,19 +973,19 @@
         <v>41.66</v>
       </c>
       <c r="C3" t="n">
-        <v>38.85</v>
+        <v>39.6</v>
       </c>
       <c r="D3" t="n">
         <v>24</v>
       </c>
       <c r="E3" t="n">
-        <v>932.4000000000001</v>
+        <v>950.4000000000001</v>
       </c>
       <c r="F3" t="n">
-        <v>-6.7451</v>
+        <v>-4.9448</v>
       </c>
       <c r="G3" t="n">
-        <v>25.65789473684217</v>
+        <v>40.31476997578689</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1003,19 +1003,19 @@
         <v>110.2</v>
       </c>
       <c r="C4" t="n">
-        <v>106.19</v>
+        <v>112.47</v>
       </c>
       <c r="D4" t="n">
         <v>7</v>
       </c>
       <c r="E4" t="n">
-        <v>743.3299999999999</v>
+        <v>787.29</v>
       </c>
       <c r="F4" t="n">
-        <v>-3.6388</v>
+        <v>2.0599</v>
       </c>
       <c r="G4" t="n">
-        <v>30.120952009364</v>
+        <v>50.64423765211167</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1033,19 +1033,19 @@
         <v>59.04999999999999</v>
       </c>
       <c r="C5" t="n">
-        <v>53.86</v>
+        <v>60</v>
       </c>
       <c r="D5" t="n">
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>646.3199999999999</v>
+        <v>720</v>
       </c>
       <c r="F5" t="n">
-        <v>-8.789199999999999</v>
+        <v>1.6088</v>
       </c>
       <c r="G5" t="n">
-        <v>14.05817174515236</v>
+        <v>56.77655677655678</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1063,19 +1063,19 @@
         <v>56.55</v>
       </c>
       <c r="C6" t="n">
-        <v>54.91</v>
+        <v>54.1</v>
       </c>
       <c r="D6" t="n">
         <v>11</v>
       </c>
       <c r="E6" t="n">
-        <v>604.01</v>
+        <v>595.1</v>
       </c>
       <c r="F6" t="n">
-        <v>-2.9001</v>
+        <v>-4.3324</v>
       </c>
       <c r="G6" t="n">
-        <v>28.97350993377476</v>
+        <v>22.64150943396223</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -1093,19 +1093,19 @@
         <v>124.34</v>
       </c>
       <c r="C7" t="n">
-        <v>123.42</v>
+        <v>124.33</v>
       </c>
       <c r="D7" t="n">
         <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>370.26</v>
+        <v>372.99</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.7399</v>
+        <v>-0.008</v>
       </c>
       <c r="G7" t="n">
-        <v>65.58441558441558</v>
+        <v>57.11361310133061</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -1123,19 +1123,19 @@
         <v>114.6</v>
       </c>
       <c r="C8" t="n">
-        <v>113.81</v>
+        <v>112.6</v>
       </c>
       <c r="D8" t="n">
         <v>4</v>
       </c>
       <c r="E8" t="n">
-        <v>455.24</v>
+        <v>450.4</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.6894</v>
+        <v>-1.7452</v>
       </c>
       <c r="G8" t="n">
-        <v>33.22314049586778</v>
+        <v>35.79304495335023</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -1153,19 +1153,19 @@
         <v>77.91</v>
       </c>
       <c r="C9" t="n">
-        <v>80.05</v>
+        <v>76.37</v>
       </c>
       <c r="D9" t="n">
         <v>6</v>
       </c>
       <c r="E9" t="n">
-        <v>480.3</v>
+        <v>458.22</v>
       </c>
       <c r="F9" t="n">
-        <v>2.7468</v>
+        <v>-1.9766</v>
       </c>
       <c r="G9" t="n">
-        <v>52.975691533948</v>
+        <v>49.82896237172177</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -1183,19 +1183,19 @@
         <v>149.11</v>
       </c>
       <c r="C10" t="n">
-        <v>147.64</v>
+        <v>144.37</v>
       </c>
       <c r="D10" t="n">
         <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>442.92</v>
+        <v>433.11</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.9858</v>
+        <v>-3.1789</v>
       </c>
       <c r="G10" t="n">
-        <v>36.54708520179367</v>
+        <v>34.71837488457984</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -1213,19 +1213,19 @@
         <v>146.5</v>
       </c>
       <c r="C11" t="n">
-        <v>135.99</v>
+        <v>146.44</v>
       </c>
       <c r="D11" t="n">
         <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>271.98</v>
+        <v>292.88</v>
       </c>
       <c r="F11" t="n">
-        <v>-7.1741</v>
+        <v>-0.041</v>
       </c>
       <c r="G11" t="n">
-        <v>12.90172333488584</v>
+        <v>49.00813008130079</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -1243,19 +1243,19 @@
         <v>88.19</v>
       </c>
       <c r="C12" t="n">
-        <v>87.52</v>
+        <v>89.47</v>
       </c>
       <c r="D12" t="n">
         <v>4</v>
       </c>
       <c r="E12" t="n">
-        <v>350.08</v>
+        <v>357.88</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.7597</v>
+        <v>1.4514</v>
       </c>
       <c r="G12" t="n">
-        <v>29.48207171314741</v>
+        <v>43.44295574502638</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -1273,19 +1273,19 @@
         <v>176.54</v>
       </c>
       <c r="C13" t="n">
-        <v>175.41</v>
+        <v>184.41</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>175.41</v>
+        <v>184.41</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.6401</v>
+        <v>4.4579</v>
       </c>
       <c r="G13" t="n">
-        <v>26.49903288201159</v>
+        <v>56.34477254588986</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -1303,19 +1303,19 @@
         <v>33.09</v>
       </c>
       <c r="C14" t="n">
-        <v>33.51</v>
+        <v>36.12</v>
       </c>
       <c r="D14" t="n">
         <v>9</v>
       </c>
       <c r="E14" t="n">
-        <v>301.59</v>
+        <v>325.08</v>
       </c>
       <c r="F14" t="n">
-        <v>1.2693</v>
+        <v>9.1568</v>
       </c>
       <c r="G14" t="n">
-        <v>35.35911602209943</v>
+        <v>60.32295271049597</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1333,19 +1333,19 @@
         <v>118.9</v>
       </c>
       <c r="C15" t="n">
-        <v>116.95</v>
+        <v>118.39</v>
       </c>
       <c r="D15" t="n">
         <v>2</v>
       </c>
       <c r="E15" t="n">
-        <v>233.9</v>
+        <v>236.78</v>
       </c>
       <c r="F15" t="n">
-        <v>-1.64</v>
+        <v>-0.4289</v>
       </c>
       <c r="G15" t="n">
-        <v>28.07570977917982</v>
+        <v>37.52711496746203</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1363,19 +1363,19 @@
         <v>44.31</v>
       </c>
       <c r="C16" t="n">
-        <v>43.7</v>
+        <v>45.03</v>
       </c>
       <c r="D16" t="n">
         <v>6</v>
       </c>
       <c r="E16" t="n">
-        <v>262.2</v>
+        <v>270.18</v>
       </c>
       <c r="F16" t="n">
-        <v>-1.3767</v>
+        <v>1.6249</v>
       </c>
       <c r="G16" t="n">
-        <v>30.89005235602093</v>
+        <v>42.50000000000002</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1393,19 +1393,19 @@
         <v>80.66</v>
       </c>
       <c r="C17" t="n">
-        <v>83.81</v>
+        <v>89.33</v>
       </c>
       <c r="D17" t="n">
         <v>3</v>
       </c>
       <c r="E17" t="n">
-        <v>251.43</v>
+        <v>267.99</v>
       </c>
       <c r="F17" t="n">
-        <v>3.9053</v>
+        <v>10.7488</v>
       </c>
       <c r="G17" t="n">
-        <v>37.890625</v>
+        <v>49.72624798711755</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1423,19 +1423,19 @@
         <v>172.09</v>
       </c>
       <c r="C18" t="n">
-        <v>174.45</v>
+        <v>179.93</v>
       </c>
       <c r="D18" t="n">
         <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>174.45</v>
+        <v>179.93</v>
       </c>
       <c r="F18" t="n">
-        <v>1.3714</v>
+        <v>4.5558</v>
       </c>
       <c r="G18" t="n">
-        <v>37.45454545454545</v>
+        <v>42.81578947368421</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1453,19 +1453,19 @@
         <v>120.81</v>
       </c>
       <c r="C19" t="n">
-        <v>122.52</v>
+        <v>137.53</v>
       </c>
       <c r="D19" t="n">
         <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>122.52</v>
+        <v>137.53</v>
       </c>
       <c r="F19" t="n">
-        <v>1.4154</v>
+        <v>13.8399</v>
       </c>
       <c r="G19" t="n">
-        <v>28.83295194508008</v>
+        <v>54.45048966267682</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1483,19 +1483,19 @@
         <v>57.43</v>
       </c>
       <c r="C20" t="n">
-        <v>59.08</v>
+        <v>62.26</v>
       </c>
       <c r="D20" t="n">
         <v>3</v>
       </c>
       <c r="E20" t="n">
-        <v>177.24</v>
+        <v>186.78</v>
       </c>
       <c r="F20" t="n">
-        <v>2.8731</v>
+        <v>8.4102</v>
       </c>
       <c r="G20" t="n">
-        <v>46.96312364425162</v>
+        <v>61.55218554861729</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1551,7 +1551,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7897.78</v>
+        <v>8207.950000000001</v>
       </c>
     </row>
     <row r="4">
@@ -1561,7 +1561,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9756.32</v>
+        <v>10066.49</v>
       </c>
     </row>
   </sheetData>
@@ -2141,7 +2141,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2379,6 +2379,22 @@
         <v>9756.32</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>25/05/2020 07:36:29</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1858.54</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8207.950000000001</v>
+      </c>
+      <c r="D15" t="n">
+        <v>10066.49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
temp manual sell order functionality
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -399,13 +399,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>35.46</v>
+        <v>36.16</v>
       </c>
       <c r="C2" t="n">
-        <v>-7.1485</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>26.81451612903231</v>
+        <v>34.67741935483868</v>
       </c>
     </row>
     <row r="3">
@@ -415,13 +415,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>123.96</v>
+        <v>123.47</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.0806</v>
+        <v>-0.3792</v>
       </c>
       <c r="D3" t="n">
-        <v>39.66597077244257</v>
+        <v>36.87943262411344</v>
       </c>
     </row>
     <row r="4">
@@ -431,29 +431,29 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>147.19</v>
+        <v>148.65</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.0487</v>
+        <v>0.2698</v>
       </c>
       <c r="D4" t="n">
-        <v>40.0718778077268</v>
+        <v>52.99455535390197</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>MRK</t>
+          <t>INTC</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>79.56</v>
+        <v>61.93</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.4371</v>
+        <v>-0.3059</v>
       </c>
       <c r="D5" t="n">
-        <v>48.76681614349776</v>
+        <v>58.10276679841898</v>
       </c>
     </row>
     <row r="6">
@@ -463,381 +463,379 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>182.83</v>
+        <v>185.36</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.2292</v>
+        <v>0.2434</v>
       </c>
       <c r="D6" t="n">
-        <v>50.70643642072217</v>
+        <v>59.15032679738569</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>VZ</t>
+          <t>CSCO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>55.78</v>
+        <v>46.94</v>
       </c>
       <c r="C7" t="n">
-        <v>-2.7884</v>
+        <v>0.1066</v>
       </c>
       <c r="D7" t="n">
-        <v>56.88545688545689</v>
+        <v>64.91677336747762</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>PG</t>
+          <t>DIS</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>117.25</v>
+        <v>122.18</v>
       </c>
       <c r="C8" t="n">
-        <v>1.1473</v>
+        <v>2.8884</v>
       </c>
       <c r="D8" t="n">
-        <v>58.8471849865952</v>
+        <v>68.08707735062529</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>CVX</t>
+          <t>VZ</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>92.79000000000001</v>
+        <v>56.83</v>
       </c>
       <c r="C9" t="n">
-        <v>1.1887</v>
+        <v>0.7624</v>
       </c>
       <c r="D9" t="n">
-        <v>61.04129263913826</v>
+        <v>68.93353941267382</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>CSCO</t>
+          <t>CVX</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>46.3</v>
+        <v>97.18000000000001</v>
       </c>
       <c r="C10" t="n">
-        <v>-3.1786</v>
+        <v>2.6296</v>
       </c>
       <c r="D10" t="n">
-        <v>62.06896551724136</v>
+        <v>69.83210912906611</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>HD</t>
+          <t>V</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>247.29</v>
+        <v>196.87</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.4789</v>
+        <v>0.2597</v>
       </c>
       <c r="D11" t="n">
-        <v>63.59289617486334</v>
+        <v>72.66143633071806</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>INTC</t>
+          <t>MRK</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>61.86</v>
+        <v>82.06</v>
       </c>
       <c r="C12" t="n">
-        <v>-1.7003</v>
+        <v>1.5092</v>
       </c>
       <c r="D12" t="n">
-        <v>65.32534246575341</v>
+        <v>74.53754080522313</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>DIS</t>
+          <t>IBM</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>118.77</v>
+        <v>129.05</v>
       </c>
       <c r="C13" t="n">
-        <v>1.2532</v>
+        <v>2.4206</v>
       </c>
       <c r="D13" t="n">
-        <v>67.10063335679101</v>
+        <v>76.10250297973778</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>XOM</t>
+          <t>WBA</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>46.28</v>
+        <v>43.61</v>
       </c>
       <c r="C14" t="n">
-        <v>1.7814</v>
+        <v>0.1378</v>
       </c>
       <c r="D14" t="n">
-        <v>69.27927927927927</v>
+        <v>76.66666666666666</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>CAT</t>
+          <t>RTX</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>120.5</v>
+        <v>67.47</v>
       </c>
       <c r="C15" t="n">
-        <v>0.308</v>
+        <v>6.4196</v>
       </c>
       <c r="D15" t="n">
-        <v>71.33649932157394</v>
+        <v>76.84507042253522</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>IBM</t>
+          <t>AXP</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>124.89</v>
+        <v>105.4</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.008</v>
+        <v>6.3894</v>
       </c>
       <c r="D16" t="n">
-        <v>71.41310232809961</v>
+        <v>77.26999398677087</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>JPM</t>
+          <t>AAPL</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>98.59999999999999</v>
+        <v>325.12</v>
       </c>
       <c r="C17" t="n">
-        <v>1.3257</v>
+        <v>0.5505</v>
       </c>
       <c r="D17" t="n">
-        <v>72.59786476868327</v>
+        <v>77.62915129151303</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>KO</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>194.35</v>
+        <v>47.9</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.4558</v>
+        <v>2.1322</v>
       </c>
       <c r="D18" t="n">
-        <v>72.66277128547576</v>
+        <v>77.63157894736835</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>AXP</t>
+          <t>GS</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>96.75</v>
+        <v>210.57</v>
       </c>
       <c r="C19" t="n">
-        <v>1.7671</v>
+        <v>3.1498</v>
       </c>
       <c r="D19" t="n">
-        <v>72.73865414710484</v>
+        <v>77.93000990425882</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>GS</t>
+          <t>PG</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>199.93</v>
+        <v>118.53</v>
       </c>
       <c r="C20" t="n">
-        <v>1.7507</v>
+        <v>0.3981</v>
       </c>
       <c r="D20" t="n">
-        <v>72.78986074166795</v>
+        <v>78.11634349030477</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>JPM</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>321.85</v>
+        <v>104.27</v>
       </c>
       <c r="C21" t="n">
-        <v>1.2298</v>
+        <v>5.3978</v>
       </c>
       <c r="D21" t="n">
-        <v>75.72780203784582</v>
+        <v>78.42565597667638</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>KO</t>
+          <t>XOM</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>46.99</v>
+        <v>49.24</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6641</v>
+        <v>4.0795</v>
       </c>
       <c r="D22" t="n">
-        <v>76.1570827489481</v>
+        <v>78.43347639484981</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>WBA</t>
+          <t>CAT</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>43.3</v>
+        <v>127.09</v>
       </c>
       <c r="C23" t="n">
-        <v>0.8384</v>
+        <v>3.0571</v>
       </c>
       <c r="D23" t="n">
-        <v>76.78391959798998</v>
+        <v>78.83211678832116</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>UNH</t>
+          <t>MMM</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>305.93</v>
+        <v>161.21</v>
       </c>
       <c r="C24" t="n">
-        <v>0.3543</v>
+        <v>2.2647</v>
       </c>
       <c r="D24" t="n">
-        <v>76.85683530678153</v>
+        <v>79.48823772183246</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>DOW</t>
+          <t>HD</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>38.61</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.0259</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="C25" t="inlineStr"/>
       <c r="D25" t="n">
-        <v>79.55974842767294</v>
+        <v>83.98492699010842</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>UNH</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>151.39</v>
+        <v>305.35</v>
       </c>
       <c r="C26" t="n">
-        <v>3.7984</v>
+        <v>-0.3134</v>
       </c>
       <c r="D26" t="n">
-        <v>80.02678400612206</v>
+        <v>86.22222222222234</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>MMM</t>
+          <t>NKE</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>155.58</v>
+        <v>104.11</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.5497</v>
+        <v>3.3452</v>
       </c>
       <c r="D27" t="n">
-        <v>80.4674457429048</v>
+        <v>88.48230353929206</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>RTX</t>
+          <t>DOW</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>64.12</v>
+        <v>41.63</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.62</v>
+        <v>2.5369</v>
       </c>
       <c r="D28" t="n">
-        <v>81.34287286736382</v>
+        <v>89.59330143540673</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>NKE</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>99.54000000000001</v>
+        <v>173.16</v>
       </c>
       <c r="C29" t="n">
-        <v>0.9738</v>
+        <v>12.9476</v>
       </c>
       <c r="D29" t="n">
-        <v>88.44069837447314</v>
+        <v>89.85074626865672</v>
       </c>
     </row>
     <row r="30">
@@ -847,13 +845,13 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>187.41</v>
+        <v>193.29</v>
       </c>
       <c r="C30" t="n">
-        <v>0.585</v>
+        <v>3.0385</v>
       </c>
       <c r="D30" t="n">
-        <v>89.00052882072984</v>
+        <v>90.18867924528304</v>
       </c>
     </row>
     <row r="31">
@@ -863,13 +861,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>109.15</v>
+        <v>114.47</v>
       </c>
       <c r="C31" t="n">
-        <v>2.0284</v>
+        <v>3.1261</v>
       </c>
       <c r="D31" t="n">
-        <v>89.05472636815921</v>
+        <v>97.2792149866191</v>
       </c>
     </row>
   </sheetData>
@@ -883,7 +881,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -943,19 +941,19 @@
         <v>56.55</v>
       </c>
       <c r="C2" t="n">
-        <v>55.78</v>
+        <v>56.83</v>
       </c>
       <c r="D2" t="n">
         <v>11</v>
       </c>
       <c r="E2" t="n">
-        <v>613.58</v>
+        <v>625.13</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.3616</v>
+        <v>0.4951</v>
       </c>
       <c r="G2" t="n">
-        <v>56.88545688545689</v>
+        <v>68.93353941267382</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -970,52 +968,52 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>124.34</v>
+        <v>123.94</v>
       </c>
       <c r="C3" t="n">
-        <v>123.96</v>
+        <v>123.47</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E3" t="n">
-        <v>371.88</v>
+        <v>987.76</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.3056</v>
+        <v>-0.3792</v>
       </c>
       <c r="G3" t="n">
-        <v>39.66597077244257</v>
+        <v>36.87943262411344</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>PG</t>
+          <t>JNJ</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>114.6</v>
+        <v>149.11</v>
       </c>
       <c r="C4" t="n">
-        <v>117.25</v>
+        <v>148.65</v>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>469</v>
+        <v>445.95</v>
       </c>
       <c r="F4" t="n">
-        <v>2.3124</v>
+        <v>-0.3085</v>
       </c>
       <c r="G4" t="n">
-        <v>58.8471849865952</v>
+        <v>52.99455535390197</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1026,90 +1024,28 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>MRK</t>
+          <t>PFE</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>77.91</v>
+        <v>35.46</v>
       </c>
       <c r="C5" t="n">
-        <v>79.56</v>
+        <v>36.16</v>
       </c>
       <c r="D5" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="E5" t="n">
-        <v>477.36</v>
+        <v>831.6799999999999</v>
       </c>
       <c r="F5" t="n">
-        <v>2.1178</v>
+        <v>1.9741</v>
       </c>
       <c r="G5" t="n">
-        <v>48.76681614349776</v>
+        <v>34.67741935483868</v>
       </c>
       <c r="H5" t="inlineStr">
-        <is>
-          <t>buy</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>JNJ</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>149.11</v>
-      </c>
-      <c r="C6" t="n">
-        <v>147.19</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3</v>
-      </c>
-      <c r="E6" t="n">
-        <v>441.57</v>
-      </c>
-      <c r="F6" t="n">
-        <v>-1.2876</v>
-      </c>
-      <c r="G6" t="n">
-        <v>40.0718778077268</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>buy</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>PFE</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>35.46</v>
-      </c>
-      <c r="C7" t="n">
-        <v>35.46</v>
-      </c>
-      <c r="D7" t="n">
-        <v>23</v>
-      </c>
-      <c r="E7" t="n">
-        <v>815.58</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>26.81451612903231</v>
-      </c>
-      <c r="H7" t="inlineStr">
         <is>
           <t>buy</t>
         </is>
@@ -1153,7 +1089,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7386.940000000001</v>
+        <v>7733.720000000001</v>
       </c>
     </row>
     <row r="3">
@@ -1163,7 +1099,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3188.97</v>
+        <v>2890.52</v>
       </c>
     </row>
     <row r="4">
@@ -1173,7 +1109,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10575.91</v>
+        <v>10624.24</v>
       </c>
     </row>
   </sheetData>
@@ -1187,7 +1123,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2182,6 +2118,84 @@
       </c>
       <c r="F38" t="n">
         <v>815.58</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>02/06/2020 18:50:13</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>WMT</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>5</v>
+      </c>
+      <c r="F39" t="n">
+        <v>619.7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>03/06/2020 18:22:42</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>4</v>
+      </c>
+      <c r="F40" t="n">
+        <v>474.12</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>03/06/2020 18:22:42</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>MRK</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>6</v>
+      </c>
+      <c r="F41" t="n">
+        <v>492.36</v>
       </c>
     </row>
   </sheetData>
@@ -2195,7 +2209,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2529,6 +2543,38 @@
         <v>10575.91</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>02/06/2020 18:50:11</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>6767.240000000002</v>
+      </c>
+      <c r="C21" t="n">
+        <v>3845.63</v>
+      </c>
+      <c r="D21" t="n">
+        <v>10612.87</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>03/06/2020 18:22:41</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>7733.720000000001</v>
+      </c>
+      <c r="C22" t="n">
+        <v>2890.52</v>
+      </c>
+      <c r="D22" t="n">
+        <v>10624.24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
compile 4y features, all tickers
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -395,17 +395,17 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>INTC</t>
+          <t>KO</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>48.03</v>
+        <v>47.72</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.1118</v>
+        <v>-0.1674</v>
       </c>
       <c r="D2" t="n">
-        <v>27.80000000000001</v>
+        <v>39.89361702127661</v>
       </c>
     </row>
     <row r="3">
@@ -415,443 +415,445 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>86.8</v>
+        <v>89.73</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.766</v>
+        <v>3.3756</v>
       </c>
       <c r="D3" t="n">
-        <v>38.21656050955416</v>
+        <v>45.94427244582043</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>KO</t>
+          <t>MMM</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>47.8</v>
+        <v>161.44</v>
       </c>
       <c r="C4" t="n">
-        <v>0.674</v>
+        <v>1.9643</v>
       </c>
       <c r="D4" t="n">
-        <v>40.65040650406499</v>
+        <v>46.49805447470815</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>WMT</t>
+          <t>V</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>129.97</v>
+        <v>196.79</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4793</v>
+        <v>0.219</v>
       </c>
       <c r="D5" t="n">
-        <v>42.34016887816635</v>
+        <v>49.71962616822428</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>CAT</t>
+          <t>INTC</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>134.92</v>
+        <v>49.22</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3944</v>
+        <v>2.4776</v>
       </c>
       <c r="D6" t="n">
-        <v>43.42885375494063</v>
+        <v>49.80694980694978</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>WMT</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>170.02</v>
+        <v>131.88</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.266</v>
+        <v>1.4696</v>
       </c>
       <c r="D7" t="n">
-        <v>45.02129925452611</v>
+        <v>53.2940019665683</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>RTX</t>
+          <t>XOM</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>61.23</v>
+        <v>44.51</v>
       </c>
       <c r="C8" t="n">
-        <v>2.2716</v>
+        <v>2.4632</v>
       </c>
       <c r="D8" t="n">
-        <v>45.906432748538</v>
+        <v>53.32326283987913</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TRV</t>
+          <t>DOW</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>117.36</v>
+        <v>44.8</v>
       </c>
       <c r="C9" t="n">
-        <v>3.1827</v>
+        <v>5.0903</v>
       </c>
       <c r="D9" t="n">
-        <v>47.08121827411167</v>
+        <v>53.83877159309019</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>MMM</t>
+          <t>CAT</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>158.33</v>
+        <v>142.02</v>
       </c>
       <c r="C10" t="n">
-        <v>1.4936</v>
+        <v>5.2624</v>
       </c>
       <c r="D10" t="n">
-        <v>47.09503655252022</v>
+        <v>54.25489412704759</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>IBM</t>
+          <t>JNJ</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>124.96</v>
-      </c>
-      <c r="C11" t="inlineStr"/>
+        <v>148.03</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-0.3836</v>
+      </c>
       <c r="D11" t="n">
-        <v>49.49381327334081</v>
+        <v>55.75101488497965</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>XOM</t>
+          <t>CSCO</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>43.44</v>
+        <v>47.73</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.4583</v>
+        <v>0.6325</v>
       </c>
       <c r="D12" t="n">
-        <v>50.08077544426492</v>
+        <v>56.33802816901405</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>DOW</t>
+          <t>MSFT</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>42.63</v>
+        <v>208.25</v>
       </c>
       <c r="C13" t="n">
-        <v>1.3793</v>
+        <v>-1.9908</v>
       </c>
       <c r="D13" t="n">
-        <v>50.10373443983404</v>
+        <v>56.92259282567655</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>TRV</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>196.36</v>
+        <v>119.12</v>
       </c>
       <c r="C14" t="n">
-        <v>-1.2125</v>
+        <v>1.4997</v>
       </c>
       <c r="D14" t="n">
-        <v>52.66168059832822</v>
+        <v>57.84499054820419</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>JNJ</t>
+          <t>MCD</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>148.6</v>
+        <v>204.12</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7116</v>
+        <v>-0.2346</v>
       </c>
       <c r="D15" t="n">
-        <v>53.09278350515457</v>
+        <v>57.98553144129104</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>JPM</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>99.38</v>
+        <v>179.41</v>
       </c>
       <c r="C16" t="n">
-        <v>2.2007</v>
+        <v>5.5229</v>
       </c>
       <c r="D16" t="n">
-        <v>54.53795379537951</v>
+        <v>60.59907834101381</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>CSCO</t>
+          <t>IBM</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>47.43</v>
+        <v>127.11</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.7117</v>
+        <v>1.7206</v>
       </c>
       <c r="D17" t="n">
-        <v>60.84210526315788</v>
+        <v>60.99044309296265</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>WBA</t>
+          <t>RTX</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>41.52</v>
+        <v>64.23</v>
       </c>
       <c r="C18" t="n">
-        <v>1.5407</v>
+        <v>4.8996</v>
       </c>
       <c r="D18" t="n">
-        <v>62.84987277353703</v>
+        <v>62.78501628664494</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>AXP</t>
+          <t>MRK</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>99.16</v>
+        <v>80.91</v>
       </c>
       <c r="C19" t="n">
-        <v>3.3778</v>
+        <v>-0.1358</v>
       </c>
       <c r="D19" t="n">
-        <v>63.66880799428976</v>
+        <v>64.90963855421676</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>MCD</t>
+          <t>JPM</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>204.6</v>
+        <v>100.64</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6989</v>
+        <v>1.2679</v>
       </c>
       <c r="D20" t="n">
-        <v>64.68531468531464</v>
+        <v>65.58333333333329</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>NKE</t>
+          <t>GS</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>101.86</v>
+        <v>209.38</v>
       </c>
       <c r="C21" t="n">
-        <v>1.4037</v>
+        <v>0.533</v>
       </c>
       <c r="D21" t="n">
-        <v>65.54850407978236</v>
+        <v>66.78986272439276</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>GS</t>
+          <t>AXP</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>208.27</v>
+        <v>101.62</v>
       </c>
       <c r="C22" t="n">
-        <v>1.9682</v>
+        <v>2.4808</v>
       </c>
       <c r="D22" t="n">
-        <v>67.54385964912279</v>
+        <v>68.20737039350402</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>PFE</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>212.48</v>
+        <v>38.39</v>
       </c>
       <c r="C23" t="n">
-        <v>-1.7888</v>
+        <v>-0.156</v>
       </c>
       <c r="D23" t="n">
-        <v>68.57142857142857</v>
+        <v>71.99999999999996</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>PFE</t>
+          <t>HD</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>38.45</v>
+        <v>274.73</v>
       </c>
       <c r="C24" t="n">
-        <v>0.4703</v>
+        <v>1.1375</v>
       </c>
       <c r="D24" t="n">
-        <v>70.46263345195737</v>
+        <v>73.9672131147542</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>HD</t>
+          <t>VZ</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>271.64</v>
+        <v>58.99</v>
       </c>
       <c r="C25" t="n">
-        <v>0.8427</v>
+        <v>0.7859</v>
       </c>
       <c r="D25" t="n">
-        <v>72.17939733707084</v>
+        <v>78.64864864864879</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>MRK</t>
+          <t>NKE</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>81.02</v>
+        <v>105.41</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.037</v>
+        <v>3.4852</v>
       </c>
       <c r="D26" t="n">
-        <v>73.44497607655495</v>
+        <v>80.68862275449104</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>VZ</t>
+          <t>DIS</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>58.53</v>
+        <v>128.79</v>
       </c>
       <c r="C27" t="n">
-        <v>1.2104</v>
+        <v>-0.8774</v>
       </c>
       <c r="D27" t="n">
-        <v>75.76687116564429</v>
+        <v>82.63598326359829</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>UNH</t>
+          <t>WBA</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>317.03</v>
+        <v>42.86</v>
       </c>
       <c r="C28" t="n">
-        <v>0.9457</v>
+        <v>3.2274</v>
       </c>
       <c r="D28" t="n">
-        <v>78.57142857142847</v>
+        <v>82.82608695652183</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>DIS</t>
+          <t>AAPL</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>129.93</v>
+        <v>450.91</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.6803</v>
+        <v>1.4535</v>
       </c>
       <c r="D29" t="n">
-        <v>81.95020746887971</v>
+        <v>84.29885275433769</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>UNH</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>444.45</v>
+        <v>319.1</v>
       </c>
       <c r="C30" t="n">
-        <v>-2.4495</v>
+        <v>0.6529</v>
       </c>
       <c r="D30" t="n">
-        <v>84.01213569918173</v>
+        <v>86.21908127208472</v>
       </c>
     </row>
     <row r="31">
@@ -861,13 +863,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>133.55</v>
+        <v>134.1</v>
       </c>
       <c r="C31" t="n">
-        <v>0.633</v>
+        <v>0.4118</v>
       </c>
       <c r="D31" t="n">
-        <v>86.66666666666693</v>
+        <v>86.9070208728655</v>
       </c>
     </row>
   </sheetData>
@@ -941,19 +943,19 @@
         <v>45.98</v>
       </c>
       <c r="C2" t="n">
-        <v>43.44</v>
+        <v>44.51</v>
       </c>
       <c r="D2" t="n">
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>521.28</v>
+        <v>534.12</v>
       </c>
       <c r="F2" t="n">
-        <v>-5.5241</v>
+        <v>-3.197</v>
       </c>
       <c r="G2" t="n">
-        <v>50.08077544426492</v>
+        <v>53.32326283987913</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -971,19 +973,19 @@
         <v>61.92</v>
       </c>
       <c r="C3" t="n">
-        <v>61.23</v>
+        <v>64.23</v>
       </c>
       <c r="D3" t="n">
         <v>7</v>
       </c>
       <c r="E3" t="n">
-        <v>428.61</v>
+        <v>449.61</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.1143</v>
+        <v>3.7306</v>
       </c>
       <c r="G3" t="n">
-        <v>45.906432748538</v>
+        <v>62.78501628664494</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1001,19 +1003,19 @@
         <v>94.52</v>
       </c>
       <c r="C4" t="n">
-        <v>99.16</v>
+        <v>101.62</v>
       </c>
       <c r="D4" t="n">
         <v>5</v>
       </c>
       <c r="E4" t="n">
-        <v>495.8</v>
+        <v>508.1</v>
       </c>
       <c r="F4" t="n">
-        <v>4.909</v>
+        <v>7.5116</v>
       </c>
       <c r="G4" t="n">
-        <v>63.66880799428976</v>
+        <v>68.20737039350402</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1031,19 +1033,19 @@
         <v>50.59</v>
       </c>
       <c r="C5" t="n">
-        <v>48.03</v>
+        <v>49.22</v>
       </c>
       <c r="D5" t="n">
         <v>18</v>
       </c>
       <c r="E5" t="n">
-        <v>864.54</v>
+        <v>885.96</v>
       </c>
       <c r="F5" t="n">
-        <v>-5.0603</v>
+        <v>-2.708</v>
       </c>
       <c r="G5" t="n">
-        <v>27.80000000000001</v>
+        <v>49.80694980694978</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1061,19 +1063,19 @@
         <v>201.62</v>
       </c>
       <c r="C6" t="n">
-        <v>208.27</v>
+        <v>209.38</v>
       </c>
       <c r="D6" t="n">
         <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>833.08</v>
+        <v>837.52</v>
       </c>
       <c r="F6" t="n">
-        <v>3.2983</v>
+        <v>3.8488</v>
       </c>
       <c r="G6" t="n">
-        <v>67.54385964912279</v>
+        <v>66.78986272439276</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -1091,19 +1093,19 @@
         <v>166.01</v>
       </c>
       <c r="C7" t="n">
-        <v>170.02</v>
+        <v>179.41</v>
       </c>
       <c r="D7" t="n">
         <v>4</v>
       </c>
       <c r="E7" t="n">
-        <v>680.08</v>
+        <v>717.64</v>
       </c>
       <c r="F7" t="n">
-        <v>2.4155</v>
+        <v>8.0718</v>
       </c>
       <c r="G7" t="n">
-        <v>45.02129925452611</v>
+        <v>60.59907834101381</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -1121,19 +1123,19 @@
         <v>146.84</v>
       </c>
       <c r="C8" t="n">
-        <v>148.6</v>
+        <v>148.03</v>
       </c>
       <c r="D8" t="n">
         <v>4</v>
       </c>
       <c r="E8" t="n">
-        <v>594.4</v>
+        <v>592.12</v>
       </c>
       <c r="F8" t="n">
-        <v>1.1986</v>
+        <v>0.8104</v>
       </c>
       <c r="G8" t="n">
-        <v>53.09278350515457</v>
+        <v>55.75101488497965</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -1151,19 +1153,19 @@
         <v>129.4</v>
       </c>
       <c r="C9" t="n">
-        <v>129.97</v>
+        <v>131.88</v>
       </c>
       <c r="D9" t="n">
         <v>4</v>
       </c>
       <c r="E9" t="n">
-        <v>519.88</v>
+        <v>527.52</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4405</v>
+        <v>1.9165</v>
       </c>
       <c r="G9" t="n">
-        <v>42.34016887816635</v>
+        <v>53.2940019665683</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -1181,19 +1183,19 @@
         <v>113.1</v>
       </c>
       <c r="C10" t="n">
-        <v>117.36</v>
+        <v>119.12</v>
       </c>
       <c r="D10" t="n">
         <v>4</v>
       </c>
       <c r="E10" t="n">
-        <v>469.44</v>
+        <v>476.48</v>
       </c>
       <c r="F10" t="n">
-        <v>3.7666</v>
+        <v>5.3227</v>
       </c>
       <c r="G10" t="n">
-        <v>47.08121827411167</v>
+        <v>57.84499054820419</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -1249,7 +1251,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5407.11</v>
+        <v>5529.07</v>
       </c>
     </row>
     <row r="4">
@@ -1259,7 +1261,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10902.06</v>
+        <v>11024.02</v>
       </c>
     </row>
   </sheetData>
@@ -2931,7 +2933,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3905,6 +3907,22 @@
         <v>10902.06</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>10/08/2020 17:38:49</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>5494.95</v>
+      </c>
+      <c r="C61" t="n">
+        <v>5529.07</v>
+      </c>
+      <c r="D61" t="n">
+        <v>11024.02</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
init separate ml scripts
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -399,333 +399,333 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>37.79</v>
+        <v>38.33</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.5629</v>
+        <v>1.4289</v>
       </c>
       <c r="D2" t="n">
-        <v>27.51322751322756</v>
+        <v>37.44292237442915</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>WMT</t>
+          <t>V</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>130.2</v>
+        <v>198.74</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.2739</v>
+        <v>0.4905</v>
       </c>
       <c r="D3" t="n">
-        <v>43.09734513274332</v>
+        <v>50.37488284910965</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>INTC</t>
+          <t>CVX</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>48.19</v>
+        <v>90.72</v>
       </c>
       <c r="C4" t="n">
-        <v>-2.0926</v>
+        <v>1.2274</v>
       </c>
       <c r="D4" t="n">
-        <v>43.87755102040817</v>
+        <v>52.24602626123015</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>KO</t>
+          <t>DOW</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>47.93</v>
+        <v>44.28</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4401</v>
+        <v>-0.4944</v>
       </c>
       <c r="D5" t="n">
-        <v>46.59400544959129</v>
+        <v>54.3879907621247</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>JNJ</t>
+          <t>CAT</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>146.97</v>
+        <v>142.57</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.7161</v>
+        <v>0.0281</v>
       </c>
       <c r="D6" t="n">
-        <v>50.86419753086412</v>
+        <v>54.80678605089537</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>CVX</t>
+          <t>WMT</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>89.62</v>
+        <v>131.89</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.1226</v>
+        <v>1.298</v>
       </c>
       <c r="D7" t="n">
-        <v>51.77948360083742</v>
+        <v>55.03355704697984</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>KO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>203.38</v>
+        <v>48.43</v>
       </c>
       <c r="C8" t="n">
-        <v>-2.3385</v>
+        <v>1.0432</v>
       </c>
       <c r="D8" t="n">
-        <v>51.95290063182078</v>
+        <v>55.11221945137152</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>MSFT</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>197.77</v>
+        <v>209.19</v>
       </c>
       <c r="C9" t="n">
-        <v>0.498</v>
+        <v>2.8567</v>
       </c>
       <c r="D9" t="n">
-        <v>52.31877532642953</v>
+        <v>56.64679968903862</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>CAT</t>
+          <t>TRV</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>142.53</v>
+        <v>118.86</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3591</v>
+        <v>-0.8839</v>
       </c>
       <c r="D10" t="n">
-        <v>59.50168918918919</v>
+        <v>57.02306079664571</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>DOW</t>
+          <t>WBA</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>44.5</v>
+        <v>41.82</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.6696</v>
+        <v>-0.0717</v>
       </c>
       <c r="D11" t="n">
-        <v>60.06423982869381</v>
+        <v>57.63888888888896</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>MRK</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>80.91</v>
+        <v>175.44</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>-2.6037</v>
       </c>
       <c r="D12" t="n">
-        <v>60.3741496598639</v>
+        <v>60.87658592848906</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>JPM</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>180.13</v>
+        <v>102.94</v>
       </c>
       <c r="C13" t="n">
-        <v>0.4013</v>
+        <v>-0.8476</v>
       </c>
       <c r="D13" t="n">
-        <v>60.68061623361692</v>
+        <v>62.27409638554213</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>XOM</t>
+          <t>INTC</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>44.97</v>
+        <v>49.19</v>
       </c>
       <c r="C14" t="n">
-        <v>1.0335</v>
+        <v>2.0751</v>
       </c>
       <c r="D14" t="n">
-        <v>60.8231707317073</v>
+        <v>62.58741258741257</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>CSCO</t>
+          <t>JNJ</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>47.19</v>
+        <v>149.66</v>
       </c>
       <c r="C15" t="n">
-        <v>-1.1314</v>
+        <v>1.8303</v>
       </c>
       <c r="D15" t="n">
-        <v>61.69665809768629</v>
+        <v>64.85714285714289</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>WBA</t>
+          <t>VZ</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>41.85</v>
+        <v>58.6</v>
       </c>
       <c r="C16" t="n">
-        <v>-2.3565</v>
+        <v>0.1538</v>
       </c>
       <c r="D16" t="n">
-        <v>62.2641509433963</v>
+        <v>65.84022038567491</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>RTX</t>
+          <t>CSCO</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>64.26000000000001</v>
+        <v>48.1</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0467</v>
+        <v>1.9284</v>
       </c>
       <c r="D17" t="n">
-        <v>63.33878887070377</v>
+        <v>65.90389016018301</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>VZ</t>
+          <t>AXP</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>58.51</v>
+        <v>101.68</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.8137</v>
+        <v>-1.5301</v>
       </c>
       <c r="D18" t="n">
-        <v>64.42577030812329</v>
+        <v>66.00384862091084</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>TRV</t>
+          <t>IBM</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>119.92</v>
+        <v>126.7</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6716</v>
+        <v>-0.0394</v>
       </c>
       <c r="D19" t="n">
-        <v>66.22428666224286</v>
+        <v>66.02564102564105</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>IBM</t>
+          <t>MMM</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>126.75</v>
+        <v>164.26</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.2832</v>
+        <v>0.5386</v>
       </c>
       <c r="D20" t="n">
-        <v>69.1625615763547</v>
+        <v>70.34027425088875</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>MMM</t>
+          <t>MRK</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>163.38</v>
+        <v>82.68000000000001</v>
       </c>
       <c r="C21" t="n">
-        <v>1.2017</v>
+        <v>2.1876</v>
       </c>
       <c r="D21" t="n">
-        <v>70.40040547389759</v>
+        <v>72.77701778385772</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>JPM</t>
+          <t>RTX</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>103.82</v>
+        <v>64.29000000000001</v>
       </c>
       <c r="C22" t="n">
-        <v>3.1598</v>
+        <v>0.0467</v>
       </c>
       <c r="D22" t="n">
-        <v>72.01897018970186</v>
+        <v>72.95774647887325</v>
       </c>
     </row>
     <row r="23">
@@ -735,13 +735,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>211.06</v>
+        <v>212.13</v>
       </c>
       <c r="C23" t="n">
-        <v>0.8024</v>
+        <v>0.507</v>
       </c>
       <c r="D23" t="n">
-        <v>74.55775234131109</v>
+        <v>74.7025349198137</v>
       </c>
     </row>
     <row r="24">
@@ -751,29 +751,29 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>315.55</v>
+        <v>322.27</v>
       </c>
       <c r="C24" t="n">
-        <v>-1.1125</v>
+        <v>2.1296</v>
       </c>
       <c r="D24" t="n">
-        <v>75.58977719528171</v>
+        <v>75.5657592653328</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>AXP</t>
+          <t>AAPL</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>103.26</v>
+        <v>452.04</v>
       </c>
       <c r="C25" t="n">
-        <v>1.6139</v>
+        <v>3.3234</v>
       </c>
       <c r="D25" t="n">
-        <v>77.14987714987711</v>
+        <v>80.2182242212227</v>
       </c>
     </row>
     <row r="26">
@@ -783,45 +783,45 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>133.23</v>
+        <v>135.46</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.6488</v>
+        <v>1.6738</v>
       </c>
       <c r="D26" t="n">
-        <v>77.15736040609151</v>
+        <v>80.68669527897012</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>MCD</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>437.5</v>
+        <v>206.02</v>
       </c>
       <c r="C27" t="n">
-        <v>-2.974</v>
+        <v>0.4976</v>
       </c>
       <c r="D27" t="n">
-        <v>78.9188709391088</v>
+        <v>83.07484828051238</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>MCD</t>
+          <t>NKE</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>205</v>
+        <v>105.22</v>
       </c>
       <c r="C28" t="n">
-        <v>0.4311</v>
+        <v>0.0951</v>
       </c>
       <c r="D28" t="n">
-        <v>81.64739884393053</v>
+        <v>84.06275805119741</v>
       </c>
     </row>
     <row r="29">
@@ -831,29 +831,27 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>130.49</v>
+        <v>131.79</v>
       </c>
       <c r="C29" t="n">
-        <v>1.32</v>
+        <v>0.9962</v>
       </c>
       <c r="D29" t="n">
-        <v>84.58192363460606</v>
+        <v>87.76844070961717</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>NKE</t>
+          <t>XOM</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>105.12</v>
-      </c>
-      <c r="C30" t="n">
-        <v>-0.2751</v>
-      </c>
+        <v>44.09</v>
+      </c>
+      <c r="C30" t="inlineStr"/>
       <c r="D30" t="n">
-        <v>84.81510621557834</v>
+        <v>89.58333333333336</v>
       </c>
     </row>
     <row r="31">
@@ -863,13 +861,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>274.92</v>
+        <v>281.58</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0692</v>
+        <v>2.4225</v>
       </c>
       <c r="D31" t="n">
-        <v>86.24060150375985</v>
+        <v>93.74353671147888</v>
       </c>
     </row>
   </sheetData>
@@ -943,19 +941,19 @@
         <v>45.98</v>
       </c>
       <c r="C2" t="n">
-        <v>44.97</v>
+        <v>44.09</v>
       </c>
       <c r="D2" t="n">
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>539.64</v>
+        <v>529.08</v>
       </c>
       <c r="F2" t="n">
-        <v>-2.1966</v>
+        <v>-4.1105</v>
       </c>
       <c r="G2" t="n">
-        <v>60.8231707317073</v>
+        <v>89.58333333333336</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -973,19 +971,19 @@
         <v>61.92</v>
       </c>
       <c r="C3" t="n">
-        <v>64.26000000000001</v>
+        <v>64.29000000000001</v>
       </c>
       <c r="D3" t="n">
         <v>7</v>
       </c>
       <c r="E3" t="n">
-        <v>449.8200000000001</v>
+        <v>450.03</v>
       </c>
       <c r="F3" t="n">
-        <v>3.7791</v>
+        <v>3.8275</v>
       </c>
       <c r="G3" t="n">
-        <v>63.33878887070377</v>
+        <v>72.95774647887325</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1003,19 +1001,19 @@
         <v>50.59</v>
       </c>
       <c r="C4" t="n">
-        <v>48.19</v>
+        <v>49.19</v>
       </c>
       <c r="D4" t="n">
         <v>18</v>
       </c>
       <c r="E4" t="n">
-        <v>867.42</v>
+        <v>885.42</v>
       </c>
       <c r="F4" t="n">
-        <v>-4.744</v>
+        <v>-2.7673</v>
       </c>
       <c r="G4" t="n">
-        <v>43.87755102040817</v>
+        <v>62.58741258741257</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1033,19 +1031,19 @@
         <v>166.01</v>
       </c>
       <c r="C5" t="n">
-        <v>180.13</v>
+        <v>175.44</v>
       </c>
       <c r="D5" t="n">
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>720.52</v>
+        <v>701.76</v>
       </c>
       <c r="F5" t="n">
-        <v>8.5055</v>
+        <v>5.6804</v>
       </c>
       <c r="G5" t="n">
-        <v>60.68061623361692</v>
+        <v>60.87658592848906</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1063,19 +1061,19 @@
         <v>146.84</v>
       </c>
       <c r="C6" t="n">
-        <v>146.97</v>
+        <v>149.66</v>
       </c>
       <c r="D6" t="n">
         <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>587.88</v>
+        <v>598.64</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0885</v>
+        <v>1.9205</v>
       </c>
       <c r="G6" t="n">
-        <v>50.86419753086412</v>
+        <v>64.85714285714289</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -1093,19 +1091,19 @@
         <v>129.4</v>
       </c>
       <c r="C7" t="n">
-        <v>130.2</v>
+        <v>131.89</v>
       </c>
       <c r="D7" t="n">
         <v>4</v>
       </c>
       <c r="E7" t="n">
-        <v>520.8</v>
+        <v>527.5599999999999</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6182</v>
+        <v>1.9243</v>
       </c>
       <c r="G7" t="n">
-        <v>43.09734513274332</v>
+        <v>55.03355704697984</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -1123,19 +1121,19 @@
         <v>113.1</v>
       </c>
       <c r="C8" t="n">
-        <v>119.92</v>
+        <v>118.86</v>
       </c>
       <c r="D8" t="n">
         <v>4</v>
       </c>
       <c r="E8" t="n">
-        <v>479.68</v>
+        <v>475.44</v>
       </c>
       <c r="F8" t="n">
-        <v>6.0301</v>
+        <v>5.0928</v>
       </c>
       <c r="G8" t="n">
-        <v>66.22428666224286</v>
+        <v>57.02306079664571</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -1153,21 +1151,19 @@
         <v>37.79</v>
       </c>
       <c r="C9" t="n">
-        <v>37.79</v>
+        <v>38.33</v>
       </c>
       <c r="D9" t="n">
         <v>14</v>
       </c>
       <c r="E9" t="n">
-        <v>529.0599999999999</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
+        <v>536.62</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.4289</v>
       </c>
       <c r="G9" t="n">
-        <v>27.51322751322756</v>
+        <v>37.44292237442915</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -1223,7 +1219,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4694.82</v>
+        <v>4704.549999999999</v>
       </c>
     </row>
     <row r="4">
@@ -1233,7 +1229,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11021.25</v>
+        <v>11030.98</v>
       </c>
     </row>
   </sheetData>
@@ -2983,7 +2979,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3989,6 +3985,22 @@
         <v>11021.25</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>12/08/2020 17:40:23</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>6326.43</v>
+      </c>
+      <c r="C63" t="n">
+        <v>4704.549999999999</v>
+      </c>
+      <c r="D63" t="n">
+        <v>11030.98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
manual sell WMT, update portfolio, ml: created input features
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -399,45 +399,45 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>42.5</v>
+        <v>42.09</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.515</v>
+        <v>-0.9647</v>
       </c>
       <c r="D2" t="n">
-        <v>24.55752212389383</v>
+        <v>23.003194888179</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>PFE</t>
+          <t>MSFT</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>38.06</v>
+        <v>210.28</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.2882</v>
+        <v>0.6606</v>
       </c>
       <c r="D3" t="n">
-        <v>39.80582524271856</v>
+        <v>38.76525484565688</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>PFE</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>208.9</v>
+        <v>38.35</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0958</v>
+        <v>0.762</v>
       </c>
       <c r="D4" t="n">
-        <v>55.11707445409104</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
@@ -447,301 +447,301 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>41.91</v>
+        <v>41.17</v>
       </c>
       <c r="C5" t="n">
-        <v>2.2195</v>
+        <v>-1.7657</v>
       </c>
       <c r="D5" t="n">
-        <v>60.98901098901098</v>
+        <v>50.7718696397942</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>JNJ</t>
+          <t>TRV</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>148.24</v>
+        <v>115.91</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1622</v>
+        <v>-2.2681</v>
       </c>
       <c r="D6" t="n">
-        <v>61.25226860254094</v>
+        <v>54.83045425463848</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>INTC</t>
+          <t>JNJ</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>48.89</v>
+        <v>148.99</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6796</v>
+        <v>0.5059</v>
       </c>
       <c r="D7" t="n">
-        <v>61.67192429022087</v>
+        <v>58.0550098231828</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>WMT</t>
+          <t>GS</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>132.6</v>
+        <v>203.07</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5688</v>
+        <v>-2.3561</v>
       </c>
       <c r="D8" t="n">
-        <v>65.76500422654263</v>
+        <v>58.23634735899732</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TRV</t>
+          <t>INTC</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>118.6</v>
+        <v>48.93</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.5618</v>
+        <v>0.0818</v>
       </c>
       <c r="D9" t="n">
-        <v>66.12654320987649</v>
+        <v>58.2474226804124</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>VZ</t>
+          <t>IBM</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>58.79</v>
+        <v>124.44</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4614</v>
+        <v>-0.6626</v>
       </c>
       <c r="D10" t="n">
-        <v>67.94520547945213</v>
+        <v>60.45673076923076</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>KO</t>
+          <t>XOM</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>48.45</v>
+        <v>42.64</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1447</v>
+        <v>-1.2963</v>
       </c>
       <c r="D11" t="n">
-        <v>68.05970149253733</v>
+        <v>61.39359698681731</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>XOM</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>43.2</v>
+        <v>172.01</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4418</v>
+        <v>-3.4086</v>
       </c>
       <c r="D12" t="n">
-        <v>69.65376782077391</v>
+        <v>61.82038834951454</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>AXP</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>459.63</v>
+        <v>97.55</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.0891</v>
+        <v>-2.8483</v>
       </c>
       <c r="D13" t="n">
-        <v>71.12465638819167</v>
+        <v>62.43025418474887</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>PG</t>
+          <t>JPM</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>135.1</v>
+        <v>99.70999999999999</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.5008</v>
+        <v>-2.6365</v>
       </c>
       <c r="D14" t="n">
-        <v>71.53679653679653</v>
+        <v>63.87394312067643</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>AAPL</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>196.64</v>
+        <v>458.43</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.4758</v>
+        <v>-0.2611</v>
       </c>
       <c r="D15" t="n">
-        <v>71.83946488294306</v>
+        <v>65.81288757077375</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>CAT</t>
+          <t>MRK</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>139.96</v>
+        <v>84.76000000000001</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.5047</v>
+        <v>1.5333</v>
       </c>
       <c r="D16" t="n">
-        <v>71.87886279357238</v>
+        <v>69.82142857142848</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>IBM</t>
+          <t>CAT</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>125.27</v>
+        <v>138.72</v>
       </c>
       <c r="C17" t="n">
-        <v>0.192</v>
+        <v>-0.886</v>
       </c>
       <c r="D17" t="n">
-        <v>72.1719457013575</v>
+        <v>71.26225490196079</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>MRK</t>
+          <t>PG</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>83.48</v>
+        <v>135.5</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.0718</v>
+        <v>0.2961</v>
       </c>
       <c r="D18" t="n">
-        <v>74.47129909365553</v>
+        <v>72.22808870116161</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>VZ</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>178.08</v>
+        <v>58.78</v>
       </c>
       <c r="C19" t="n">
-        <v>1.9172</v>
+        <v>-0.017</v>
       </c>
       <c r="D19" t="n">
-        <v>75.48223350253809</v>
+        <v>72.51461988304095</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>AXP</t>
+          <t>WMT</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>100.41</v>
+        <v>135.6</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.01</v>
+        <v>2.2624</v>
       </c>
       <c r="D20" t="n">
-        <v>76.27872498146769</v>
+        <v>73.18397827562788</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>GS</t>
+          <t>V</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>207.97</v>
+        <v>199.43</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.2015</v>
+        <v>1.4188</v>
       </c>
       <c r="D21" t="n">
-        <v>76.52358240593531</v>
+        <v>75.87392550143264</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>JPM</t>
+          <t>UNH</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>102.41</v>
+        <v>320.51</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0391</v>
+        <v>-0.9855</v>
       </c>
       <c r="D22" t="n">
-        <v>76.58986175115211</v>
+        <v>76.50564617314927</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>DOW</t>
+          <t>NKE</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>44.87</v>
+        <v>105.66</v>
       </c>
       <c r="C23" t="n">
-        <v>0.9903</v>
+        <v>-0.7235</v>
       </c>
       <c r="D23" t="n">
-        <v>78.05596465390283</v>
+        <v>79.06423473433789</v>
       </c>
     </row>
     <row r="24">
@@ -751,13 +751,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>130.53</v>
+        <v>129.37</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.3283</v>
+        <v>-0.8887</v>
       </c>
       <c r="D24" t="n">
-        <v>81.82669789227168</v>
+        <v>79.69890510948909</v>
       </c>
     </row>
     <row r="25">
@@ -767,109 +767,109 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>90.34999999999999</v>
+        <v>90.77</v>
       </c>
       <c r="C25" t="n">
-        <v>0.5901</v>
+        <v>0.4649</v>
       </c>
       <c r="D25" t="n">
-        <v>82.80450358239504</v>
+        <v>81.97424892703857</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>NKE</t>
+          <t>RTX</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>106.43</v>
+        <v>62.77</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.08450000000000001</v>
+        <v>-1.3671</v>
       </c>
       <c r="D26" t="n">
-        <v>85.111464968153</v>
+        <v>82.42009132420087</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>UNH</t>
+          <t>DOW</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>323.7</v>
+        <v>44.46</v>
       </c>
       <c r="C27" t="n">
-        <v>0.678</v>
+        <v>-0.9137999999999999</v>
       </c>
       <c r="D27" t="n">
-        <v>85.43360433604335</v>
+        <v>85.07223113964695</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>HD</t>
+          <t>KO</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>280.55</v>
+        <v>48.21</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.3941</v>
+        <v>-0.4954</v>
       </c>
       <c r="D28" t="n">
-        <v>91.69435215946844</v>
+        <v>86.0377358490567</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>RTX</t>
+          <t>MMM</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>63.64</v>
+        <v>164.71</v>
       </c>
       <c r="C29" t="n">
-        <v>0.5371</v>
+        <v>-0.8368</v>
       </c>
       <c r="D29" t="n">
-        <v>92.3165137614678</v>
+        <v>91.86182669789234</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>MCD</t>
+          <t>HD</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>207.03</v>
+        <v>288.24</v>
       </c>
       <c r="C30" t="n">
-        <v>0.2615</v>
+        <v>2.741</v>
       </c>
       <c r="D30" t="n">
-        <v>95.83033788641256</v>
+        <v>94.01436552274541</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>MMM</t>
+          <t>MCD</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>166.1</v>
+        <v>208.67</v>
       </c>
       <c r="C31" t="n">
-        <v>0.1447</v>
+        <v>0.7922</v>
       </c>
       <c r="D31" t="n">
-        <v>99.61904761904761</v>
+        <v>96.2410887880751</v>
       </c>
     </row>
   </sheetData>
@@ -883,7 +883,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -943,19 +943,19 @@
         <v>45.98</v>
       </c>
       <c r="C2" t="n">
-        <v>43.2</v>
+        <v>42.64</v>
       </c>
       <c r="D2" t="n">
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>518.4000000000001</v>
+        <v>511.68</v>
       </c>
       <c r="F2" t="n">
-        <v>-6.0461</v>
+        <v>-7.264</v>
       </c>
       <c r="G2" t="n">
-        <v>69.65376782077391</v>
+        <v>61.39359698681731</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -973,19 +973,19 @@
         <v>50.59</v>
       </c>
       <c r="C3" t="n">
-        <v>48.89</v>
+        <v>48.93</v>
       </c>
       <c r="D3" t="n">
         <v>18</v>
       </c>
       <c r="E3" t="n">
-        <v>880.02</v>
+        <v>880.74</v>
       </c>
       <c r="F3" t="n">
-        <v>-3.3603</v>
+        <v>-3.2813</v>
       </c>
       <c r="G3" t="n">
-        <v>61.67192429022087</v>
+        <v>58.2474226804124</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1003,19 +1003,19 @@
         <v>146.84</v>
       </c>
       <c r="C4" t="n">
-        <v>148.24</v>
+        <v>148.99</v>
       </c>
       <c r="D4" t="n">
         <v>4</v>
       </c>
       <c r="E4" t="n">
-        <v>592.96</v>
+        <v>595.96</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9534</v>
+        <v>1.4642</v>
       </c>
       <c r="G4" t="n">
-        <v>61.25226860254094</v>
+        <v>58.0550098231828</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1026,26 +1026,26 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>WMT</t>
+          <t>TRV</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>129.4</v>
+        <v>113.1</v>
       </c>
       <c r="C5" t="n">
-        <v>132.6</v>
+        <v>115.91</v>
       </c>
       <c r="D5" t="n">
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>530.4</v>
+        <v>463.64</v>
       </c>
       <c r="F5" t="n">
-        <v>2.473</v>
+        <v>2.4845</v>
       </c>
       <c r="G5" t="n">
-        <v>65.76500422654263</v>
+        <v>54.83045425463848</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1056,26 +1056,26 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>TRV</t>
+          <t>PFE</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>113.1</v>
+        <v>37.79</v>
       </c>
       <c r="C6" t="n">
-        <v>118.6</v>
+        <v>38.35</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>474.4</v>
+        <v>536.9</v>
       </c>
       <c r="F6" t="n">
-        <v>4.863</v>
+        <v>1.4819</v>
       </c>
       <c r="G6" t="n">
-        <v>66.12654320987649</v>
+        <v>50</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -1086,60 +1086,28 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>PFE</t>
+          <t>CSCO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>37.79</v>
+        <v>42.5</v>
       </c>
       <c r="C7" t="n">
-        <v>38.06</v>
+        <v>42.09</v>
       </c>
       <c r="D7" t="n">
         <v>14</v>
       </c>
       <c r="E7" t="n">
-        <v>532.84</v>
+        <v>589.26</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7145</v>
+        <v>-0.9647</v>
       </c>
       <c r="G7" t="n">
-        <v>39.80582524271856</v>
+        <v>23.003194888179</v>
       </c>
       <c r="H7" t="inlineStr">
-        <is>
-          <t>buy</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>CSCO</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>42.5</v>
-      </c>
-      <c r="C8" t="n">
-        <v>42.5</v>
-      </c>
-      <c r="D8" t="n">
-        <v>14</v>
-      </c>
-      <c r="E8" t="n">
-        <v>595</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>24.55752212389383</v>
-      </c>
-      <c r="H8" t="inlineStr">
         <is>
           <t>buy</t>
         </is>
@@ -1183,7 +1151,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6889.23</v>
+        <v>7431.629999999999</v>
       </c>
     </row>
     <row r="3">
@@ -1193,7 +1161,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4124.02</v>
+        <v>3578.18</v>
       </c>
     </row>
     <row r="4">
@@ -1203,7 +1171,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11013.25</v>
+        <v>11009.81</v>
       </c>
     </row>
   </sheetData>
@@ -1217,7 +1185,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2992,6 +2960,32 @@
       </c>
       <c r="F68" t="n">
         <v>595</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>17/08/2020 17:56:45</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>WMT</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>4</v>
+      </c>
+      <c r="F69" t="n">
+        <v>542.4</v>
       </c>
     </row>
   </sheetData>
@@ -3005,7 +2999,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4043,6 +4037,22 @@
         <v>11013.25</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>17/08/2020 17:56:45</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>7431.629999999999</v>
+      </c>
+      <c r="C65" t="n">
+        <v>3578.18</v>
+      </c>
+      <c r="D65" t="n">
+        <v>11009.81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
08-18 and 08-19 predictions, rearrange scripts
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -399,93 +399,93 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>42.09</v>
+        <v>41.87</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.9647</v>
+        <v>-0.262</v>
       </c>
       <c r="D2" t="n">
-        <v>23.003194888179</v>
+        <v>18.8356164383562</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>XOM</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>210.28</v>
+        <v>41.96</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6606</v>
+        <v>-1.1077</v>
       </c>
       <c r="D3" t="n">
-        <v>38.76525484565688</v>
+        <v>38.23529411764709</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>PFE</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>38.35</v>
+        <v>169.27</v>
       </c>
       <c r="C4" t="n">
-        <v>0.762</v>
+        <v>-0.5639</v>
       </c>
       <c r="D4" t="n">
-        <v>50</v>
+        <v>42.15471343564047</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>WBA</t>
+          <t>TRV</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>41.17</v>
+        <v>113.2</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.7657</v>
+        <v>-1.5053</v>
       </c>
       <c r="D5" t="n">
-        <v>50.7718696397942</v>
+        <v>43.75830013280214</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>TRV</t>
+          <t>MSFT</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>115.91</v>
+        <v>209.7</v>
       </c>
       <c r="C6" t="n">
-        <v>-2.2681</v>
+        <v>-0.8464</v>
       </c>
       <c r="D6" t="n">
-        <v>54.83045425463848</v>
+        <v>44.05722670579603</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>JNJ</t>
+          <t>PFE</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>148.99</v>
+        <v>38.26</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5059</v>
+        <v>-0.2607</v>
       </c>
       <c r="D7" t="n">
-        <v>58.0550098231828</v>
+        <v>45.73991031390123</v>
       </c>
     </row>
     <row r="8">
@@ -495,13 +495,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>203.07</v>
+        <v>203.02</v>
       </c>
       <c r="C8" t="n">
-        <v>-2.3561</v>
+        <v>0.8494</v>
       </c>
       <c r="D8" t="n">
-        <v>58.23634735899732</v>
+        <v>46.37330754352031</v>
       </c>
     </row>
     <row r="9">
@@ -511,285 +511,285 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>48.93</v>
+        <v>48.33</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0818</v>
+        <v>-0.6578000000000001</v>
       </c>
       <c r="D9" t="n">
-        <v>58.2474226804124</v>
+        <v>47.58364312267653</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>IBM</t>
+          <t>WBA</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>124.44</v>
+        <v>40.25</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.6626</v>
+        <v>-1.2512</v>
       </c>
       <c r="D10" t="n">
-        <v>60.45673076923076</v>
+        <v>49.17218543046356</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>XOM</t>
+          <t>IBM</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>42.64</v>
+        <v>123.84</v>
       </c>
       <c r="C11" t="n">
-        <v>-1.2963</v>
+        <v>-0.8646</v>
       </c>
       <c r="D11" t="n">
-        <v>61.39359698681731</v>
+        <v>50.06257822277852</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>DIS</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>172.01</v>
+        <v>127.77</v>
       </c>
       <c r="C12" t="n">
-        <v>-3.4086</v>
+        <v>-0.892</v>
       </c>
       <c r="D12" t="n">
-        <v>61.82038834951454</v>
+        <v>50.65252854812396</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>AXP</t>
+          <t>CVX</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>97.55</v>
+        <v>86.39</v>
       </c>
       <c r="C13" t="n">
-        <v>-2.8483</v>
+        <v>-1.415</v>
       </c>
       <c r="D13" t="n">
-        <v>62.43025418474887</v>
+        <v>52.16952573158428</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>JPM</t>
+          <t>KO</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>99.70999999999999</v>
+        <v>47.37</v>
       </c>
       <c r="C14" t="n">
-        <v>-2.6365</v>
+        <v>-2.1685</v>
       </c>
       <c r="D14" t="n">
-        <v>63.87394312067643</v>
+        <v>52.50836120401335</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>AXP</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>458.43</v>
+        <v>96.89</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.2611</v>
+        <v>0.2276</v>
       </c>
       <c r="D15" t="n">
-        <v>65.81288757077375</v>
+        <v>55.10899182561308</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>MRK</t>
+          <t>UNH</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>84.76000000000001</v>
+        <v>315.4</v>
       </c>
       <c r="C16" t="n">
-        <v>1.5333</v>
+        <v>-0.4451</v>
       </c>
       <c r="D16" t="n">
-        <v>69.82142857142848</v>
+        <v>55.20796302879479</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>CAT</t>
+          <t>JPM</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>138.72</v>
+        <v>98.55</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.886</v>
+        <v>0.2339</v>
       </c>
       <c r="D17" t="n">
-        <v>71.26225490196079</v>
+        <v>55.39452495974237</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>PG</t>
+          <t>JNJ</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>135.5</v>
+        <v>150.39</v>
       </c>
       <c r="C18" t="n">
-        <v>0.2961</v>
+        <v>0.1999</v>
       </c>
       <c r="D18" t="n">
-        <v>72.22808870116161</v>
+        <v>59.68841285296976</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>VZ</t>
+          <t>WMT</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>58.78</v>
+        <v>132.41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.017</v>
+        <v>-1.7074</v>
       </c>
       <c r="D19" t="n">
-        <v>72.51461988304095</v>
+        <v>61.36528685548289</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>WMT</t>
+          <t>CAT</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>135.6</v>
+        <v>138.02</v>
       </c>
       <c r="C20" t="n">
-        <v>2.2624</v>
+        <v>-0.2529</v>
       </c>
       <c r="D20" t="n">
-        <v>73.18397827562788</v>
+        <v>61.4575507137491</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>RTX</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>199.43</v>
+        <v>61.64</v>
       </c>
       <c r="C21" t="n">
-        <v>1.4188</v>
+        <v>-0.7407</v>
       </c>
       <c r="D21" t="n">
-        <v>75.87392550143264</v>
+        <v>63.87009472259805</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>UNH</t>
+          <t>PG</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>320.51</v>
+        <v>135.77</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.9855</v>
+        <v>-0.5421</v>
       </c>
       <c r="D22" t="n">
-        <v>76.50564617314927</v>
+        <v>63.91875746714468</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>NKE</t>
+          <t>AAPL</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>105.66</v>
+        <v>462.83</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.7235</v>
+        <v>0.1255</v>
       </c>
       <c r="D23" t="n">
-        <v>79.06423473433789</v>
+        <v>65.77135915778103</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>DIS</t>
+          <t>V</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>129.37</v>
+        <v>200.99</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.8887</v>
+        <v>0.9949</v>
       </c>
       <c r="D24" t="n">
-        <v>79.69890510948909</v>
+        <v>67.95847750865045</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>CVX</t>
+          <t>VZ</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>90.77</v>
+        <v>59.05</v>
       </c>
       <c r="C25" t="n">
-        <v>0.4649</v>
+        <v>-0.2197</v>
       </c>
       <c r="D25" t="n">
-        <v>81.97424892703857</v>
+        <v>75.94501718213053</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>RTX</t>
+          <t>HD</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>62.77</v>
+        <v>282.86</v>
       </c>
       <c r="C26" t="n">
-        <v>-1.3671</v>
+        <v>-0.7509</v>
       </c>
       <c r="D26" t="n">
-        <v>82.42009132420087</v>
+        <v>77.11565585331451</v>
       </c>
     </row>
     <row r="27">
@@ -799,29 +799,29 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>44.46</v>
+        <v>44.64</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.9137999999999999</v>
+        <v>-0.1566</v>
       </c>
       <c r="D27" t="n">
-        <v>85.07223113964695</v>
+        <v>78.49462365591407</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>KO</t>
+          <t>MRK</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>48.21</v>
+        <v>85.03</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.4954</v>
+        <v>0.5558</v>
       </c>
       <c r="D28" t="n">
-        <v>86.0377358490567</v>
+        <v>81.56424581005577</v>
       </c>
     </row>
     <row r="29">
@@ -831,29 +831,29 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>164.71</v>
+        <v>163.97</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.8368</v>
+        <v>-0.2494</v>
       </c>
       <c r="D29" t="n">
-        <v>91.86182669789234</v>
+        <v>83.46273291925469</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>HD</t>
+          <t>NKE</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>288.24</v>
+        <v>108.39</v>
       </c>
       <c r="C30" t="n">
-        <v>2.741</v>
+        <v>1.3275</v>
       </c>
       <c r="D30" t="n">
-        <v>94.01436552274541</v>
+        <v>84.71575023299171</v>
       </c>
     </row>
     <row r="31">
@@ -863,13 +863,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>208.67</v>
+        <v>209.51</v>
       </c>
       <c r="C31" t="n">
-        <v>0.7922</v>
+        <v>-0.3851</v>
       </c>
       <c r="D31" t="n">
-        <v>96.2410887880751</v>
+        <v>89.94544037412319</v>
       </c>
     </row>
   </sheetData>
@@ -943,19 +943,19 @@
         <v>45.98</v>
       </c>
       <c r="C2" t="n">
-        <v>42.64</v>
+        <v>41.96</v>
       </c>
       <c r="D2" t="n">
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>511.68</v>
+        <v>503.52</v>
       </c>
       <c r="F2" t="n">
-        <v>-7.264</v>
+        <v>-8.742900000000001</v>
       </c>
       <c r="G2" t="n">
-        <v>61.39359698681731</v>
+        <v>38.23529411764709</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -973,19 +973,19 @@
         <v>50.59</v>
       </c>
       <c r="C3" t="n">
-        <v>48.93</v>
+        <v>48.33</v>
       </c>
       <c r="D3" t="n">
         <v>18</v>
       </c>
       <c r="E3" t="n">
-        <v>880.74</v>
+        <v>869.9399999999999</v>
       </c>
       <c r="F3" t="n">
-        <v>-3.2813</v>
+        <v>-4.4673</v>
       </c>
       <c r="G3" t="n">
-        <v>58.2474226804124</v>
+        <v>47.58364312267653</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1003,19 +1003,19 @@
         <v>146.84</v>
       </c>
       <c r="C4" t="n">
-        <v>148.99</v>
+        <v>150.39</v>
       </c>
       <c r="D4" t="n">
         <v>4</v>
       </c>
       <c r="E4" t="n">
-        <v>595.96</v>
+        <v>601.5599999999999</v>
       </c>
       <c r="F4" t="n">
-        <v>1.4642</v>
+        <v>2.4176</v>
       </c>
       <c r="G4" t="n">
-        <v>58.0550098231828</v>
+        <v>59.68841285296976</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1033,19 +1033,19 @@
         <v>113.1</v>
       </c>
       <c r="C5" t="n">
-        <v>115.91</v>
+        <v>113.2</v>
       </c>
       <c r="D5" t="n">
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>463.64</v>
+        <v>452.8</v>
       </c>
       <c r="F5" t="n">
-        <v>2.4845</v>
+        <v>0.08840000000000001</v>
       </c>
       <c r="G5" t="n">
-        <v>54.83045425463848</v>
+        <v>43.75830013280214</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1063,19 +1063,19 @@
         <v>37.79</v>
       </c>
       <c r="C6" t="n">
-        <v>38.35</v>
+        <v>38.26</v>
       </c>
       <c r="D6" t="n">
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>536.9</v>
+        <v>535.64</v>
       </c>
       <c r="F6" t="n">
-        <v>1.4819</v>
+        <v>1.2437</v>
       </c>
       <c r="G6" t="n">
-        <v>50</v>
+        <v>45.73991031390123</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -1093,19 +1093,19 @@
         <v>42.5</v>
       </c>
       <c r="C7" t="n">
-        <v>42.09</v>
+        <v>41.87</v>
       </c>
       <c r="D7" t="n">
         <v>14</v>
       </c>
       <c r="E7" t="n">
-        <v>589.26</v>
+        <v>586.1799999999999</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.9647</v>
+        <v>-1.4824</v>
       </c>
       <c r="G7" t="n">
-        <v>23.003194888179</v>
+        <v>18.8356164383562</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -1161,7 +1161,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3578.18</v>
+        <v>3549.64</v>
       </c>
     </row>
     <row r="4">
@@ -1171,7 +1171,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11009.81</v>
+        <v>10981.27</v>
       </c>
     </row>
   </sheetData>
@@ -2999,7 +2999,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4053,6 +4053,38 @@
         <v>11009.81</v>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>18/08/2020 17:22:15</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>7431.629999999999</v>
+      </c>
+      <c r="C66" t="n">
+        <v>3569.699999999999</v>
+      </c>
+      <c r="D66" t="n">
+        <v>11001.33</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>19/08/2020 17:04:31</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>7431.629999999999</v>
+      </c>
+      <c r="C67" t="n">
+        <v>3549.64</v>
+      </c>
+      <c r="D67" t="n">
+        <v>10981.27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added add_all_features func, input feature creation
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -399,10 +399,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>41.87</v>
+        <v>42.31</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.262</v>
+        <v>1.0509</v>
       </c>
       <c r="D2" t="n">
         <v>18.8356164383562</v>
@@ -415,189 +415,189 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>41.96</v>
+        <v>41.32</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.1077</v>
+        <v>-1.5253</v>
       </c>
       <c r="D3" t="n">
-        <v>38.23529411764709</v>
+        <v>34.77366255144038</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>DIS</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>169.27</v>
+        <v>128.12</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.5639</v>
+        <v>0.2739</v>
       </c>
       <c r="D4" t="n">
-        <v>42.15471343564047</v>
+        <v>35.63829787234049</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>TRV</t>
+          <t>IBM</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>113.2</v>
+        <v>123.15</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.5053</v>
+        <v>-0.5572</v>
       </c>
       <c r="D5" t="n">
-        <v>43.75830013280214</v>
+        <v>41.64588528678311</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>CVX</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>209.7</v>
+        <v>84.81</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.8464</v>
+        <v>-1.8289</v>
       </c>
       <c r="D6" t="n">
-        <v>44.05722670579603</v>
+        <v>43.67201426024958</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>PFE</t>
+          <t>GS</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>38.26</v>
+        <v>201.85</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.2607</v>
+        <v>-0.5763</v>
       </c>
       <c r="D7" t="n">
-        <v>45.73991031390123</v>
+        <v>44.43929564411491</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>GS</t>
+          <t>WBA</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>203.02</v>
+        <v>39.71</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8494</v>
+        <v>-1.3416</v>
       </c>
       <c r="D8" t="n">
-        <v>46.37330754352031</v>
+        <v>44.46153846153847</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>INTC</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>48.33</v>
+        <v>169.58</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.6578000000000001</v>
+        <v>0.1831</v>
       </c>
       <c r="D9" t="n">
-        <v>47.58364312267653</v>
+        <v>45.65649867374009</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>WBA</t>
+          <t>TRV</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>40.25</v>
+        <v>112.53</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.2512</v>
+        <v>-0.5919</v>
       </c>
       <c r="D10" t="n">
-        <v>49.17218543046356</v>
+        <v>45.79569145239752</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>IBM</t>
+          <t>KO</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>123.84</v>
+        <v>47.35</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.8646</v>
+        <v>-0.0422</v>
       </c>
       <c r="D11" t="n">
-        <v>50.06257822277852</v>
+        <v>47.63636363636373</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>DIS</t>
+          <t>MSFT</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>127.77</v>
+        <v>214.58</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.892</v>
+        <v>2.3271</v>
       </c>
       <c r="D12" t="n">
-        <v>50.65252854812396</v>
+        <v>47.78132765353214</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>CVX</t>
+          <t>UNH</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>86.39</v>
+        <v>313.33</v>
       </c>
       <c r="C13" t="n">
-        <v>-1.415</v>
+        <v>-0.6563</v>
       </c>
       <c r="D13" t="n">
-        <v>52.16952573158428</v>
+        <v>48.72422229989511</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>KO</t>
+          <t>JPM</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>47.37</v>
+        <v>97.37</v>
       </c>
       <c r="C14" t="n">
-        <v>-2.1685</v>
+        <v>-1.1974</v>
       </c>
       <c r="D14" t="n">
-        <v>52.50836120401335</v>
+        <v>50.47899778924101</v>
       </c>
     </row>
     <row r="15">
@@ -607,77 +607,77 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>96.89</v>
+        <v>96.72</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2276</v>
+        <v>-0.1755</v>
       </c>
       <c r="D15" t="n">
-        <v>55.10899182561308</v>
+        <v>52.79329608938547</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>UNH</t>
+          <t>INTC</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>315.4</v>
+        <v>49.17</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.4451</v>
+        <v>1.7381</v>
       </c>
       <c r="D16" t="n">
-        <v>55.20796302879479</v>
+        <v>54.83870967741937</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>JPM</t>
+          <t>WMT</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>98.55</v>
+        <v>130.57</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2339</v>
+        <v>-1.3896</v>
       </c>
       <c r="D17" t="n">
-        <v>55.39452495974237</v>
+        <v>55.77557755775576</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>JNJ</t>
+          <t>PFE</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>150.39</v>
+        <v>38.72</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1999</v>
+        <v>1.2023</v>
       </c>
       <c r="D18" t="n">
-        <v>59.68841285296976</v>
+        <v>58.96414342629474</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>WMT</t>
+          <t>RTX</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>132.41</v>
+        <v>60.99</v>
       </c>
       <c r="C19" t="n">
-        <v>-1.7074</v>
+        <v>-1.0545</v>
       </c>
       <c r="D19" t="n">
-        <v>61.36528685548289</v>
+        <v>59.8984771573604</v>
       </c>
     </row>
     <row r="20">
@@ -687,61 +687,61 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>138.02</v>
+        <v>137.48</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.2529</v>
+        <v>-0.3912</v>
       </c>
       <c r="D20" t="n">
-        <v>61.4575507137491</v>
+        <v>61.64280331574982</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>RTX</t>
+          <t>AAPL</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>61.64</v>
+        <v>473.1</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.7407</v>
+        <v>2.219</v>
       </c>
       <c r="D21" t="n">
-        <v>63.87009472259805</v>
+        <v>63.26234970302764</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>PG</t>
+          <t>DOW</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>135.77</v>
+        <v>43.69</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.5421</v>
+        <v>-2.1281</v>
       </c>
       <c r="D22" t="n">
-        <v>63.91875746714468</v>
+        <v>64.80144404332133</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>JNJ</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>462.83</v>
+        <v>151.42</v>
       </c>
       <c r="C23" t="n">
-        <v>0.1255</v>
+        <v>0.6849</v>
       </c>
       <c r="D23" t="n">
-        <v>65.77135915778103</v>
+        <v>68.51674641148321</v>
       </c>
     </row>
     <row r="24">
@@ -751,125 +751,125 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>200.99</v>
+        <v>204.15</v>
       </c>
       <c r="C24" t="n">
-        <v>0.9949</v>
+        <v>1.5722</v>
       </c>
       <c r="D24" t="n">
-        <v>67.95847750865045</v>
+        <v>69.00937081659968</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>VZ</t>
+          <t>HD</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>59.05</v>
+        <v>280.68</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.2197</v>
+        <v>-0.7707000000000001</v>
       </c>
       <c r="D25" t="n">
-        <v>75.94501718213053</v>
+        <v>69.73821989528794</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>HD</t>
+          <t>VZ</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>282.86</v>
+        <v>58.96</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.7509</v>
+        <v>-0.1524</v>
       </c>
       <c r="D26" t="n">
-        <v>77.11565585331451</v>
+        <v>70.84870848708491</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>DOW</t>
+          <t>PG</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>44.64</v>
+        <v>136.85</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.1566</v>
+        <v>0.7955</v>
       </c>
       <c r="D27" t="n">
-        <v>78.49462365591407</v>
+        <v>73.73853211009174</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>MRK</t>
+          <t>MMM</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>85.03</v>
+        <v>162.97</v>
       </c>
       <c r="C28" t="n">
-        <v>0.5558</v>
+        <v>-0.6099</v>
       </c>
       <c r="D28" t="n">
-        <v>81.56424581005577</v>
+        <v>76.34164777021921</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>MMM</t>
+          <t>NKE</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>163.97</v>
+        <v>108.01</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.2494</v>
+        <v>-0.3506</v>
       </c>
       <c r="D29" t="n">
-        <v>83.46273291925469</v>
+        <v>85.59322033898314</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>NKE</t>
+          <t>MCD</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>108.39</v>
+        <v>209.88</v>
       </c>
       <c r="C30" t="n">
-        <v>1.3275</v>
+        <v>0.1766</v>
       </c>
       <c r="D30" t="n">
-        <v>84.71575023299171</v>
+        <v>86.09913793103453</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>MCD</t>
+          <t>MRK</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>209.51</v>
+        <v>85.03</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.3851</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>89.94544037412319</v>
+        <v>91.63179916317982</v>
       </c>
     </row>
   </sheetData>
@@ -943,19 +943,19 @@
         <v>45.98</v>
       </c>
       <c r="C2" t="n">
-        <v>41.96</v>
+        <v>41.32</v>
       </c>
       <c r="D2" t="n">
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>503.52</v>
+        <v>495.84</v>
       </c>
       <c r="F2" t="n">
-        <v>-8.742900000000001</v>
+        <v>-10.1348</v>
       </c>
       <c r="G2" t="n">
-        <v>38.23529411764709</v>
+        <v>34.77366255144038</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -973,19 +973,19 @@
         <v>50.59</v>
       </c>
       <c r="C3" t="n">
-        <v>48.33</v>
+        <v>49.17</v>
       </c>
       <c r="D3" t="n">
         <v>18</v>
       </c>
       <c r="E3" t="n">
-        <v>869.9399999999999</v>
+        <v>885.0600000000001</v>
       </c>
       <c r="F3" t="n">
-        <v>-4.4673</v>
+        <v>-2.8069</v>
       </c>
       <c r="G3" t="n">
-        <v>47.58364312267653</v>
+        <v>54.83870967741937</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1003,19 +1003,19 @@
         <v>146.84</v>
       </c>
       <c r="C4" t="n">
-        <v>150.39</v>
+        <v>151.42</v>
       </c>
       <c r="D4" t="n">
         <v>4</v>
       </c>
       <c r="E4" t="n">
-        <v>601.5599999999999</v>
+        <v>605.6799999999999</v>
       </c>
       <c r="F4" t="n">
-        <v>2.4176</v>
+        <v>3.119</v>
       </c>
       <c r="G4" t="n">
-        <v>59.68841285296976</v>
+        <v>68.51674641148321</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1033,19 +1033,19 @@
         <v>113.1</v>
       </c>
       <c r="C5" t="n">
-        <v>113.2</v>
+        <v>112.53</v>
       </c>
       <c r="D5" t="n">
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>452.8</v>
+        <v>450.12</v>
       </c>
       <c r="F5" t="n">
-        <v>0.08840000000000001</v>
+        <v>-0.504</v>
       </c>
       <c r="G5" t="n">
-        <v>43.75830013280214</v>
+        <v>45.79569145239752</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1063,19 +1063,19 @@
         <v>37.79</v>
       </c>
       <c r="C6" t="n">
-        <v>38.26</v>
+        <v>38.72</v>
       </c>
       <c r="D6" t="n">
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>535.64</v>
+        <v>542.0799999999999</v>
       </c>
       <c r="F6" t="n">
-        <v>1.2437</v>
+        <v>2.461</v>
       </c>
       <c r="G6" t="n">
-        <v>45.73991031390123</v>
+        <v>58.96414342629474</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -1093,16 +1093,16 @@
         <v>42.5</v>
       </c>
       <c r="C7" t="n">
-        <v>41.87</v>
+        <v>42.31</v>
       </c>
       <c r="D7" t="n">
         <v>14</v>
       </c>
       <c r="E7" t="n">
-        <v>586.1799999999999</v>
+        <v>592.34</v>
       </c>
       <c r="F7" t="n">
-        <v>-1.4824</v>
+        <v>-0.4471</v>
       </c>
       <c r="G7" t="n">
         <v>18.8356164383562</v>
@@ -1161,7 +1161,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3549.64</v>
+        <v>3571.12</v>
       </c>
     </row>
     <row r="4">
@@ -1171,7 +1171,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10981.27</v>
+        <v>11002.75</v>
       </c>
     </row>
   </sheetData>
@@ -2999,7 +2999,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4085,6 +4085,22 @@
         <v>10981.27</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>20/08/2020 17:45:39</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>7431.629999999999</v>
+      </c>
+      <c r="C68" t="n">
+        <v>3571.12</v>
+      </c>
+      <c r="D68" t="n">
+        <v>11002.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update_history_subset() logic; update history based on relevant trading window
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9cefadc21042b88c/PET_PROJECTS/Al-the-Trader/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_B1C150B80D03F194F17B52340BF2FAA582AF4364" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1A6B543B-9403-3647-B979-8B9A1351C073}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_B1C150B80D03F194F17B52340BF2FAA582AF4364" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2A19E093-4B26-CF4A-83E1-4DEE33C99FEC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="17920" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="17920" windowHeight="21900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="watchlist" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="204">
   <si>
     <t>ticker</t>
   </si>
@@ -140,9 +140,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>performance</t>
-  </si>
-  <si>
     <t>current_rsi</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
   </si>
   <si>
     <t>buy</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>asset</t>
@@ -1006,7 +1000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1453,13 +1447,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1481,11 +1477,8 @@
       <c r="G1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1502,16 +1495,13 @@
         <v>453.6</v>
       </c>
       <c r="F2">
-        <v>-17.790299999999998</v>
-      </c>
-      <c r="G2">
         <v>34.451901565995513</v>
       </c>
-      <c r="H2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1528,16 +1518,13 @@
         <v>450.4</v>
       </c>
       <c r="F3">
-        <v>-0.44209999999999999</v>
-      </c>
-      <c r="G3">
         <v>36.893840104849268</v>
       </c>
-      <c r="H3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1554,16 +1541,13 @@
         <v>515.48</v>
       </c>
       <c r="F4">
-        <v>-2.5668000000000002</v>
-      </c>
-      <c r="G4">
         <v>44.836956521739097</v>
       </c>
-      <c r="H4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1580,16 +1564,13 @@
         <v>565.17999999999995</v>
       </c>
       <c r="F5">
-        <v>-5.0118</v>
-      </c>
-      <c r="G5">
         <v>26.544622425629299</v>
       </c>
-      <c r="H5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1606,16 +1587,13 @@
         <v>669.78</v>
       </c>
       <c r="F6">
-        <v>-6.3663999999999996</v>
-      </c>
-      <c r="G6">
         <v>50.396825396825378</v>
       </c>
-      <c r="H6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -1632,16 +1610,13 @@
         <v>753.72</v>
       </c>
       <c r="F7">
-        <v>3.0516999999999999</v>
-      </c>
-      <c r="G7">
         <v>54.861944777911177</v>
       </c>
-      <c r="H7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1658,16 +1633,13 @@
         <v>551.53000000000009</v>
       </c>
       <c r="F8">
-        <v>-7.0652999999999997</v>
-      </c>
-      <c r="G8">
         <v>30.701754385964989</v>
       </c>
-      <c r="H8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1684,16 +1656,13 @@
         <v>609.96</v>
       </c>
       <c r="F9">
-        <v>-1.2434000000000001</v>
-      </c>
-      <c r="G9">
         <v>31.46425724156256</v>
       </c>
-      <c r="H9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1709,17 +1678,14 @@
       <c r="E10">
         <v>588.67999999999995</v>
       </c>
-      <c r="F10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10">
+      <c r="F10">
         <v>28.516129032257979</v>
       </c>
-      <c r="H10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1735,17 +1701,14 @@
       <c r="E11">
         <v>608.73</v>
       </c>
-      <c r="F11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11">
+      <c r="F11">
         <v>24.108108108108102</v>
       </c>
-      <c r="H11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1761,17 +1724,14 @@
       <c r="E12">
         <v>551.70000000000005</v>
       </c>
-      <c r="F12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12">
+      <c r="F12">
         <v>21.76943699731903</v>
       </c>
-      <c r="H12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1787,17 +1747,14 @@
       <c r="E13">
         <v>520.88</v>
       </c>
-      <c r="F13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13">
+      <c r="F13">
         <v>27.10363153232942</v>
       </c>
-      <c r="H13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1813,17 +1770,14 @@
       <c r="E14">
         <v>584.49</v>
       </c>
-      <c r="F14" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14">
+      <c r="F14">
         <v>24.641547182394159</v>
       </c>
-      <c r="H14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1839,14 +1793,11 @@
       <c r="E15">
         <v>546.76</v>
       </c>
-      <c r="F15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15">
+      <c r="F15">
         <v>15.76323987538953</v>
       </c>
-      <c r="H15" t="s">
-        <v>41</v>
+      <c r="G15" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1864,7 +1815,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>37</v>
@@ -1872,7 +1823,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <v>2898.27</v>
@@ -1880,7 +1831,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>7970.8899999999994</v>
@@ -1888,7 +1839,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>10869.16</v>
@@ -1909,13 +1860,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>36</v>
@@ -1929,13 +1880,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -1949,13 +1900,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <v>24</v>
@@ -1969,13 +1920,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4">
         <v>7</v>
@@ -1989,13 +1940,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -2009,13 +1960,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6">
         <v>11</v>
@@ -2029,13 +1980,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -2049,13 +2000,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -2069,13 +2020,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9">
         <v>6</v>
@@ -2089,13 +2040,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -2109,13 +2060,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -2129,13 +2080,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -2149,13 +2100,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -2169,13 +2120,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14">
         <v>9</v>
@@ -2189,13 +2140,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -2209,13 +2160,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16">
         <v>6</v>
@@ -2229,13 +2180,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
         <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -2249,13 +2200,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -2269,13 +2220,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -2289,13 +2240,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -2309,13 +2260,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -2329,13 +2280,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22">
         <v>2</v>
@@ -2349,13 +2300,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -2369,13 +2320,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
         <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -2389,13 +2340,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
         <v>20</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E25">
         <v>4</v>
@@ -2409,13 +2360,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C26" t="s">
         <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -2429,13 +2380,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
         <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -2449,13 +2400,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C28" t="s">
         <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E28">
         <v>3</v>
@@ -2469,13 +2420,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C29" t="s">
         <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E29">
         <v>7</v>
@@ -2489,13 +2440,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C30" t="s">
         <v>19</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -2509,13 +2460,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E31">
         <v>10</v>
@@ -2529,13 +2480,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s">
         <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E32">
         <v>24</v>
@@ -2549,13 +2500,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C33" t="s">
         <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E33">
         <v>10</v>
@@ -2569,13 +2520,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C34" t="s">
         <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E34">
         <v>5</v>
@@ -2589,13 +2540,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E35">
         <v>2</v>
@@ -2609,13 +2560,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
       </c>
       <c r="D36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E36">
         <v>3</v>
@@ -2629,13 +2580,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C37" t="s">
         <v>24</v>
       </c>
       <c r="D37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E37">
         <v>6</v>
@@ -2649,13 +2600,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s">
         <v>22</v>
       </c>
       <c r="D38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E38">
         <v>23</v>
@@ -2669,13 +2620,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E39">
         <v>5</v>
@@ -2689,13 +2640,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C40" t="s">
         <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E40">
         <v>4</v>
@@ -2709,13 +2660,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
       </c>
       <c r="D41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E41">
         <v>6</v>
@@ -2729,13 +2680,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
         <v>27</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E42">
         <v>11</v>
@@ -2749,13 +2700,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E43">
         <v>14</v>
@@ -2769,13 +2720,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C44" t="s">
         <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E44">
         <v>3</v>
@@ -2789,13 +2740,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E45">
         <v>18</v>
@@ -2809,13 +2760,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C46" t="s">
         <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E46">
         <v>12</v>
@@ -2829,13 +2780,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C47" t="s">
         <v>20</v>
       </c>
       <c r="D47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E47">
         <v>6</v>
@@ -2849,13 +2800,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C48" t="s">
         <v>29</v>
       </c>
       <c r="D48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E48">
         <v>7</v>
@@ -2869,13 +2820,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
         <v>28</v>
       </c>
       <c r="D49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E49">
         <v>5</v>
@@ -2889,13 +2840,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C50" t="s">
         <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E50">
         <v>18</v>
@@ -2909,13 +2860,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C51" t="s">
         <v>4</v>
       </c>
       <c r="D51" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E51">
         <v>8</v>
@@ -2929,13 +2880,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C52" t="s">
         <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E52">
         <v>3</v>
@@ -2949,13 +2900,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C53" t="s">
         <v>22</v>
       </c>
       <c r="D53" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E53">
         <v>23</v>
@@ -2969,13 +2920,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C54" t="s">
         <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E54">
         <v>3</v>
@@ -2989,13 +2940,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
       </c>
       <c r="D55" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E55">
         <v>14</v>
@@ -3009,13 +2960,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C56" t="s">
         <v>14</v>
       </c>
       <c r="D56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E56">
         <v>18</v>
@@ -3029,13 +2980,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C57" t="s">
         <v>7</v>
       </c>
       <c r="D57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E57">
         <v>4</v>
@@ -3049,13 +3000,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C58" t="s">
         <v>9</v>
       </c>
       <c r="D58" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E58">
         <v>6</v>
@@ -3069,13 +3020,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C59" t="s">
         <v>19</v>
       </c>
       <c r="D59" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E59">
         <v>4</v>
@@ -3089,13 +3040,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C60" t="s">
         <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E60">
         <v>4</v>
@@ -3109,13 +3060,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C61" t="s">
         <v>4</v>
       </c>
       <c r="D61" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E61">
         <v>4</v>
@@ -3129,13 +3080,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C62" t="s">
         <v>17</v>
       </c>
       <c r="D62" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E62">
         <v>4</v>
@@ -3149,13 +3100,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C63" t="s">
         <v>9</v>
       </c>
       <c r="D63" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E63">
         <v>6</v>
@@ -3169,13 +3120,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C64" t="s">
         <v>7</v>
       </c>
       <c r="D64" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E64">
         <v>4</v>
@@ -3189,13 +3140,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C65" t="s">
         <v>28</v>
       </c>
       <c r="D65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E65">
         <v>5</v>
@@ -3209,13 +3160,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C66" t="s">
         <v>22</v>
       </c>
       <c r="D66" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E66">
         <v>14</v>
@@ -3229,13 +3180,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C67" t="s">
         <v>19</v>
       </c>
       <c r="D67" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E67">
         <v>4</v>
@@ -3249,13 +3200,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C68" t="s">
         <v>8</v>
       </c>
       <c r="D68" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E68">
         <v>14</v>
@@ -3269,13 +3220,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C69" t="s">
         <v>4</v>
       </c>
       <c r="D69" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E69">
         <v>4</v>
@@ -3289,13 +3240,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C70" t="s">
         <v>26</v>
       </c>
       <c r="D70" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E70">
         <v>18</v>
@@ -3309,13 +3260,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C71" t="s">
         <v>10</v>
       </c>
       <c r="D71" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E71">
         <v>4</v>
@@ -3329,13 +3280,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C72" t="s">
         <v>29</v>
       </c>
       <c r="D72" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E72">
         <v>12</v>
@@ -3349,13 +3300,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C73" t="s">
         <v>12</v>
       </c>
       <c r="D73" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E73">
         <v>7</v>
@@ -3369,13 +3320,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C74" t="s">
         <v>13</v>
       </c>
       <c r="D74" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E74">
         <v>2</v>
@@ -3389,13 +3340,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C75" t="s">
         <v>14</v>
       </c>
       <c r="D75" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E75">
         <v>18</v>
@@ -3409,13 +3360,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C76" t="s">
         <v>10</v>
       </c>
       <c r="D76" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E76">
         <v>4</v>
@@ -3429,13 +3380,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E77">
         <v>3</v>
@@ -3449,13 +3400,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C78" t="s">
         <v>5</v>
       </c>
       <c r="D78" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E78">
         <v>5</v>
@@ -3469,13 +3420,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C79" t="s">
         <v>9</v>
       </c>
       <c r="D79" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E79">
         <v>4</v>
@@ -3489,13 +3440,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C80" t="s">
         <v>7</v>
       </c>
       <c r="D80" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E80">
         <v>3</v>
@@ -3509,13 +3460,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C81" t="s">
         <v>4</v>
       </c>
       <c r="D81" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E81">
         <v>4</v>
@@ -3539,21 +3490,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2">
         <v>8039.66</v>
@@ -3567,7 +3518,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B3">
         <v>8039.66</v>
@@ -3581,7 +3532,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B4">
         <v>8039.66</v>
@@ -3595,7 +3546,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B5">
         <v>6559.66</v>
@@ -3609,7 +3560,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B6">
         <v>4979.93</v>
@@ -3623,7 +3574,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B7">
         <v>4979.93</v>
@@ -3637,7 +3588,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B8">
         <v>4979.93</v>
@@ -3651,7 +3602,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B9">
         <v>4979.93</v>
@@ -3665,7 +3616,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B10">
         <v>4979.93</v>
@@ -3679,7 +3630,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B11">
         <v>3242.84</v>
@@ -3693,7 +3644,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B12">
         <v>1734.2</v>
@@ -3707,7 +3658,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B13">
         <v>1858.54</v>
@@ -3721,7 +3672,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B14">
         <v>1858.54</v>
@@ -3735,7 +3686,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B15">
         <v>1858.54</v>
@@ -3749,7 +3700,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B16">
         <v>2140.56</v>
@@ -3763,7 +3714,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B17">
         <v>5590.56</v>
@@ -3777,7 +3728,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B18">
         <v>8202.52</v>
@@ -3791,7 +3742,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B19">
         <v>8202.52</v>
@@ -3805,7 +3756,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B20">
         <v>7386.9400000000014</v>
@@ -3819,7 +3770,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B21">
         <v>6767.2400000000016</v>
@@ -3833,7 +3784,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B22">
         <v>7733.7200000000012</v>
@@ -3847,7 +3798,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B23">
         <v>8370.18</v>
@@ -3861,7 +3812,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B24">
         <v>8370.18</v>
@@ -3875,7 +3826,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B25">
         <v>8370.18</v>
@@ -3889,7 +3840,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B26">
         <v>8370.18</v>
@@ -3903,7 +3854,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B27">
         <v>5922.63</v>
@@ -3917,7 +3868,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B28">
         <v>5922.63</v>
@@ -3931,7 +3882,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B29">
         <v>5922.63</v>
@@ -3945,7 +3896,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B30">
         <v>5922.63</v>
@@ -3959,7 +3910,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B31">
         <v>4784.01</v>
@@ -3973,7 +3924,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B32">
         <v>3877.9700000000012</v>
@@ -3987,7 +3938,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B33">
         <v>3877.9700000000012</v>
@@ -4001,7 +3952,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B34">
         <v>3877.9700000000012</v>
@@ -4015,7 +3966,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B35">
         <v>3877.9700000000012</v>
@@ -4029,7 +3980,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B36">
         <v>3877.9700000000012</v>
@@ -4043,7 +3994,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B37">
         <v>3877.9700000000012</v>
@@ -4057,7 +4008,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B38">
         <v>3877.9700000000012</v>
@@ -4071,7 +4022,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B39">
         <v>3877.9700000000012</v>
@@ -4085,7 +4036,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B40">
         <v>5740.5700000000024</v>
@@ -4099,7 +4050,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B41">
         <v>5740.5700000000024</v>
@@ -4113,7 +4064,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B42">
         <v>5740.5700000000024</v>
@@ -4127,7 +4078,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B43">
         <v>5740.5700000000024</v>
@@ -4141,7 +4092,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B44">
         <v>6986.0300000000016</v>
@@ -4155,7 +4106,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B45">
         <v>7911.590000000002</v>
@@ -4169,7 +4120,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B46">
         <v>7911.590000000002</v>
@@ -4183,7 +4134,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B47">
         <v>7911.590000000002</v>
@@ -4197,7 +4148,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B48">
         <v>8511.65</v>
@@ -4211,7 +4162,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B49">
         <v>8511.65</v>
@@ -4225,7 +4176,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B50">
         <v>9361.4499999999989</v>
@@ -4239,7 +4190,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B51">
         <v>9361.4499999999989</v>
@@ -4253,7 +4204,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B52">
         <v>8450.8299999999981</v>
@@ -4267,7 +4218,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B53">
         <v>8450.8299999999981</v>
@@ -4281,7 +4232,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B54">
         <v>7644.3499999999995</v>
@@ -4295,7 +4246,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B55">
         <v>5699.29</v>
@@ -4309,7 +4260,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B56">
         <v>5181.6899999999996</v>
@@ -4323,7 +4274,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B57">
         <v>4729.29</v>
@@ -4337,7 +4288,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B58">
         <v>5494.95</v>
@@ -4351,7 +4302,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B59">
         <v>5494.95</v>
@@ -4365,7 +4316,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B60">
         <v>5494.95</v>
@@ -4379,7 +4330,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B61">
         <v>5494.95</v>
@@ -4393,7 +4344,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B62">
         <v>6326.43</v>
@@ -4407,7 +4358,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B63">
         <v>6326.43</v>
@@ -4421,7 +4372,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B64">
         <v>6889.23</v>
@@ -4435,7 +4386,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B65">
         <v>7431.6299999999992</v>
@@ -4449,7 +4400,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B66">
         <v>7431.6299999999992</v>
@@ -4463,7 +4414,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B67">
         <v>7431.6299999999992</v>
@@ -4477,7 +4428,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B68">
         <v>7431.6299999999992</v>
@@ -4491,7 +4442,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B69">
         <v>7431.6299999999992</v>
@@ -4505,7 +4456,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B70">
         <v>7324.91</v>
@@ -4519,7 +4470,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B71">
         <v>6593.51</v>
@@ -4533,7 +4484,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B72">
         <v>5382.41</v>
@@ -4547,7 +4498,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B73">
         <v>5382.41</v>
@@ -4561,7 +4512,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B74">
         <v>6299.51</v>
@@ -4575,7 +4526,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B75">
         <v>6299.51</v>
@@ -4589,7 +4540,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B76">
         <v>6299.51</v>
@@ -4603,7 +4554,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B77">
         <v>2898.27</v>

</xml_diff>

<commit_message>
fix market value updates each trading day
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -938,16 +938,16 @@
         <v>52.96</v>
       </c>
       <c r="C2" t="n">
-        <v>52.96</v>
+        <v>47.2</v>
       </c>
       <c r="D2" t="n">
         <v>18</v>
       </c>
       <c r="E2" t="n">
-        <v>953.28</v>
+        <v>849.6</v>
       </c>
       <c r="F2" t="n">
-        <v>24.80620155038761</v>
+        <v>30.42452830188694</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
         <v>137.78</v>
       </c>
       <c r="C3" t="n">
-        <v>137.78</v>
+        <v>125.98</v>
       </c>
       <c r="D3" t="n">
         <v>7</v>
       </c>
       <c r="E3" t="n">
-        <v>964.46</v>
+        <v>881.86</v>
       </c>
       <c r="F3" t="n">
-        <v>29.24528301886784</v>
+        <v>45.43269230769231</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -992,16 +992,16 @@
         <v>59.28</v>
       </c>
       <c r="C4" t="n">
-        <v>59.28</v>
+        <v>56</v>
       </c>
       <c r="D4" t="n">
         <v>16</v>
       </c>
       <c r="E4" t="n">
-        <v>948.48</v>
+        <v>896</v>
       </c>
       <c r="F4" t="n">
-        <v>29.85915492957741</v>
+        <v>45.59686888454011</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -1019,16 +1019,16 @@
         <v>36.98</v>
       </c>
       <c r="C5" t="n">
-        <v>36.98</v>
+        <v>34.39</v>
       </c>
       <c r="D5" t="n">
         <v>27</v>
       </c>
       <c r="E5" t="n">
-        <v>998.4599999999999</v>
+        <v>928.53</v>
       </c>
       <c r="F5" t="n">
-        <v>21.7967599410898</v>
+        <v>49.08424908424913</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -1046,16 +1046,16 @@
         <v>75.04000000000001</v>
       </c>
       <c r="C6" t="n">
-        <v>75.04000000000001</v>
+        <v>73.13</v>
       </c>
       <c r="D6" t="n">
         <v>13</v>
       </c>
       <c r="E6" t="n">
-        <v>975.5200000000001</v>
+        <v>950.6899999999999</v>
       </c>
       <c r="F6" t="n">
-        <v>16.82953311617815</v>
+        <v>40.69400630914822</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -1073,16 +1073,16 @@
         <v>129.87</v>
       </c>
       <c r="C7" t="n">
-        <v>129.87</v>
+        <v>121.42</v>
       </c>
       <c r="D7" t="n">
         <v>7</v>
       </c>
       <c r="E7" t="n">
-        <v>909.09</v>
+        <v>849.9400000000001</v>
       </c>
       <c r="F7" t="n">
-        <v>6.539833531510226</v>
+        <v>32.84612261469755</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -1100,16 +1100,16 @@
         <v>234.51</v>
       </c>
       <c r="C8" t="n">
-        <v>234.51</v>
+        <v>231.6</v>
       </c>
       <c r="D8" t="n">
         <v>4</v>
       </c>
       <c r="E8" t="n">
-        <v>938.04</v>
+        <v>926.4</v>
       </c>
       <c r="F8" t="n">
-        <v>28.69097429766896</v>
+        <v>37.52994410433855</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -1127,16 +1127,16 @@
         <v>45.43</v>
       </c>
       <c r="C9" t="n">
-        <v>45.43</v>
+        <v>46.25</v>
       </c>
       <c r="D9" t="n">
         <v>22</v>
       </c>
       <c r="E9" t="n">
-        <v>999.46</v>
+        <v>1017.5</v>
       </c>
       <c r="F9" t="n">
-        <v>24.66539196940727</v>
+        <v>55.15370705244122</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -1154,16 +1154,16 @@
         <v>136.39</v>
       </c>
       <c r="C10" t="n">
-        <v>136.39</v>
+        <v>133.35</v>
       </c>
       <c r="D10" t="n">
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>954.7299999999999</v>
+        <v>933.4499999999999</v>
       </c>
       <c r="F10" t="n">
-        <v>27.44783306581064</v>
+        <v>24.97013142174436</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1181,16 +1181,16 @@
         <v>135.47</v>
       </c>
       <c r="C11" t="n">
-        <v>135.47</v>
+        <v>129.12</v>
       </c>
       <c r="D11" t="n">
         <v>7</v>
       </c>
       <c r="E11" t="n">
-        <v>948.29</v>
+        <v>903.84</v>
       </c>
       <c r="F11" t="n">
-        <v>24.68220338983049</v>
+        <v>19.86928104575172</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1208,16 +1208,16 @@
         <v>156.22</v>
       </c>
       <c r="C12" t="n">
-        <v>156.22</v>
+        <v>156.1</v>
       </c>
       <c r="D12" t="n">
         <v>6</v>
       </c>
       <c r="E12" t="n">
-        <v>937.3199999999999</v>
+        <v>936.5999999999999</v>
       </c>
       <c r="F12" t="n">
-        <v>21.83523107836568</v>
+        <v>33.95297977036628</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11287</v>
+        <v>10834</v>
       </c>
     </row>
     <row r="4">
@@ -1310,7 +1310,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11641</v>
+        <v>11188</v>
       </c>
     </row>
   </sheetData>
@@ -5066,10 +5066,10 @@
         <v>8196</v>
       </c>
       <c r="C3" t="n">
-        <v>1803</v>
+        <v>1825</v>
       </c>
       <c r="D3" t="n">
-        <v>9999</v>
+        <v>10021</v>
       </c>
     </row>
     <row r="4">
@@ -5082,10 +5082,10 @@
         <v>8196</v>
       </c>
       <c r="C4" t="n">
-        <v>1803</v>
+        <v>1806</v>
       </c>
       <c r="D4" t="n">
-        <v>9999</v>
+        <v>10002</v>
       </c>
     </row>
     <row r="5">
@@ -5098,10 +5098,10 @@
         <v>7225</v>
       </c>
       <c r="C5" t="n">
-        <v>2774</v>
+        <v>2770</v>
       </c>
       <c r="D5" t="n">
-        <v>9999</v>
+        <v>9995</v>
       </c>
     </row>
     <row r="6">
@@ -5114,10 +5114,10 @@
         <v>5317</v>
       </c>
       <c r="C6" t="n">
-        <v>4681</v>
+        <v>4669</v>
       </c>
       <c r="D6" t="n">
-        <v>9998</v>
+        <v>9986</v>
       </c>
     </row>
     <row r="7">
@@ -5130,10 +5130,10 @@
         <v>2429</v>
       </c>
       <c r="C7" t="n">
-        <v>7568</v>
+        <v>7566</v>
       </c>
       <c r="D7" t="n">
-        <v>9997</v>
+        <v>9995</v>
       </c>
     </row>
     <row r="8">
@@ -5146,10 +5146,10 @@
         <v>2429</v>
       </c>
       <c r="C8" t="n">
-        <v>7568</v>
+        <v>7555</v>
       </c>
       <c r="D8" t="n">
-        <v>9997</v>
+        <v>9984</v>
       </c>
     </row>
     <row r="9">
@@ -5162,10 +5162,10 @@
         <v>2429</v>
       </c>
       <c r="C9" t="n">
-        <v>7568</v>
+        <v>7521</v>
       </c>
       <c r="D9" t="n">
-        <v>9997</v>
+        <v>9950</v>
       </c>
     </row>
     <row r="10">
@@ -5178,10 +5178,10 @@
         <v>2429</v>
       </c>
       <c r="C10" t="n">
-        <v>7568</v>
+        <v>7537</v>
       </c>
       <c r="D10" t="n">
-        <v>9997</v>
+        <v>9966</v>
       </c>
     </row>
     <row r="11">
@@ -5194,10 +5194,10 @@
         <v>2429</v>
       </c>
       <c r="C11" t="n">
-        <v>7568</v>
+        <v>7554</v>
       </c>
       <c r="D11" t="n">
-        <v>9997</v>
+        <v>9983</v>
       </c>
     </row>
     <row r="12">
@@ -5210,10 +5210,10 @@
         <v>2429</v>
       </c>
       <c r="C12" t="n">
-        <v>7568</v>
+        <v>7565</v>
       </c>
       <c r="D12" t="n">
-        <v>9997</v>
+        <v>9994</v>
       </c>
     </row>
     <row r="13">
@@ -5226,10 +5226,10 @@
         <v>3407</v>
       </c>
       <c r="C13" t="n">
-        <v>6621</v>
+        <v>6613</v>
       </c>
       <c r="D13" t="n">
-        <v>10028</v>
+        <v>10020</v>
       </c>
     </row>
     <row r="14">
@@ -5242,10 +5242,10 @@
         <v>3407</v>
       </c>
       <c r="C14" t="n">
-        <v>6621</v>
+        <v>6611</v>
       </c>
       <c r="D14" t="n">
-        <v>10028</v>
+        <v>10018</v>
       </c>
     </row>
     <row r="15">
@@ -5258,10 +5258,10 @@
         <v>3407</v>
       </c>
       <c r="C15" t="n">
-        <v>6621</v>
+        <v>6611</v>
       </c>
       <c r="D15" t="n">
-        <v>10028</v>
+        <v>10018</v>
       </c>
     </row>
     <row r="16">
@@ -5274,10 +5274,10 @@
         <v>1487</v>
       </c>
       <c r="C16" t="n">
-        <v>8540</v>
+        <v>8481</v>
       </c>
       <c r="D16" t="n">
-        <v>10027</v>
+        <v>9968</v>
       </c>
     </row>
     <row r="17">
@@ -5290,10 +5290,10 @@
         <v>2471</v>
       </c>
       <c r="C17" t="n">
-        <v>7580</v>
+        <v>7440</v>
       </c>
       <c r="D17" t="n">
-        <v>10051</v>
+        <v>9911</v>
       </c>
     </row>
     <row r="18">
@@ -5306,10 +5306,10 @@
         <v>2471</v>
       </c>
       <c r="C18" t="n">
-        <v>7580</v>
+        <v>7423</v>
       </c>
       <c r="D18" t="n">
-        <v>10051</v>
+        <v>9894</v>
       </c>
     </row>
     <row r="19">
@@ -5322,10 +5322,10 @@
         <v>1515</v>
       </c>
       <c r="C19" t="n">
-        <v>8535</v>
+        <v>8271</v>
       </c>
       <c r="D19" t="n">
-        <v>10050</v>
+        <v>9786</v>
       </c>
     </row>
     <row r="20">
@@ -5338,10 +5338,10 @@
         <v>675</v>
       </c>
       <c r="C20" t="n">
-        <v>9375</v>
+        <v>8992</v>
       </c>
       <c r="D20" t="n">
-        <v>10050</v>
+        <v>9667</v>
       </c>
     </row>
     <row r="21">
@@ -5354,10 +5354,10 @@
         <v>675</v>
       </c>
       <c r="C21" t="n">
-        <v>9375</v>
+        <v>8987</v>
       </c>
       <c r="D21" t="n">
-        <v>10050</v>
+        <v>9662</v>
       </c>
     </row>
     <row r="22">
@@ -5370,10 +5370,10 @@
         <v>675</v>
       </c>
       <c r="C22" t="n">
-        <v>9375</v>
+        <v>8995</v>
       </c>
       <c r="D22" t="n">
-        <v>10050</v>
+        <v>9670</v>
       </c>
     </row>
     <row r="23">
@@ -5386,10 +5386,10 @@
         <v>675</v>
       </c>
       <c r="C23" t="n">
-        <v>9375</v>
+        <v>8996</v>
       </c>
       <c r="D23" t="n">
-        <v>10050</v>
+        <v>9671</v>
       </c>
     </row>
     <row r="24">
@@ -5402,10 +5402,10 @@
         <v>675</v>
       </c>
       <c r="C24" t="n">
-        <v>9375</v>
+        <v>8773</v>
       </c>
       <c r="D24" t="n">
-        <v>10050</v>
+        <v>9448</v>
       </c>
     </row>
     <row r="25">
@@ -5418,10 +5418,10 @@
         <v>675</v>
       </c>
       <c r="C25" t="n">
-        <v>9375</v>
+        <v>8768</v>
       </c>
       <c r="D25" t="n">
-        <v>10050</v>
+        <v>9443</v>
       </c>
     </row>
     <row r="26">
@@ -5434,10 +5434,10 @@
         <v>675</v>
       </c>
       <c r="C26" t="n">
-        <v>9375</v>
+        <v>8884</v>
       </c>
       <c r="D26" t="n">
-        <v>10050</v>
+        <v>9559</v>
       </c>
     </row>
     <row r="27">
@@ -5450,10 +5450,10 @@
         <v>1657</v>
       </c>
       <c r="C27" t="n">
-        <v>8440</v>
+        <v>8061</v>
       </c>
       <c r="D27" t="n">
-        <v>10097</v>
+        <v>9718</v>
       </c>
     </row>
     <row r="28">
@@ -5466,10 +5466,10 @@
         <v>681</v>
       </c>
       <c r="C28" t="n">
-        <v>9416</v>
+        <v>9022</v>
       </c>
       <c r="D28" t="n">
-        <v>10097</v>
+        <v>9703</v>
       </c>
     </row>
     <row r="29">
@@ -5482,10 +5482,10 @@
         <v>681</v>
       </c>
       <c r="C29" t="n">
-        <v>9416</v>
+        <v>8925</v>
       </c>
       <c r="D29" t="n">
-        <v>10097</v>
+        <v>9606</v>
       </c>
     </row>
     <row r="30">
@@ -5498,10 +5498,10 @@
         <v>681</v>
       </c>
       <c r="C30" t="n">
-        <v>9416</v>
+        <v>8936</v>
       </c>
       <c r="D30" t="n">
-        <v>10097</v>
+        <v>9617</v>
       </c>
     </row>
     <row r="31">
@@ -5514,10 +5514,10 @@
         <v>681</v>
       </c>
       <c r="C31" t="n">
-        <v>9416</v>
+        <v>8979</v>
       </c>
       <c r="D31" t="n">
-        <v>10097</v>
+        <v>9660</v>
       </c>
     </row>
     <row r="32">
@@ -5530,10 +5530,10 @@
         <v>681</v>
       </c>
       <c r="C32" t="n">
-        <v>9416</v>
+        <v>9040</v>
       </c>
       <c r="D32" t="n">
-        <v>10097</v>
+        <v>9721</v>
       </c>
     </row>
     <row r="33">
@@ -5546,10 +5546,10 @@
         <v>681</v>
       </c>
       <c r="C33" t="n">
-        <v>9416</v>
+        <v>8958</v>
       </c>
       <c r="D33" t="n">
-        <v>10097</v>
+        <v>9639</v>
       </c>
     </row>
     <row r="34">
@@ -5562,10 +5562,10 @@
         <v>2543</v>
       </c>
       <c r="C34" t="n">
-        <v>7492</v>
+        <v>7068</v>
       </c>
       <c r="D34" t="n">
-        <v>10035</v>
+        <v>9611</v>
       </c>
     </row>
     <row r="35">
@@ -5578,10 +5578,10 @@
         <v>2543</v>
       </c>
       <c r="C35" t="n">
-        <v>7492</v>
+        <v>7068</v>
       </c>
       <c r="D35" t="n">
-        <v>10035</v>
+        <v>9611</v>
       </c>
     </row>
     <row r="36">
@@ -5594,10 +5594,10 @@
         <v>2543</v>
       </c>
       <c r="C36" t="n">
-        <v>7492</v>
+        <v>7002</v>
       </c>
       <c r="D36" t="n">
-        <v>10035</v>
+        <v>9545</v>
       </c>
     </row>
     <row r="37">
@@ -5610,10 +5610,10 @@
         <v>2543</v>
       </c>
       <c r="C37" t="n">
-        <v>7492</v>
+        <v>7019</v>
       </c>
       <c r="D37" t="n">
-        <v>10035</v>
+        <v>9562</v>
       </c>
     </row>
     <row r="38">
@@ -5626,10 +5626,10 @@
         <v>775</v>
       </c>
       <c r="C38" t="n">
-        <v>9258</v>
+        <v>8784</v>
       </c>
       <c r="D38" t="n">
-        <v>10033</v>
+        <v>9559</v>
       </c>
     </row>
     <row r="39">
@@ -5642,10 +5642,10 @@
         <v>775</v>
       </c>
       <c r="C39" t="n">
-        <v>9258</v>
+        <v>8739</v>
       </c>
       <c r="D39" t="n">
-        <v>10033</v>
+        <v>9514</v>
       </c>
     </row>
     <row r="40">
@@ -5658,10 +5658,10 @@
         <v>775</v>
       </c>
       <c r="C40" t="n">
-        <v>9258</v>
+        <v>8448</v>
       </c>
       <c r="D40" t="n">
-        <v>10033</v>
+        <v>9223</v>
       </c>
     </row>
     <row r="41">
@@ -5674,10 +5674,10 @@
         <v>775</v>
       </c>
       <c r="C41" t="n">
-        <v>9258</v>
+        <v>8205</v>
       </c>
       <c r="D41" t="n">
-        <v>10033</v>
+        <v>8980</v>
       </c>
     </row>
     <row r="42">
@@ -5690,10 +5690,10 @@
         <v>775</v>
       </c>
       <c r="C42" t="n">
-        <v>9258</v>
+        <v>8153</v>
       </c>
       <c r="D42" t="n">
-        <v>10033</v>
+        <v>8928</v>
       </c>
     </row>
     <row r="43">
@@ -5706,10 +5706,10 @@
         <v>775</v>
       </c>
       <c r="C43" t="n">
-        <v>9258</v>
+        <v>7867</v>
       </c>
       <c r="D43" t="n">
-        <v>10033</v>
+        <v>8642</v>
       </c>
     </row>
     <row r="44">
@@ -5722,10 +5722,10 @@
         <v>22</v>
       </c>
       <c r="C44" t="n">
-        <v>10011</v>
+        <v>8576</v>
       </c>
       <c r="D44" t="n">
-        <v>10033</v>
+        <v>8598</v>
       </c>
     </row>
     <row r="45">
@@ -5738,10 +5738,10 @@
         <v>22</v>
       </c>
       <c r="C45" t="n">
-        <v>10011</v>
+        <v>8935</v>
       </c>
       <c r="D45" t="n">
-        <v>10033</v>
+        <v>8957</v>
       </c>
     </row>
     <row r="46">
@@ -5754,10 +5754,10 @@
         <v>22</v>
       </c>
       <c r="C46" t="n">
-        <v>10011</v>
+        <v>8643</v>
       </c>
       <c r="D46" t="n">
-        <v>10033</v>
+        <v>8665</v>
       </c>
     </row>
     <row r="47">
@@ -5770,10 +5770,10 @@
         <v>22</v>
       </c>
       <c r="C47" t="n">
-        <v>10011</v>
+        <v>9053</v>
       </c>
       <c r="D47" t="n">
-        <v>10033</v>
+        <v>9075</v>
       </c>
     </row>
     <row r="48">
@@ -5786,10 +5786,10 @@
         <v>22</v>
       </c>
       <c r="C48" t="n">
-        <v>10011</v>
+        <v>8800</v>
       </c>
       <c r="D48" t="n">
-        <v>10033</v>
+        <v>8822</v>
       </c>
     </row>
     <row r="49">
@@ -5802,10 +5802,10 @@
         <v>22</v>
       </c>
       <c r="C49" t="n">
-        <v>10011</v>
+        <v>8762</v>
       </c>
       <c r="D49" t="n">
-        <v>10033</v>
+        <v>8784</v>
       </c>
     </row>
     <row r="50">
@@ -5818,10 +5818,10 @@
         <v>22</v>
       </c>
       <c r="C50" t="n">
-        <v>10011</v>
+        <v>8042</v>
       </c>
       <c r="D50" t="n">
-        <v>10033</v>
+        <v>8064</v>
       </c>
     </row>
     <row r="51">
@@ -5834,10 +5834,10 @@
         <v>22</v>
       </c>
       <c r="C51" t="n">
-        <v>10011</v>
+        <v>8347</v>
       </c>
       <c r="D51" t="n">
-        <v>10033</v>
+        <v>8369</v>
       </c>
     </row>
     <row r="52">
@@ -5850,10 +5850,10 @@
         <v>22</v>
       </c>
       <c r="C52" t="n">
-        <v>10011</v>
+        <v>7899</v>
       </c>
       <c r="D52" t="n">
-        <v>10033</v>
+        <v>7921</v>
       </c>
     </row>
     <row r="53">
@@ -5866,10 +5866,10 @@
         <v>22</v>
       </c>
       <c r="C53" t="n">
-        <v>10011</v>
+        <v>7147</v>
       </c>
       <c r="D53" t="n">
-        <v>10033</v>
+        <v>7169</v>
       </c>
     </row>
     <row r="54">
@@ -5882,10 +5882,10 @@
         <v>22</v>
       </c>
       <c r="C54" t="n">
-        <v>10011</v>
+        <v>7765</v>
       </c>
       <c r="D54" t="n">
-        <v>10033</v>
+        <v>7787</v>
       </c>
     </row>
     <row r="55">
@@ -5898,10 +5898,10 @@
         <v>22</v>
       </c>
       <c r="C55" t="n">
-        <v>10011</v>
+        <v>7076</v>
       </c>
       <c r="D55" t="n">
-        <v>10033</v>
+        <v>7098</v>
       </c>
     </row>
     <row r="56">
@@ -5914,10 +5914,10 @@
         <v>22</v>
       </c>
       <c r="C56" t="n">
-        <v>10011</v>
+        <v>7556</v>
       </c>
       <c r="D56" t="n">
-        <v>10033</v>
+        <v>7578</v>
       </c>
     </row>
     <row r="57">
@@ -5930,10 +5930,10 @@
         <v>22</v>
       </c>
       <c r="C57" t="n">
-        <v>10011</v>
+        <v>7349</v>
       </c>
       <c r="D57" t="n">
-        <v>10033</v>
+        <v>7371</v>
       </c>
     </row>
     <row r="58">
@@ -5946,10 +5946,10 @@
         <v>22</v>
       </c>
       <c r="C58" t="n">
-        <v>10011</v>
+        <v>7325</v>
       </c>
       <c r="D58" t="n">
-        <v>10033</v>
+        <v>7347</v>
       </c>
     </row>
     <row r="59">
@@ -5962,10 +5962,10 @@
         <v>22</v>
       </c>
       <c r="C59" t="n">
-        <v>10011</v>
+        <v>6932</v>
       </c>
       <c r="D59" t="n">
-        <v>10033</v>
+        <v>6954</v>
       </c>
     </row>
     <row r="60">
@@ -5978,10 +5978,10 @@
         <v>22</v>
       </c>
       <c r="C60" t="n">
-        <v>10011</v>
+        <v>6622</v>
       </c>
       <c r="D60" t="n">
-        <v>10033</v>
+        <v>6644</v>
       </c>
     </row>
     <row r="61">
@@ -5994,10 +5994,10 @@
         <v>22</v>
       </c>
       <c r="C61" t="n">
-        <v>10011</v>
+        <v>7208</v>
       </c>
       <c r="D61" t="n">
-        <v>10033</v>
+        <v>7230</v>
       </c>
     </row>
     <row r="62">
@@ -6010,10 +6010,10 @@
         <v>22</v>
       </c>
       <c r="C62" t="n">
-        <v>10011</v>
+        <v>7282</v>
       </c>
       <c r="D62" t="n">
-        <v>10033</v>
+        <v>7304</v>
       </c>
     </row>
     <row r="63">
@@ -6026,10 +6026,10 @@
         <v>22</v>
       </c>
       <c r="C63" t="n">
-        <v>10011</v>
+        <v>7708</v>
       </c>
       <c r="D63" t="n">
-        <v>10033</v>
+        <v>7730</v>
       </c>
     </row>
     <row r="64">
@@ -6042,10 +6042,10 @@
         <v>22</v>
       </c>
       <c r="C64" t="n">
-        <v>10011</v>
+        <v>7400</v>
       </c>
       <c r="D64" t="n">
-        <v>10033</v>
+        <v>7422</v>
       </c>
     </row>
     <row r="65">
@@ -6058,10 +6058,10 @@
         <v>22</v>
       </c>
       <c r="C65" t="n">
-        <v>10011</v>
+        <v>7704</v>
       </c>
       <c r="D65" t="n">
-        <v>10033</v>
+        <v>7726</v>
       </c>
     </row>
     <row r="66">
@@ -6074,10 +6074,10 @@
         <v>22</v>
       </c>
       <c r="C66" t="n">
-        <v>10011</v>
+        <v>7699</v>
       </c>
       <c r="D66" t="n">
-        <v>10033</v>
+        <v>7721</v>
       </c>
     </row>
     <row r="67">
@@ -6090,10 +6090,10 @@
         <v>22</v>
       </c>
       <c r="C67" t="n">
-        <v>10011</v>
+        <v>7404</v>
       </c>
       <c r="D67" t="n">
-        <v>10033</v>
+        <v>7426</v>
       </c>
     </row>
     <row r="68">
@@ -6106,10 +6106,10 @@
         <v>22</v>
       </c>
       <c r="C68" t="n">
-        <v>10011</v>
+        <v>7605</v>
       </c>
       <c r="D68" t="n">
-        <v>10033</v>
+        <v>7627</v>
       </c>
     </row>
     <row r="69">
@@ -6122,10 +6122,10 @@
         <v>22</v>
       </c>
       <c r="C69" t="n">
-        <v>10011</v>
+        <v>7515</v>
       </c>
       <c r="D69" t="n">
-        <v>10033</v>
+        <v>7537</v>
       </c>
     </row>
     <row r="70">
@@ -6138,10 +6138,10 @@
         <v>22</v>
       </c>
       <c r="C70" t="n">
-        <v>10011</v>
+        <v>7922</v>
       </c>
       <c r="D70" t="n">
-        <v>10033</v>
+        <v>7944</v>
       </c>
     </row>
     <row r="71">
@@ -6154,10 +6154,10 @@
         <v>22</v>
       </c>
       <c r="C71" t="n">
-        <v>10011</v>
+        <v>7982</v>
       </c>
       <c r="D71" t="n">
-        <v>10033</v>
+        <v>8004</v>
       </c>
     </row>
     <row r="72">
@@ -6170,10 +6170,10 @@
         <v>22</v>
       </c>
       <c r="C72" t="n">
-        <v>10011</v>
+        <v>8323</v>
       </c>
       <c r="D72" t="n">
-        <v>10033</v>
+        <v>8345</v>
       </c>
     </row>
     <row r="73">
@@ -6186,10 +6186,10 @@
         <v>22</v>
       </c>
       <c r="C73" t="n">
-        <v>10011</v>
+        <v>8395</v>
       </c>
       <c r="D73" t="n">
-        <v>10033</v>
+        <v>8417</v>
       </c>
     </row>
     <row r="74">
@@ -6202,10 +6202,10 @@
         <v>22</v>
       </c>
       <c r="C74" t="n">
-        <v>10011</v>
+        <v>8395</v>
       </c>
       <c r="D74" t="n">
-        <v>10033</v>
+        <v>8417</v>
       </c>
     </row>
     <row r="75">
@@ -6218,10 +6218,10 @@
         <v>22</v>
       </c>
       <c r="C75" t="n">
-        <v>10011</v>
+        <v>8222</v>
       </c>
       <c r="D75" t="n">
-        <v>10033</v>
+        <v>8244</v>
       </c>
     </row>
     <row r="76">
@@ -6234,10 +6234,10 @@
         <v>22</v>
       </c>
       <c r="C76" t="n">
-        <v>10011</v>
+        <v>8420</v>
       </c>
       <c r="D76" t="n">
-        <v>10033</v>
+        <v>8442</v>
       </c>
     </row>
     <row r="77">
@@ -6250,10 +6250,10 @@
         <v>884</v>
       </c>
       <c r="C77" t="n">
-        <v>9150</v>
+        <v>7368</v>
       </c>
       <c r="D77" t="n">
-        <v>10034</v>
+        <v>8252</v>
       </c>
     </row>
     <row r="78">
@@ -6266,10 +6266,10 @@
         <v>1768</v>
       </c>
       <c r="C78" t="n">
-        <v>8397</v>
+        <v>6503</v>
       </c>
       <c r="D78" t="n">
-        <v>10165</v>
+        <v>8271</v>
       </c>
     </row>
     <row r="79">
@@ -6282,10 +6282,10 @@
         <v>1768</v>
       </c>
       <c r="C79" t="n">
-        <v>8397</v>
+        <v>6738</v>
       </c>
       <c r="D79" t="n">
-        <v>10165</v>
+        <v>8506</v>
       </c>
     </row>
     <row r="80">
@@ -6298,10 +6298,10 @@
         <v>1768</v>
       </c>
       <c r="C80" t="n">
-        <v>8397</v>
+        <v>6556</v>
       </c>
       <c r="D80" t="n">
-        <v>10165</v>
+        <v>8324</v>
       </c>
     </row>
     <row r="81">
@@ -6314,10 +6314,10 @@
         <v>1768</v>
       </c>
       <c r="C81" t="n">
-        <v>8397</v>
+        <v>6396</v>
       </c>
       <c r="D81" t="n">
-        <v>10165</v>
+        <v>8164</v>
       </c>
     </row>
     <row r="82">
@@ -6330,10 +6330,10 @@
         <v>1768</v>
       </c>
       <c r="C82" t="n">
-        <v>8397</v>
+        <v>6502</v>
       </c>
       <c r="D82" t="n">
-        <v>10165</v>
+        <v>8270</v>
       </c>
     </row>
     <row r="83">
@@ -6346,10 +6346,10 @@
         <v>1768</v>
       </c>
       <c r="C83" t="n">
-        <v>8397</v>
+        <v>6575</v>
       </c>
       <c r="D83" t="n">
-        <v>10165</v>
+        <v>8343</v>
       </c>
     </row>
     <row r="84">
@@ -6362,10 +6362,10 @@
         <v>782</v>
       </c>
       <c r="C84" t="n">
-        <v>9383</v>
+        <v>7632</v>
       </c>
       <c r="D84" t="n">
-        <v>10165</v>
+        <v>8414</v>
       </c>
     </row>
     <row r="85">
@@ -6378,10 +6378,10 @@
         <v>1759</v>
       </c>
       <c r="C85" t="n">
-        <v>8407</v>
+        <v>6864</v>
       </c>
       <c r="D85" t="n">
-        <v>10166</v>
+        <v>8623</v>
       </c>
     </row>
     <row r="86">
@@ -6394,10 +6394,10 @@
         <v>1759</v>
       </c>
       <c r="C86" t="n">
-        <v>8407</v>
+        <v>6952</v>
       </c>
       <c r="D86" t="n">
-        <v>10166</v>
+        <v>8711</v>
       </c>
     </row>
     <row r="87">
@@ -6410,10 +6410,10 @@
         <v>2898</v>
       </c>
       <c r="C87" t="n">
-        <v>7421</v>
+        <v>6055</v>
       </c>
       <c r="D87" t="n">
-        <v>10319</v>
+        <v>8953</v>
       </c>
     </row>
     <row r="88">
@@ -6426,10 +6426,10 @@
         <v>1937</v>
       </c>
       <c r="C88" t="n">
-        <v>8382</v>
+        <v>6838</v>
       </c>
       <c r="D88" t="n">
-        <v>10319</v>
+        <v>8775</v>
       </c>
     </row>
     <row r="89">
@@ -6442,10 +6442,10 @@
         <v>78</v>
       </c>
       <c r="C89" t="n">
-        <v>10241</v>
+        <v>8466</v>
       </c>
       <c r="D89" t="n">
-        <v>10319</v>
+        <v>8544</v>
       </c>
     </row>
     <row r="90">
@@ -6458,10 +6458,10 @@
         <v>78</v>
       </c>
       <c r="C90" t="n">
-        <v>10241</v>
+        <v>8446</v>
       </c>
       <c r="D90" t="n">
-        <v>10319</v>
+        <v>8524</v>
       </c>
     </row>
     <row r="91">
@@ -6474,10 +6474,10 @@
         <v>78</v>
       </c>
       <c r="C91" t="n">
-        <v>10241</v>
+        <v>8465</v>
       </c>
       <c r="D91" t="n">
-        <v>10319</v>
+        <v>8543</v>
       </c>
     </row>
     <row r="92">
@@ -6490,10 +6490,10 @@
         <v>78</v>
       </c>
       <c r="C92" t="n">
-        <v>10241</v>
+        <v>8312</v>
       </c>
       <c r="D92" t="n">
-        <v>10319</v>
+        <v>8390</v>
       </c>
     </row>
     <row r="93">
@@ -6506,10 +6506,10 @@
         <v>78</v>
       </c>
       <c r="C93" t="n">
-        <v>10241</v>
+        <v>8362</v>
       </c>
       <c r="D93" t="n">
-        <v>10319</v>
+        <v>8440</v>
       </c>
     </row>
     <row r="94">
@@ -6522,10 +6522,10 @@
         <v>78</v>
       </c>
       <c r="C94" t="n">
-        <v>10241</v>
+        <v>8578</v>
       </c>
       <c r="D94" t="n">
-        <v>10319</v>
+        <v>8656</v>
       </c>
     </row>
     <row r="95">
@@ -6538,10 +6538,10 @@
         <v>78</v>
       </c>
       <c r="C95" t="n">
-        <v>10241</v>
+        <v>8509</v>
       </c>
       <c r="D95" t="n">
-        <v>10319</v>
+        <v>8587</v>
       </c>
     </row>
     <row r="96">
@@ -6554,10 +6554,10 @@
         <v>78</v>
       </c>
       <c r="C96" t="n">
-        <v>10241</v>
+        <v>8359</v>
       </c>
       <c r="D96" t="n">
-        <v>10319</v>
+        <v>8437</v>
       </c>
     </row>
     <row r="97">
@@ -6570,10 +6570,10 @@
         <v>78</v>
       </c>
       <c r="C97" t="n">
-        <v>10241</v>
+        <v>8163</v>
       </c>
       <c r="D97" t="n">
-        <v>10319</v>
+        <v>8241</v>
       </c>
     </row>
     <row r="98">
@@ -6586,10 +6586,10 @@
         <v>78</v>
       </c>
       <c r="C98" t="n">
-        <v>10241</v>
+        <v>8262</v>
       </c>
       <c r="D98" t="n">
-        <v>10319</v>
+        <v>8340</v>
       </c>
     </row>
     <row r="99">
@@ -6602,10 +6602,10 @@
         <v>95</v>
       </c>
       <c r="C99" t="n">
-        <v>10262</v>
+        <v>8290</v>
       </c>
       <c r="D99" t="n">
-        <v>10357</v>
+        <v>8385</v>
       </c>
     </row>
     <row r="100">
@@ -6618,10 +6618,10 @@
         <v>95</v>
       </c>
       <c r="C100" t="n">
-        <v>10262</v>
+        <v>8786</v>
       </c>
       <c r="D100" t="n">
-        <v>10357</v>
+        <v>8881</v>
       </c>
     </row>
     <row r="101">
@@ -6634,10 +6634,10 @@
         <v>95</v>
       </c>
       <c r="C101" t="n">
-        <v>10262</v>
+        <v>8605</v>
       </c>
       <c r="D101" t="n">
-        <v>10357</v>
+        <v>8700</v>
       </c>
     </row>
     <row r="102">
@@ -6650,10 +6650,10 @@
         <v>95</v>
       </c>
       <c r="C102" t="n">
-        <v>10262</v>
+        <v>8741</v>
       </c>
       <c r="D102" t="n">
-        <v>10357</v>
+        <v>8836</v>
       </c>
     </row>
     <row r="103">
@@ -6666,10 +6666,10 @@
         <v>95</v>
       </c>
       <c r="C103" t="n">
-        <v>10262</v>
+        <v>8736</v>
       </c>
       <c r="D103" t="n">
-        <v>10357</v>
+        <v>8831</v>
       </c>
     </row>
     <row r="104">
@@ -6682,10 +6682,10 @@
         <v>95</v>
       </c>
       <c r="C104" t="n">
-        <v>10262</v>
+        <v>8745</v>
       </c>
       <c r="D104" t="n">
-        <v>10357</v>
+        <v>8840</v>
       </c>
     </row>
     <row r="105">
@@ -6698,10 +6698,10 @@
         <v>95</v>
       </c>
       <c r="C105" t="n">
-        <v>10262</v>
+        <v>8745</v>
       </c>
       <c r="D105" t="n">
-        <v>10357</v>
+        <v>8840</v>
       </c>
     </row>
     <row r="106">
@@ -6714,10 +6714,10 @@
         <v>1294</v>
       </c>
       <c r="C106" t="n">
-        <v>9280</v>
+        <v>7923</v>
       </c>
       <c r="D106" t="n">
-        <v>10574</v>
+        <v>9217</v>
       </c>
     </row>
     <row r="107">
@@ -6730,10 +6730,10 @@
         <v>3160</v>
       </c>
       <c r="C107" t="n">
-        <v>7434</v>
+        <v>6267</v>
       </c>
       <c r="D107" t="n">
-        <v>10594</v>
+        <v>9427</v>
       </c>
     </row>
     <row r="108">
@@ -6746,10 +6746,10 @@
         <v>3160</v>
       </c>
       <c r="C108" t="n">
-        <v>7434</v>
+        <v>6207</v>
       </c>
       <c r="D108" t="n">
-        <v>10594</v>
+        <v>9367</v>
       </c>
     </row>
     <row r="109">
@@ -6762,10 +6762,10 @@
         <v>3160</v>
       </c>
       <c r="C109" t="n">
-        <v>7434</v>
+        <v>6245</v>
       </c>
       <c r="D109" t="n">
-        <v>10594</v>
+        <v>9405</v>
       </c>
     </row>
     <row r="110">
@@ -6778,10 +6778,10 @@
         <v>2181</v>
       </c>
       <c r="C110" t="n">
-        <v>8412</v>
+        <v>7248</v>
       </c>
       <c r="D110" t="n">
-        <v>10593</v>
+        <v>9429</v>
       </c>
     </row>
     <row r="111">
@@ -6794,10 +6794,10 @@
         <v>1197</v>
       </c>
       <c r="C111" t="n">
-        <v>9396</v>
+        <v>8358</v>
       </c>
       <c r="D111" t="n">
-        <v>10593</v>
+        <v>9555</v>
       </c>
     </row>
     <row r="112">
@@ -6810,10 +6810,10 @@
         <v>2128</v>
       </c>
       <c r="C112" t="n">
-        <v>8478</v>
+        <v>7554</v>
       </c>
       <c r="D112" t="n">
-        <v>10606</v>
+        <v>9682</v>
       </c>
     </row>
     <row r="113">
@@ -6826,10 +6826,10 @@
         <v>3013</v>
       </c>
       <c r="C113" t="n">
-        <v>7523</v>
+        <v>6705</v>
       </c>
       <c r="D113" t="n">
-        <v>10536</v>
+        <v>9718</v>
       </c>
     </row>
     <row r="114">
@@ -6842,10 +6842,10 @@
         <v>3013</v>
       </c>
       <c r="C114" t="n">
-        <v>7523</v>
+        <v>6842</v>
       </c>
       <c r="D114" t="n">
-        <v>10536</v>
+        <v>9855</v>
       </c>
     </row>
     <row r="115">
@@ -6858,10 +6858,10 @@
         <v>3013</v>
       </c>
       <c r="C115" t="n">
-        <v>7523</v>
+        <v>6966</v>
       </c>
       <c r="D115" t="n">
-        <v>10536</v>
+        <v>9979</v>
       </c>
     </row>
     <row r="116">
@@ -6874,10 +6874,10 @@
         <v>3013</v>
       </c>
       <c r="C116" t="n">
-        <v>7523</v>
+        <v>6851</v>
       </c>
       <c r="D116" t="n">
-        <v>10536</v>
+        <v>9864</v>
       </c>
     </row>
     <row r="117">
@@ -6890,10 +6890,10 @@
         <v>3013</v>
       </c>
       <c r="C117" t="n">
-        <v>7523</v>
+        <v>6736</v>
       </c>
       <c r="D117" t="n">
-        <v>10536</v>
+        <v>9749</v>
       </c>
     </row>
     <row r="118">
@@ -6906,10 +6906,10 @@
         <v>3013</v>
       </c>
       <c r="C118" t="n">
-        <v>7523</v>
+        <v>6283</v>
       </c>
       <c r="D118" t="n">
-        <v>10536</v>
+        <v>9296</v>
       </c>
     </row>
     <row r="119">
@@ -6922,10 +6922,10 @@
         <v>3013</v>
       </c>
       <c r="C119" t="n">
-        <v>7523</v>
+        <v>6365</v>
       </c>
       <c r="D119" t="n">
-        <v>10536</v>
+        <v>9378</v>
       </c>
     </row>
     <row r="120">
@@ -6938,10 +6938,10 @@
         <v>3013</v>
       </c>
       <c r="C120" t="n">
-        <v>7523</v>
+        <v>6371</v>
       </c>
       <c r="D120" t="n">
-        <v>10536</v>
+        <v>9384</v>
       </c>
     </row>
     <row r="121">
@@ -6954,10 +6954,10 @@
         <v>3013</v>
       </c>
       <c r="C121" t="n">
-        <v>7523</v>
+        <v>6467</v>
       </c>
       <c r="D121" t="n">
-        <v>10536</v>
+        <v>9480</v>
       </c>
     </row>
     <row r="122">
@@ -6970,10 +6970,10 @@
         <v>3013</v>
       </c>
       <c r="C122" t="n">
-        <v>7523</v>
+        <v>6408</v>
       </c>
       <c r="D122" t="n">
-        <v>10536</v>
+        <v>9421</v>
       </c>
     </row>
     <row r="123">
@@ -6986,10 +6986,10 @@
         <v>3013</v>
       </c>
       <c r="C123" t="n">
-        <v>7523</v>
+        <v>6404</v>
       </c>
       <c r="D123" t="n">
-        <v>10536</v>
+        <v>9417</v>
       </c>
     </row>
     <row r="124">
@@ -7002,10 +7002,10 @@
         <v>198</v>
       </c>
       <c r="C124" t="n">
-        <v>10336</v>
+        <v>9250</v>
       </c>
       <c r="D124" t="n">
-        <v>10534</v>
+        <v>9448</v>
       </c>
     </row>
     <row r="125">
@@ -7018,10 +7018,10 @@
         <v>198</v>
       </c>
       <c r="C125" t="n">
-        <v>10336</v>
+        <v>9241</v>
       </c>
       <c r="D125" t="n">
-        <v>10534</v>
+        <v>9439</v>
       </c>
     </row>
     <row r="126">
@@ -7034,10 +7034,10 @@
         <v>198</v>
       </c>
       <c r="C126" t="n">
-        <v>10336</v>
+        <v>9253</v>
       </c>
       <c r="D126" t="n">
-        <v>10534</v>
+        <v>9451</v>
       </c>
     </row>
     <row r="127">
@@ -7050,10 +7050,10 @@
         <v>198</v>
       </c>
       <c r="C127" t="n">
-        <v>10336</v>
+        <v>8974</v>
       </c>
       <c r="D127" t="n">
-        <v>10534</v>
+        <v>9172</v>
       </c>
     </row>
     <row r="128">
@@ -7066,10 +7066,10 @@
         <v>80</v>
       </c>
       <c r="C128" t="n">
-        <v>10468</v>
+        <v>9203</v>
       </c>
       <c r="D128" t="n">
-        <v>10548</v>
+        <v>9283</v>
       </c>
     </row>
     <row r="129">
@@ -7082,10 +7082,10 @@
         <v>80</v>
       </c>
       <c r="C129" t="n">
-        <v>10468</v>
+        <v>9013</v>
       </c>
       <c r="D129" t="n">
-        <v>10548</v>
+        <v>9093</v>
       </c>
     </row>
     <row r="130">
@@ -7098,10 +7098,10 @@
         <v>80</v>
       </c>
       <c r="C130" t="n">
-        <v>10468</v>
+        <v>9174</v>
       </c>
       <c r="D130" t="n">
-        <v>10548</v>
+        <v>9254</v>
       </c>
     </row>
     <row r="131">
@@ -7114,10 +7114,10 @@
         <v>80</v>
       </c>
       <c r="C131" t="n">
-        <v>10468</v>
+        <v>9243</v>
       </c>
       <c r="D131" t="n">
-        <v>10548</v>
+        <v>9323</v>
       </c>
     </row>
     <row r="132">
@@ -7130,10 +7130,10 @@
         <v>80</v>
       </c>
       <c r="C132" t="n">
-        <v>10468</v>
+        <v>9211</v>
       </c>
       <c r="D132" t="n">
-        <v>10548</v>
+        <v>9291</v>
       </c>
     </row>
     <row r="133">
@@ -7146,10 +7146,10 @@
         <v>80</v>
       </c>
       <c r="C133" t="n">
-        <v>10468</v>
+        <v>9290</v>
       </c>
       <c r="D133" t="n">
-        <v>10548</v>
+        <v>9370</v>
       </c>
     </row>
     <row r="134">
@@ -7162,10 +7162,10 @@
         <v>80</v>
       </c>
       <c r="C134" t="n">
-        <v>10468</v>
+        <v>9290</v>
       </c>
       <c r="D134" t="n">
-        <v>10548</v>
+        <v>9370</v>
       </c>
     </row>
     <row r="135">
@@ -7178,10 +7178,10 @@
         <v>80</v>
       </c>
       <c r="C135" t="n">
-        <v>10468</v>
+        <v>9395</v>
       </c>
       <c r="D135" t="n">
-        <v>10548</v>
+        <v>9475</v>
       </c>
     </row>
     <row r="136">
@@ -7194,10 +7194,10 @@
         <v>80</v>
       </c>
       <c r="C136" t="n">
-        <v>10468</v>
+        <v>9316</v>
       </c>
       <c r="D136" t="n">
-        <v>10548</v>
+        <v>9396</v>
       </c>
     </row>
     <row r="137">
@@ -7210,10 +7210,10 @@
         <v>80</v>
       </c>
       <c r="C137" t="n">
-        <v>10468</v>
+        <v>9292</v>
       </c>
       <c r="D137" t="n">
-        <v>10548</v>
+        <v>9372</v>
       </c>
     </row>
     <row r="138">
@@ -7226,10 +7226,10 @@
         <v>1094</v>
       </c>
       <c r="C138" t="n">
-        <v>9484</v>
+        <v>8129</v>
       </c>
       <c r="D138" t="n">
-        <v>10578</v>
+        <v>9223</v>
       </c>
     </row>
     <row r="139">
@@ -7242,10 +7242,10 @@
         <v>1094</v>
       </c>
       <c r="C139" t="n">
-        <v>9484</v>
+        <v>8303</v>
       </c>
       <c r="D139" t="n">
-        <v>10578</v>
+        <v>9397</v>
       </c>
     </row>
     <row r="140">
@@ -7258,10 +7258,10 @@
         <v>2065</v>
       </c>
       <c r="C140" t="n">
-        <v>8505</v>
+        <v>7364</v>
       </c>
       <c r="D140" t="n">
-        <v>10570</v>
+        <v>9429</v>
       </c>
     </row>
     <row r="141">
@@ -7274,10 +7274,10 @@
         <v>2065</v>
       </c>
       <c r="C141" t="n">
-        <v>8505</v>
+        <v>7491</v>
       </c>
       <c r="D141" t="n">
-        <v>10570</v>
+        <v>9556</v>
       </c>
     </row>
     <row r="142">
@@ -7290,10 +7290,10 @@
         <v>2065</v>
       </c>
       <c r="C142" t="n">
-        <v>8505</v>
+        <v>7565</v>
       </c>
       <c r="D142" t="n">
-        <v>10570</v>
+        <v>9630</v>
       </c>
     </row>
     <row r="143">
@@ -7306,10 +7306,10 @@
         <v>3048</v>
       </c>
       <c r="C143" t="n">
-        <v>7552</v>
+        <v>6612</v>
       </c>
       <c r="D143" t="n">
-        <v>10600</v>
+        <v>9660</v>
       </c>
     </row>
     <row r="144">
@@ -7322,10 +7322,10 @@
         <v>4095</v>
       </c>
       <c r="C144" t="n">
-        <v>6554</v>
+        <v>5573</v>
       </c>
       <c r="D144" t="n">
-        <v>10649</v>
+        <v>9668</v>
       </c>
     </row>
     <row r="145">
@@ -7338,10 +7338,10 @@
         <v>4095</v>
       </c>
       <c r="C145" t="n">
-        <v>6554</v>
+        <v>5506</v>
       </c>
       <c r="D145" t="n">
-        <v>10649</v>
+        <v>9601</v>
       </c>
     </row>
     <row r="146">
@@ -7354,10 +7354,10 @@
         <v>5106</v>
       </c>
       <c r="C146" t="n">
-        <v>5560</v>
+        <v>4540</v>
       </c>
       <c r="D146" t="n">
-        <v>10666</v>
+        <v>9646</v>
       </c>
     </row>
     <row r="147">
@@ -7370,10 +7370,10 @@
         <v>5106</v>
       </c>
       <c r="C147" t="n">
-        <v>5560</v>
+        <v>4559</v>
       </c>
       <c r="D147" t="n">
-        <v>10666</v>
+        <v>9665</v>
       </c>
     </row>
     <row r="148">
@@ -7386,10 +7386,10 @@
         <v>5106</v>
       </c>
       <c r="C148" t="n">
-        <v>5560</v>
+        <v>4515</v>
       </c>
       <c r="D148" t="n">
-        <v>10666</v>
+        <v>9621</v>
       </c>
     </row>
     <row r="149">
@@ -7402,10 +7402,10 @@
         <v>4114</v>
       </c>
       <c r="C149" t="n">
-        <v>6552</v>
+        <v>5491</v>
       </c>
       <c r="D149" t="n">
-        <v>10666</v>
+        <v>9605</v>
       </c>
     </row>
     <row r="150">
@@ -7418,10 +7418,10 @@
         <v>4114</v>
       </c>
       <c r="C150" t="n">
-        <v>6552</v>
+        <v>5524</v>
       </c>
       <c r="D150" t="n">
-        <v>10666</v>
+        <v>9638</v>
       </c>
     </row>
     <row r="151">
@@ -7434,10 +7434,10 @@
         <v>3121</v>
       </c>
       <c r="C151" t="n">
-        <v>7545</v>
+        <v>6459</v>
       </c>
       <c r="D151" t="n">
-        <v>10666</v>
+        <v>9580</v>
       </c>
     </row>
     <row r="152">
@@ -7450,10 +7450,10 @@
         <v>1134</v>
       </c>
       <c r="C152" t="n">
-        <v>9530</v>
+        <v>8456</v>
       </c>
       <c r="D152" t="n">
-        <v>10664</v>
+        <v>9590</v>
       </c>
     </row>
     <row r="153">
@@ -7466,10 +7466,10 @@
         <v>270</v>
       </c>
       <c r="C153" t="n">
-        <v>10393</v>
+        <v>9147</v>
       </c>
       <c r="D153" t="n">
-        <v>10663</v>
+        <v>9417</v>
       </c>
     </row>
     <row r="154">
@@ -7482,10 +7482,10 @@
         <v>270</v>
       </c>
       <c r="C154" t="n">
-        <v>10393</v>
+        <v>9096</v>
       </c>
       <c r="D154" t="n">
-        <v>10663</v>
+        <v>9366</v>
       </c>
     </row>
     <row r="155">
@@ -7498,10 +7498,10 @@
         <v>270</v>
       </c>
       <c r="C155" t="n">
-        <v>10393</v>
+        <v>9175</v>
       </c>
       <c r="D155" t="n">
-        <v>10663</v>
+        <v>9445</v>
       </c>
     </row>
     <row r="156">
@@ -7514,10 +7514,10 @@
         <v>270</v>
       </c>
       <c r="C156" t="n">
-        <v>10393</v>
+        <v>9258</v>
       </c>
       <c r="D156" t="n">
-        <v>10663</v>
+        <v>9528</v>
       </c>
     </row>
     <row r="157">
@@ -7530,10 +7530,10 @@
         <v>270</v>
       </c>
       <c r="C157" t="n">
-        <v>10393</v>
+        <v>9470</v>
       </c>
       <c r="D157" t="n">
-        <v>10663</v>
+        <v>9740</v>
       </c>
     </row>
     <row r="158">
@@ -7546,10 +7546,10 @@
         <v>270</v>
       </c>
       <c r="C158" t="n">
-        <v>10393</v>
+        <v>9464</v>
       </c>
       <c r="D158" t="n">
-        <v>10663</v>
+        <v>9734</v>
       </c>
     </row>
     <row r="159">
@@ -7562,10 +7562,10 @@
         <v>270</v>
       </c>
       <c r="C159" t="n">
-        <v>10393</v>
+        <v>9513</v>
       </c>
       <c r="D159" t="n">
-        <v>10663</v>
+        <v>9783</v>
       </c>
     </row>
     <row r="160">
@@ -7578,10 +7578,10 @@
         <v>270</v>
       </c>
       <c r="C160" t="n">
-        <v>10393</v>
+        <v>9734</v>
       </c>
       <c r="D160" t="n">
-        <v>10663</v>
+        <v>10004</v>
       </c>
     </row>
     <row r="161">
@@ -7594,10 +7594,10 @@
         <v>325</v>
       </c>
       <c r="C161" t="n">
-        <v>10384</v>
+        <v>9667</v>
       </c>
       <c r="D161" t="n">
-        <v>10709</v>
+        <v>9992</v>
       </c>
     </row>
     <row r="162">
@@ -7610,10 +7610,10 @@
         <v>1395</v>
       </c>
       <c r="C162" t="n">
-        <v>9395</v>
+        <v>8645</v>
       </c>
       <c r="D162" t="n">
-        <v>10790</v>
+        <v>10040</v>
       </c>
     </row>
     <row r="163">
@@ -7626,10 +7626,10 @@
         <v>1395</v>
       </c>
       <c r="C163" t="n">
-        <v>9395</v>
+        <v>8599</v>
       </c>
       <c r="D163" t="n">
-        <v>10790</v>
+        <v>9994</v>
       </c>
     </row>
     <row r="164">
@@ -7642,10 +7642,10 @@
         <v>1502</v>
       </c>
       <c r="C164" t="n">
-        <v>9359</v>
+        <v>8541</v>
       </c>
       <c r="D164" t="n">
-        <v>10861</v>
+        <v>10043</v>
       </c>
     </row>
     <row r="165">
@@ -7658,10 +7658,10 @@
         <v>1502</v>
       </c>
       <c r="C165" t="n">
-        <v>9359</v>
+        <v>8516</v>
       </c>
       <c r="D165" t="n">
-        <v>10861</v>
+        <v>10018</v>
       </c>
     </row>
     <row r="166">
@@ -7674,10 +7674,10 @@
         <v>1502</v>
       </c>
       <c r="C166" t="n">
-        <v>9359</v>
+        <v>8510</v>
       </c>
       <c r="D166" t="n">
-        <v>10861</v>
+        <v>10012</v>
       </c>
     </row>
     <row r="167">
@@ -7690,10 +7690,10 @@
         <v>2423</v>
       </c>
       <c r="C167" t="n">
-        <v>8415</v>
+        <v>7558</v>
       </c>
       <c r="D167" t="n">
-        <v>10838</v>
+        <v>9981</v>
       </c>
     </row>
     <row r="168">
@@ -7706,10 +7706,10 @@
         <v>2423</v>
       </c>
       <c r="C168" t="n">
-        <v>8415</v>
+        <v>7562</v>
       </c>
       <c r="D168" t="n">
-        <v>10838</v>
+        <v>9985</v>
       </c>
     </row>
     <row r="169">
@@ -7722,10 +7722,10 @@
         <v>1430</v>
       </c>
       <c r="C169" t="n">
-        <v>9408</v>
+        <v>8554</v>
       </c>
       <c r="D169" t="n">
-        <v>10838</v>
+        <v>9984</v>
       </c>
     </row>
     <row r="170">
@@ -7738,10 +7738,10 @@
         <v>2330</v>
       </c>
       <c r="C170" t="n">
-        <v>8544</v>
+        <v>7777</v>
       </c>
       <c r="D170" t="n">
-        <v>10874</v>
+        <v>10107</v>
       </c>
     </row>
     <row r="171">
@@ -7754,10 +7754,10 @@
         <v>1367</v>
       </c>
       <c r="C171" t="n">
-        <v>9506</v>
+        <v>8693</v>
       </c>
       <c r="D171" t="n">
-        <v>10873</v>
+        <v>10060</v>
       </c>
     </row>
     <row r="172">
@@ -7770,10 +7770,10 @@
         <v>378</v>
       </c>
       <c r="C172" t="n">
-        <v>10495</v>
+        <v>9665</v>
       </c>
       <c r="D172" t="n">
-        <v>10873</v>
+        <v>10043</v>
       </c>
     </row>
     <row r="173">
@@ -7786,10 +7786,10 @@
         <v>378</v>
       </c>
       <c r="C173" t="n">
-        <v>10495</v>
+        <v>9708</v>
       </c>
       <c r="D173" t="n">
-        <v>10873</v>
+        <v>10086</v>
       </c>
     </row>
     <row r="174">
@@ -7802,10 +7802,10 @@
         <v>1373</v>
       </c>
       <c r="C174" t="n">
-        <v>9503</v>
+        <v>8785</v>
       </c>
       <c r="D174" t="n">
-        <v>10876</v>
+        <v>10158</v>
       </c>
     </row>
     <row r="175">
@@ -7818,10 +7818,10 @@
         <v>1373</v>
       </c>
       <c r="C175" t="n">
-        <v>9503</v>
+        <v>8667</v>
       </c>
       <c r="D175" t="n">
-        <v>10876</v>
+        <v>10040</v>
       </c>
     </row>
     <row r="176">
@@ -7834,10 +7834,10 @@
         <v>1373</v>
       </c>
       <c r="C176" t="n">
-        <v>9503</v>
+        <v>8642</v>
       </c>
       <c r="D176" t="n">
-        <v>10876</v>
+        <v>10015</v>
       </c>
     </row>
     <row r="177">
@@ -7850,10 +7850,10 @@
         <v>3167</v>
       </c>
       <c r="C177" t="n">
-        <v>7693</v>
+        <v>6987</v>
       </c>
       <c r="D177" t="n">
-        <v>10860</v>
+        <v>10154</v>
       </c>
     </row>
     <row r="178">
@@ -7866,10 +7866,10 @@
         <v>3167</v>
       </c>
       <c r="C178" t="n">
-        <v>7693</v>
+        <v>6870</v>
       </c>
       <c r="D178" t="n">
-        <v>10860</v>
+        <v>10037</v>
       </c>
     </row>
     <row r="179">
@@ -7882,10 +7882,10 @@
         <v>3167</v>
       </c>
       <c r="C179" t="n">
-        <v>7693</v>
+        <v>6866</v>
       </c>
       <c r="D179" t="n">
-        <v>10860</v>
+        <v>10033</v>
       </c>
     </row>
     <row r="180">
@@ -7898,10 +7898,10 @@
         <v>3167</v>
       </c>
       <c r="C180" t="n">
-        <v>7693</v>
+        <v>6866</v>
       </c>
       <c r="D180" t="n">
-        <v>10860</v>
+        <v>10033</v>
       </c>
     </row>
     <row r="181">
@@ -7914,10 +7914,10 @@
         <v>1396</v>
       </c>
       <c r="C181" t="n">
-        <v>9462</v>
+        <v>8502</v>
       </c>
       <c r="D181" t="n">
-        <v>10858</v>
+        <v>9898</v>
       </c>
     </row>
     <row r="182">
@@ -7930,10 +7930,10 @@
         <v>1396</v>
       </c>
       <c r="C182" t="n">
-        <v>9462</v>
+        <v>8535</v>
       </c>
       <c r="D182" t="n">
-        <v>10858</v>
+        <v>9931</v>
       </c>
     </row>
     <row r="183">
@@ -7946,10 +7946,10 @@
         <v>1396</v>
       </c>
       <c r="C183" t="n">
-        <v>9462</v>
+        <v>8411</v>
       </c>
       <c r="D183" t="n">
-        <v>10858</v>
+        <v>9807</v>
       </c>
     </row>
     <row r="184">
@@ -7962,10 +7962,10 @@
         <v>1396</v>
       </c>
       <c r="C184" t="n">
-        <v>9462</v>
+        <v>8472</v>
       </c>
       <c r="D184" t="n">
-        <v>10858</v>
+        <v>9868</v>
       </c>
     </row>
     <row r="185">
@@ -7978,10 +7978,10 @@
         <v>578</v>
       </c>
       <c r="C185" t="n">
-        <v>10280</v>
+        <v>9395</v>
       </c>
       <c r="D185" t="n">
-        <v>10858</v>
+        <v>9973</v>
       </c>
     </row>
     <row r="186">
@@ -7994,10 +7994,10 @@
         <v>578</v>
       </c>
       <c r="C186" t="n">
-        <v>10280</v>
+        <v>9372</v>
       </c>
       <c r="D186" t="n">
-        <v>10858</v>
+        <v>9950</v>
       </c>
     </row>
     <row r="187">
@@ -8010,10 +8010,10 @@
         <v>578</v>
       </c>
       <c r="C187" t="n">
-        <v>10280</v>
+        <v>9465</v>
       </c>
       <c r="D187" t="n">
-        <v>10858</v>
+        <v>10043</v>
       </c>
     </row>
     <row r="188">
@@ -8026,10 +8026,10 @@
         <v>578</v>
       </c>
       <c r="C188" t="n">
-        <v>10280</v>
+        <v>9453</v>
       </c>
       <c r="D188" t="n">
-        <v>10858</v>
+        <v>10031</v>
       </c>
     </row>
     <row r="189">
@@ -8042,10 +8042,10 @@
         <v>578</v>
       </c>
       <c r="C189" t="n">
-        <v>10280</v>
+        <v>9326</v>
       </c>
       <c r="D189" t="n">
-        <v>10858</v>
+        <v>9904</v>
       </c>
     </row>
     <row r="190">
@@ -8058,10 +8058,10 @@
         <v>578</v>
       </c>
       <c r="C190" t="n">
-        <v>10280</v>
+        <v>9135</v>
       </c>
       <c r="D190" t="n">
-        <v>10858</v>
+        <v>9713</v>
       </c>
     </row>
     <row r="191">
@@ -8074,10 +8074,10 @@
         <v>578</v>
       </c>
       <c r="C191" t="n">
-        <v>10280</v>
+        <v>9154</v>
       </c>
       <c r="D191" t="n">
-        <v>10858</v>
+        <v>9732</v>
       </c>
     </row>
     <row r="192">
@@ -8090,10 +8090,10 @@
         <v>578</v>
       </c>
       <c r="C192" t="n">
-        <v>10280</v>
+        <v>8909</v>
       </c>
       <c r="D192" t="n">
-        <v>10858</v>
+        <v>9487</v>
       </c>
     </row>
     <row r="193">
@@ -8106,10 +8106,10 @@
         <v>578</v>
       </c>
       <c r="C193" t="n">
-        <v>10280</v>
+        <v>8850</v>
       </c>
       <c r="D193" t="n">
-        <v>10858</v>
+        <v>9428</v>
       </c>
     </row>
     <row r="194">
@@ -8122,10 +8122,10 @@
         <v>578</v>
       </c>
       <c r="C194" t="n">
-        <v>10280</v>
+        <v>8984</v>
       </c>
       <c r="D194" t="n">
-        <v>10858</v>
+        <v>9562</v>
       </c>
     </row>
     <row r="195">
@@ -8138,10 +8138,10 @@
         <v>578</v>
       </c>
       <c r="C195" t="n">
-        <v>10280</v>
+        <v>9185</v>
       </c>
       <c r="D195" t="n">
-        <v>10858</v>
+        <v>9763</v>
       </c>
     </row>
     <row r="196">
@@ -8154,10 +8154,10 @@
         <v>578</v>
       </c>
       <c r="C196" t="n">
-        <v>10280</v>
+        <v>9053</v>
       </c>
       <c r="D196" t="n">
-        <v>10858</v>
+        <v>9631</v>
       </c>
     </row>
     <row r="197">
@@ -8170,10 +8170,10 @@
         <v>578</v>
       </c>
       <c r="C197" t="n">
-        <v>10280</v>
+        <v>9122</v>
       </c>
       <c r="D197" t="n">
-        <v>10858</v>
+        <v>9700</v>
       </c>
     </row>
     <row r="198">
@@ -8186,10 +8186,10 @@
         <v>578</v>
       </c>
       <c r="C198" t="n">
-        <v>10280</v>
+        <v>9085</v>
       </c>
       <c r="D198" t="n">
-        <v>10858</v>
+        <v>9663</v>
       </c>
     </row>
     <row r="199">
@@ -8202,10 +8202,10 @@
         <v>578</v>
       </c>
       <c r="C199" t="n">
-        <v>10280</v>
+        <v>9092</v>
       </c>
       <c r="D199" t="n">
-        <v>10858</v>
+        <v>9670</v>
       </c>
     </row>
     <row r="200">
@@ -8218,10 +8218,10 @@
         <v>578</v>
       </c>
       <c r="C200" t="n">
-        <v>10280</v>
+        <v>9234</v>
       </c>
       <c r="D200" t="n">
-        <v>10858</v>
+        <v>9812</v>
       </c>
     </row>
     <row r="201">
@@ -8234,10 +8234,10 @@
         <v>578</v>
       </c>
       <c r="C201" t="n">
-        <v>10280</v>
+        <v>9057</v>
       </c>
       <c r="D201" t="n">
-        <v>10858</v>
+        <v>9635</v>
       </c>
     </row>
     <row r="202">
@@ -8250,10 +8250,10 @@
         <v>2438</v>
       </c>
       <c r="C202" t="n">
-        <v>8484</v>
+        <v>7368</v>
       </c>
       <c r="D202" t="n">
-        <v>10922</v>
+        <v>9806</v>
       </c>
     </row>
     <row r="203">
@@ -8266,10 +8266,10 @@
         <v>4405</v>
       </c>
       <c r="C203" t="n">
-        <v>6555</v>
+        <v>5516</v>
       </c>
       <c r="D203" t="n">
-        <v>10960</v>
+        <v>9921</v>
       </c>
     </row>
     <row r="204">
@@ -8282,10 +8282,10 @@
         <v>4405</v>
       </c>
       <c r="C204" t="n">
-        <v>6555</v>
+        <v>5512</v>
       </c>
       <c r="D204" t="n">
-        <v>10960</v>
+        <v>9917</v>
       </c>
     </row>
     <row r="205">
@@ -8298,10 +8298,10 @@
         <v>4405</v>
       </c>
       <c r="C205" t="n">
-        <v>6555</v>
+        <v>5561</v>
       </c>
       <c r="D205" t="n">
-        <v>10960</v>
+        <v>9966</v>
       </c>
     </row>
     <row r="206">
@@ -8314,10 +8314,10 @@
         <v>5292</v>
       </c>
       <c r="C206" t="n">
-        <v>5738</v>
+        <v>4661</v>
       </c>
       <c r="D206" t="n">
-        <v>11030</v>
+        <v>9953</v>
       </c>
     </row>
     <row r="207">
@@ -8330,10 +8330,10 @@
         <v>4333</v>
       </c>
       <c r="C207" t="n">
-        <v>6696</v>
+        <v>5594</v>
       </c>
       <c r="D207" t="n">
-        <v>11029</v>
+        <v>9927</v>
       </c>
     </row>
     <row r="208">
@@ -8346,10 +8346,10 @@
         <v>4333</v>
       </c>
       <c r="C208" t="n">
-        <v>6696</v>
+        <v>5618</v>
       </c>
       <c r="D208" t="n">
-        <v>11029</v>
+        <v>9951</v>
       </c>
     </row>
     <row r="209">
@@ -8362,10 +8362,10 @@
         <v>5320</v>
       </c>
       <c r="C209" t="n">
-        <v>5713</v>
+        <v>4660</v>
       </c>
       <c r="D209" t="n">
-        <v>11033</v>
+        <v>9980</v>
       </c>
     </row>
     <row r="210">
@@ -8378,10 +8378,10 @@
         <v>4356</v>
       </c>
       <c r="C210" t="n">
-        <v>6677</v>
+        <v>5538</v>
       </c>
       <c r="D210" t="n">
-        <v>11033</v>
+        <v>9894</v>
       </c>
     </row>
     <row r="211">
@@ -8394,10 +8394,10 @@
         <v>4356</v>
       </c>
       <c r="C211" t="n">
-        <v>6677</v>
+        <v>5553</v>
       </c>
       <c r="D211" t="n">
-        <v>11033</v>
+        <v>9909</v>
       </c>
     </row>
     <row r="212">
@@ -8410,10 +8410,10 @@
         <v>4356</v>
       </c>
       <c r="C212" t="n">
-        <v>6677</v>
+        <v>5529</v>
       </c>
       <c r="D212" t="n">
-        <v>11033</v>
+        <v>9885</v>
       </c>
     </row>
     <row r="213">
@@ -8426,10 +8426,10 @@
         <v>3455</v>
       </c>
       <c r="C213" t="n">
-        <v>7578</v>
+        <v>6511</v>
       </c>
       <c r="D213" t="n">
-        <v>11033</v>
+        <v>9966</v>
       </c>
     </row>
     <row r="214">
@@ -8442,10 +8442,10 @@
         <v>607</v>
       </c>
       <c r="C214" t="n">
-        <v>10424</v>
+        <v>9371</v>
       </c>
       <c r="D214" t="n">
-        <v>11031</v>
+        <v>9978</v>
       </c>
     </row>
     <row r="215">
@@ -8458,10 +8458,10 @@
         <v>607</v>
       </c>
       <c r="C215" t="n">
-        <v>10424</v>
+        <v>9166</v>
       </c>
       <c r="D215" t="n">
-        <v>11031</v>
+        <v>9773</v>
       </c>
     </row>
     <row r="216">
@@ -8474,10 +8474,10 @@
         <v>607</v>
       </c>
       <c r="C216" t="n">
-        <v>10424</v>
+        <v>9024</v>
       </c>
       <c r="D216" t="n">
-        <v>11031</v>
+        <v>9631</v>
       </c>
     </row>
     <row r="217">
@@ -8490,10 +8490,10 @@
         <v>607</v>
       </c>
       <c r="C217" t="n">
-        <v>10424</v>
+        <v>8721</v>
       </c>
       <c r="D217" t="n">
-        <v>11031</v>
+        <v>9328</v>
       </c>
     </row>
     <row r="218">
@@ -8506,10 +8506,10 @@
         <v>607</v>
       </c>
       <c r="C218" t="n">
-        <v>10424</v>
+        <v>8796</v>
       </c>
       <c r="D218" t="n">
-        <v>11031</v>
+        <v>9403</v>
       </c>
     </row>
     <row r="219">
@@ -8522,10 +8522,10 @@
         <v>607</v>
       </c>
       <c r="C219" t="n">
-        <v>10424</v>
+        <v>8816</v>
       </c>
       <c r="D219" t="n">
-        <v>11031</v>
+        <v>9423</v>
       </c>
     </row>
     <row r="220">
@@ -8538,10 +8538,10 @@
         <v>607</v>
       </c>
       <c r="C220" t="n">
-        <v>10424</v>
+        <v>8960</v>
       </c>
       <c r="D220" t="n">
-        <v>11031</v>
+        <v>9567</v>
       </c>
     </row>
     <row r="221">
@@ -8554,10 +8554,10 @@
         <v>607</v>
       </c>
       <c r="C221" t="n">
-        <v>10424</v>
+        <v>9053</v>
       </c>
       <c r="D221" t="n">
-        <v>11031</v>
+        <v>9660</v>
       </c>
     </row>
     <row r="222">
@@ -8570,10 +8570,10 @@
         <v>607</v>
       </c>
       <c r="C222" t="n">
-        <v>10424</v>
+        <v>9104</v>
       </c>
       <c r="D222" t="n">
-        <v>11031</v>
+        <v>9711</v>
       </c>
     </row>
     <row r="223">
@@ -8586,10 +8586,10 @@
         <v>607</v>
       </c>
       <c r="C223" t="n">
-        <v>10424</v>
+        <v>9218</v>
       </c>
       <c r="D223" t="n">
-        <v>11031</v>
+        <v>9825</v>
       </c>
     </row>
     <row r="224">
@@ -8602,10 +8602,10 @@
         <v>607</v>
       </c>
       <c r="C224" t="n">
-        <v>10424</v>
+        <v>9219</v>
       </c>
       <c r="D224" t="n">
-        <v>11031</v>
+        <v>9826</v>
       </c>
     </row>
     <row r="225">
@@ -8618,10 +8618,10 @@
         <v>689</v>
       </c>
       <c r="C225" t="n">
-        <v>10277</v>
+        <v>9591</v>
       </c>
       <c r="D225" t="n">
-        <v>10966</v>
+        <v>10280</v>
       </c>
     </row>
     <row r="226">
@@ -8634,10 +8634,10 @@
         <v>2779</v>
       </c>
       <c r="C226" t="n">
-        <v>8327</v>
+        <v>7628</v>
       </c>
       <c r="D226" t="n">
-        <v>11106</v>
+        <v>10407</v>
       </c>
     </row>
     <row r="227">
@@ -8650,10 +8650,10 @@
         <v>6511</v>
       </c>
       <c r="C227" t="n">
-        <v>4609</v>
+        <v>3889</v>
       </c>
       <c r="D227" t="n">
-        <v>11120</v>
+        <v>10400</v>
       </c>
     </row>
     <row r="228">
@@ -8666,10 +8666,10 @@
         <v>6511</v>
       </c>
       <c r="C228" t="n">
-        <v>4609</v>
+        <v>3810</v>
       </c>
       <c r="D228" t="n">
-        <v>11120</v>
+        <v>10321</v>
       </c>
     </row>
     <row r="229">
@@ -8682,10 +8682,10 @@
         <v>6511</v>
       </c>
       <c r="C229" t="n">
-        <v>4609</v>
+        <v>3937</v>
       </c>
       <c r="D229" t="n">
-        <v>11120</v>
+        <v>10448</v>
       </c>
     </row>
     <row r="230">
@@ -8698,10 +8698,10 @@
         <v>8349</v>
       </c>
       <c r="C230" t="n">
-        <v>2780</v>
+        <v>2233</v>
       </c>
       <c r="D230" t="n">
-        <v>11129</v>
+        <v>10582</v>
       </c>
     </row>
     <row r="231">
@@ -8714,10 +8714,10 @@
         <v>8349</v>
       </c>
       <c r="C231" t="n">
-        <v>2780</v>
+        <v>2164</v>
       </c>
       <c r="D231" t="n">
-        <v>11129</v>
+        <v>10513</v>
       </c>
     </row>
     <row r="232">
@@ -8730,10 +8730,10 @@
         <v>8349</v>
       </c>
       <c r="C232" t="n">
-        <v>2780</v>
+        <v>2118</v>
       </c>
       <c r="D232" t="n">
-        <v>11129</v>
+        <v>10467</v>
       </c>
     </row>
     <row r="233">
@@ -8746,10 +8746,10 @@
         <v>7677</v>
       </c>
       <c r="C233" t="n">
-        <v>3452</v>
+        <v>2785</v>
       </c>
       <c r="D233" t="n">
-        <v>11129</v>
+        <v>10462</v>
       </c>
     </row>
     <row r="234">
@@ -8762,10 +8762,10 @@
         <v>6837</v>
       </c>
       <c r="C234" t="n">
-        <v>4291</v>
+        <v>3603</v>
       </c>
       <c r="D234" t="n">
-        <v>11128</v>
+        <v>10440</v>
       </c>
     </row>
     <row r="235">
@@ -8778,10 +8778,10 @@
         <v>6837</v>
       </c>
       <c r="C235" t="n">
-        <v>4291</v>
+        <v>3660</v>
       </c>
       <c r="D235" t="n">
-        <v>11128</v>
+        <v>10497</v>
       </c>
     </row>
     <row r="236">
@@ -8794,10 +8794,10 @@
         <v>6837</v>
       </c>
       <c r="C236" t="n">
-        <v>4291</v>
+        <v>3738</v>
       </c>
       <c r="D236" t="n">
-        <v>11128</v>
+        <v>10575</v>
       </c>
     </row>
     <row r="237">
@@ -8810,10 +8810,10 @@
         <v>6837</v>
       </c>
       <c r="C237" t="n">
-        <v>4291</v>
+        <v>3723</v>
       </c>
       <c r="D237" t="n">
-        <v>11128</v>
+        <v>10560</v>
       </c>
     </row>
     <row r="238">
@@ -8826,10 +8826,10 @@
         <v>6837</v>
       </c>
       <c r="C238" t="n">
-        <v>4291</v>
+        <v>3723</v>
       </c>
       <c r="D238" t="n">
-        <v>11128</v>
+        <v>10560</v>
       </c>
     </row>
     <row r="239">
@@ -8842,10 +8842,10 @@
         <v>5872</v>
       </c>
       <c r="C239" t="n">
-        <v>5256</v>
+        <v>4687</v>
       </c>
       <c r="D239" t="n">
-        <v>11128</v>
+        <v>10559</v>
       </c>
     </row>
     <row r="240">
@@ -8858,10 +8858,10 @@
         <v>5873</v>
       </c>
       <c r="C240" t="n">
-        <v>5276</v>
+        <v>4631</v>
       </c>
       <c r="D240" t="n">
-        <v>11149</v>
+        <v>10504</v>
       </c>
     </row>
     <row r="241">
@@ -8874,10 +8874,10 @@
         <v>5873</v>
       </c>
       <c r="C241" t="n">
-        <v>5276</v>
+        <v>4683</v>
       </c>
       <c r="D241" t="n">
-        <v>11149</v>
+        <v>10556</v>
       </c>
     </row>
     <row r="242">
@@ -8890,10 +8890,10 @@
         <v>5873</v>
       </c>
       <c r="C242" t="n">
-        <v>5276</v>
+        <v>4736</v>
       </c>
       <c r="D242" t="n">
-        <v>11149</v>
+        <v>10609</v>
       </c>
     </row>
     <row r="243">
@@ -8906,10 +8906,10 @@
         <v>5873</v>
       </c>
       <c r="C243" t="n">
-        <v>5276</v>
+        <v>4790</v>
       </c>
       <c r="D243" t="n">
-        <v>11149</v>
+        <v>10663</v>
       </c>
     </row>
     <row r="244">
@@ -8922,10 +8922,10 @@
         <v>7468</v>
       </c>
       <c r="C244" t="n">
-        <v>3742</v>
+        <v>3241</v>
       </c>
       <c r="D244" t="n">
-        <v>11210</v>
+        <v>10709</v>
       </c>
     </row>
     <row r="245">
@@ -8938,10 +8938,10 @@
         <v>7468</v>
       </c>
       <c r="C245" t="n">
-        <v>3742</v>
+        <v>3213</v>
       </c>
       <c r="D245" t="n">
-        <v>11210</v>
+        <v>10681</v>
       </c>
     </row>
     <row r="246">
@@ -8954,10 +8954,10 @@
         <v>6715</v>
       </c>
       <c r="C246" t="n">
-        <v>4516</v>
+        <v>3987</v>
       </c>
       <c r="D246" t="n">
-        <v>11231</v>
+        <v>10702</v>
       </c>
     </row>
     <row r="247">
@@ -8970,10 +8970,10 @@
         <v>6715</v>
       </c>
       <c r="C247" t="n">
-        <v>4516</v>
+        <v>3993</v>
       </c>
       <c r="D247" t="n">
-        <v>11231</v>
+        <v>10708</v>
       </c>
     </row>
     <row r="248">
@@ -8986,10 +8986,10 @@
         <v>5832</v>
       </c>
       <c r="C248" t="n">
-        <v>5398</v>
+        <v>4881</v>
       </c>
       <c r="D248" t="n">
-        <v>11230</v>
+        <v>10713</v>
       </c>
     </row>
     <row r="249">
@@ -9002,10 +9002,10 @@
         <v>5832</v>
       </c>
       <c r="C249" t="n">
-        <v>5398</v>
+        <v>4881</v>
       </c>
       <c r="D249" t="n">
-        <v>11230</v>
+        <v>10713</v>
       </c>
     </row>
     <row r="250">
@@ -9018,10 +9018,10 @@
         <v>5832</v>
       </c>
       <c r="C250" t="n">
-        <v>5398</v>
+        <v>4862</v>
       </c>
       <c r="D250" t="n">
-        <v>11230</v>
+        <v>10694</v>
       </c>
     </row>
     <row r="251">
@@ -9034,10 +9034,10 @@
         <v>5832</v>
       </c>
       <c r="C251" t="n">
-        <v>5398</v>
+        <v>4896</v>
       </c>
       <c r="D251" t="n">
-        <v>11230</v>
+        <v>10728</v>
       </c>
     </row>
     <row r="252">
@@ -9050,10 +9050,10 @@
         <v>4883</v>
       </c>
       <c r="C252" t="n">
-        <v>6346</v>
+        <v>5843</v>
       </c>
       <c r="D252" t="n">
-        <v>11229</v>
+        <v>10726</v>
       </c>
     </row>
     <row r="253">
@@ -9066,10 +9066,10 @@
         <v>3998</v>
       </c>
       <c r="C253" t="n">
-        <v>7231</v>
+        <v>6759</v>
       </c>
       <c r="D253" t="n">
-        <v>11229</v>
+        <v>10757</v>
       </c>
     </row>
     <row r="254">
@@ -9082,10 +9082,10 @@
         <v>447</v>
       </c>
       <c r="C254" t="n">
-        <v>10781</v>
+        <v>10293</v>
       </c>
       <c r="D254" t="n">
-        <v>11228</v>
+        <v>10740</v>
       </c>
     </row>
     <row r="255">
@@ -9098,10 +9098,10 @@
         <v>260</v>
       </c>
       <c r="C255" t="n">
-        <v>10994</v>
+        <v>10378</v>
       </c>
       <c r="D255" t="n">
-        <v>11254</v>
+        <v>10638</v>
       </c>
     </row>
     <row r="256">
@@ -9114,10 +9114,10 @@
         <v>260</v>
       </c>
       <c r="C256" t="n">
-        <v>10994</v>
+        <v>10258</v>
       </c>
       <c r="D256" t="n">
-        <v>11254</v>
+        <v>10518</v>
       </c>
     </row>
     <row r="257">
@@ -9130,10 +9130,10 @@
         <v>260</v>
       </c>
       <c r="C257" t="n">
-        <v>10994</v>
+        <v>10340</v>
       </c>
       <c r="D257" t="n">
-        <v>11254</v>
+        <v>10600</v>
       </c>
     </row>
     <row r="258">
@@ -9146,10 +9146,10 @@
         <v>260</v>
       </c>
       <c r="C258" t="n">
-        <v>10994</v>
+        <v>10341</v>
       </c>
       <c r="D258" t="n">
-        <v>11254</v>
+        <v>10601</v>
       </c>
     </row>
     <row r="259">
@@ -9162,10 +9162,10 @@
         <v>260</v>
       </c>
       <c r="C259" t="n">
-        <v>10994</v>
+        <v>10341</v>
       </c>
       <c r="D259" t="n">
-        <v>11254</v>
+        <v>10601</v>
       </c>
     </row>
     <row r="260">
@@ -9178,10 +9178,10 @@
         <v>260</v>
       </c>
       <c r="C260" t="n">
-        <v>10994</v>
+        <v>10371</v>
       </c>
       <c r="D260" t="n">
-        <v>11254</v>
+        <v>10631</v>
       </c>
     </row>
     <row r="261">
@@ -9194,10 +9194,10 @@
         <v>954</v>
       </c>
       <c r="C261" t="n">
-        <v>10318</v>
+        <v>9702</v>
       </c>
       <c r="D261" t="n">
-        <v>11272</v>
+        <v>10656</v>
       </c>
     </row>
     <row r="262">
@@ -9210,10 +9210,10 @@
         <v>954</v>
       </c>
       <c r="C262" t="n">
-        <v>10318</v>
+        <v>9684</v>
       </c>
       <c r="D262" t="n">
-        <v>11272</v>
+        <v>10638</v>
       </c>
     </row>
     <row r="263">
@@ -9226,10 +9226,10 @@
         <v>954</v>
       </c>
       <c r="C263" t="n">
-        <v>10318</v>
+        <v>9734</v>
       </c>
       <c r="D263" t="n">
-        <v>11272</v>
+        <v>10688</v>
       </c>
     </row>
     <row r="264">
@@ -9242,10 +9242,10 @@
         <v>954</v>
       </c>
       <c r="C264" t="n">
-        <v>10318</v>
+        <v>9734</v>
       </c>
       <c r="D264" t="n">
-        <v>11272</v>
+        <v>10688</v>
       </c>
     </row>
     <row r="265">
@@ -9258,10 +9258,10 @@
         <v>162</v>
       </c>
       <c r="C265" t="n">
-        <v>11109</v>
+        <v>10479</v>
       </c>
       <c r="D265" t="n">
-        <v>11271</v>
+        <v>10641</v>
       </c>
     </row>
     <row r="266">
@@ -9274,10 +9274,10 @@
         <v>367</v>
       </c>
       <c r="C266" t="n">
-        <v>10970</v>
+        <v>10404</v>
       </c>
       <c r="D266" t="n">
-        <v>11337</v>
+        <v>10771</v>
       </c>
     </row>
     <row r="267">
@@ -9290,10 +9290,10 @@
         <v>1348</v>
       </c>
       <c r="C267" t="n">
-        <v>10033</v>
+        <v>9571</v>
       </c>
       <c r="D267" t="n">
-        <v>11381</v>
+        <v>10919</v>
       </c>
     </row>
     <row r="268">
@@ -9306,10 +9306,10 @@
         <v>2326</v>
       </c>
       <c r="C268" t="n">
-        <v>9087</v>
+        <v>8620</v>
       </c>
       <c r="D268" t="n">
-        <v>11413</v>
+        <v>10946</v>
       </c>
     </row>
     <row r="269">
@@ -9322,10 +9322,10 @@
         <v>3205</v>
       </c>
       <c r="C269" t="n">
-        <v>8205</v>
+        <v>7734</v>
       </c>
       <c r="D269" t="n">
-        <v>11410</v>
+        <v>10939</v>
       </c>
     </row>
     <row r="270">
@@ -9338,10 +9338,10 @@
         <v>3205</v>
       </c>
       <c r="C270" t="n">
-        <v>8205</v>
+        <v>7786</v>
       </c>
       <c r="D270" t="n">
-        <v>11410</v>
+        <v>10991</v>
       </c>
     </row>
     <row r="271">
@@ -9354,10 +9354,10 @@
         <v>2252</v>
       </c>
       <c r="C271" t="n">
-        <v>9157</v>
+        <v>8753</v>
       </c>
       <c r="D271" t="n">
-        <v>11409</v>
+        <v>11005</v>
       </c>
     </row>
     <row r="272">
@@ -9370,10 +9370,10 @@
         <v>2252</v>
       </c>
       <c r="C272" t="n">
-        <v>9157</v>
+        <v>8758</v>
       </c>
       <c r="D272" t="n">
-        <v>11409</v>
+        <v>11010</v>
       </c>
     </row>
     <row r="273">
@@ -9386,10 +9386,10 @@
         <v>577</v>
       </c>
       <c r="C273" t="n">
-        <v>10830</v>
+        <v>10417</v>
       </c>
       <c r="D273" t="n">
-        <v>11407</v>
+        <v>10994</v>
       </c>
     </row>
     <row r="274">
@@ -9402,10 +9402,10 @@
         <v>577</v>
       </c>
       <c r="C274" t="n">
-        <v>10830</v>
+        <v>10349</v>
       </c>
       <c r="D274" t="n">
-        <v>11407</v>
+        <v>10926</v>
       </c>
     </row>
     <row r="275">
@@ -9418,10 +9418,10 @@
         <v>577</v>
       </c>
       <c r="C275" t="n">
-        <v>10830</v>
+        <v>10349</v>
       </c>
       <c r="D275" t="n">
-        <v>11407</v>
+        <v>10926</v>
       </c>
     </row>
     <row r="276">
@@ -9434,10 +9434,10 @@
         <v>577</v>
       </c>
       <c r="C276" t="n">
-        <v>10830</v>
+        <v>10370</v>
       </c>
       <c r="D276" t="n">
-        <v>11407</v>
+        <v>10947</v>
       </c>
     </row>
     <row r="277">
@@ -9450,10 +9450,10 @@
         <v>577</v>
       </c>
       <c r="C277" t="n">
-        <v>10830</v>
+        <v>10423</v>
       </c>
       <c r="D277" t="n">
-        <v>11407</v>
+        <v>11000</v>
       </c>
     </row>
     <row r="278">
@@ -9466,10 +9466,10 @@
         <v>577</v>
       </c>
       <c r="C278" t="n">
-        <v>10830</v>
+        <v>10371</v>
       </c>
       <c r="D278" t="n">
-        <v>11407</v>
+        <v>10948</v>
       </c>
     </row>
     <row r="279">
@@ -9482,10 +9482,10 @@
         <v>1429</v>
       </c>
       <c r="C279" t="n">
-        <v>10039</v>
+        <v>9500</v>
       </c>
       <c r="D279" t="n">
-        <v>11468</v>
+        <v>10929</v>
       </c>
     </row>
     <row r="280">
@@ -9498,10 +9498,10 @@
         <v>733</v>
       </c>
       <c r="C280" t="n">
-        <v>10734</v>
+        <v>10237</v>
       </c>
       <c r="D280" t="n">
-        <v>11467</v>
+        <v>10970</v>
       </c>
     </row>
     <row r="281">
@@ -9514,10 +9514,10 @@
         <v>1605</v>
       </c>
       <c r="C281" t="n">
-        <v>9883</v>
+        <v>9373</v>
       </c>
       <c r="D281" t="n">
-        <v>11488</v>
+        <v>10978</v>
       </c>
     </row>
     <row r="282">
@@ -9530,10 +9530,10 @@
         <v>788</v>
       </c>
       <c r="C282" t="n">
-        <v>10700</v>
+        <v>9972</v>
       </c>
       <c r="D282" t="n">
-        <v>11488</v>
+        <v>10760</v>
       </c>
     </row>
     <row r="283">
@@ -9546,10 +9546,10 @@
         <v>788</v>
       </c>
       <c r="C283" t="n">
-        <v>10700</v>
+        <v>10089</v>
       </c>
       <c r="D283" t="n">
-        <v>11488</v>
+        <v>10877</v>
       </c>
     </row>
     <row r="284">
@@ -9562,10 +9562,10 @@
         <v>788</v>
       </c>
       <c r="C284" t="n">
-        <v>10700</v>
+        <v>9952</v>
       </c>
       <c r="D284" t="n">
-        <v>11488</v>
+        <v>10740</v>
       </c>
     </row>
     <row r="285">
@@ -9578,10 +9578,10 @@
         <v>788</v>
       </c>
       <c r="C285" t="n">
-        <v>10700</v>
+        <v>9982</v>
       </c>
       <c r="D285" t="n">
-        <v>11488</v>
+        <v>10770</v>
       </c>
     </row>
     <row r="286">
@@ -9594,10 +9594,10 @@
         <v>788</v>
       </c>
       <c r="C286" t="n">
-        <v>10700</v>
+        <v>10096</v>
       </c>
       <c r="D286" t="n">
-        <v>11488</v>
+        <v>10884</v>
       </c>
     </row>
     <row r="287">
@@ -9610,10 +9610,10 @@
         <v>788</v>
       </c>
       <c r="C287" t="n">
-        <v>10700</v>
+        <v>10148</v>
       </c>
       <c r="D287" t="n">
-        <v>11488</v>
+        <v>10936</v>
       </c>
     </row>
     <row r="288">
@@ -9626,10 +9626,10 @@
         <v>788</v>
       </c>
       <c r="C288" t="n">
-        <v>10700</v>
+        <v>10252</v>
       </c>
       <c r="D288" t="n">
-        <v>11488</v>
+        <v>11040</v>
       </c>
     </row>
     <row r="289">
@@ -9642,10 +9642,10 @@
         <v>788</v>
       </c>
       <c r="C289" t="n">
-        <v>10700</v>
+        <v>10294</v>
       </c>
       <c r="D289" t="n">
-        <v>11488</v>
+        <v>11082</v>
       </c>
     </row>
     <row r="290">
@@ -9658,10 +9658,10 @@
         <v>762</v>
       </c>
       <c r="C290" t="n">
-        <v>10808</v>
+        <v>10419</v>
       </c>
       <c r="D290" t="n">
-        <v>11570</v>
+        <v>11181</v>
       </c>
     </row>
     <row r="291">
@@ -9674,10 +9674,10 @@
         <v>1659</v>
       </c>
       <c r="C291" t="n">
-        <v>9992</v>
+        <v>9549</v>
       </c>
       <c r="D291" t="n">
-        <v>11651</v>
+        <v>11208</v>
       </c>
     </row>
     <row r="292">
@@ -9690,10 +9690,10 @@
         <v>3358</v>
       </c>
       <c r="C292" t="n">
-        <v>8278</v>
+        <v>7860</v>
       </c>
       <c r="D292" t="n">
-        <v>11636</v>
+        <v>11218</v>
       </c>
     </row>
     <row r="293">
@@ -9706,10 +9706,10 @@
         <v>4200</v>
       </c>
       <c r="C293" t="n">
-        <v>7472</v>
+        <v>6986</v>
       </c>
       <c r="D293" t="n">
-        <v>11672</v>
+        <v>11186</v>
       </c>
     </row>
     <row r="294">
@@ -9722,10 +9722,10 @@
         <v>5163</v>
       </c>
       <c r="C294" t="n">
-        <v>6520</v>
+        <v>6035</v>
       </c>
       <c r="D294" t="n">
-        <v>11683</v>
+        <v>11198</v>
       </c>
     </row>
     <row r="295">
@@ -9738,10 +9738,10 @@
         <v>5163</v>
       </c>
       <c r="C295" t="n">
-        <v>6520</v>
+        <v>6035</v>
       </c>
       <c r="D295" t="n">
-        <v>11683</v>
+        <v>11198</v>
       </c>
     </row>
     <row r="296">
@@ -9754,10 +9754,10 @@
         <v>5163</v>
       </c>
       <c r="C296" t="n">
-        <v>6520</v>
+        <v>6021</v>
       </c>
       <c r="D296" t="n">
-        <v>11683</v>
+        <v>11184</v>
       </c>
     </row>
     <row r="297">
@@ -9770,10 +9770,10 @@
         <v>5163</v>
       </c>
       <c r="C297" t="n">
-        <v>6520</v>
+        <v>6118</v>
       </c>
       <c r="D297" t="n">
-        <v>11683</v>
+        <v>11281</v>
       </c>
     </row>
     <row r="298">
@@ -9786,10 +9786,10 @@
         <v>5163</v>
       </c>
       <c r="C298" t="n">
-        <v>6520</v>
+        <v>6101</v>
       </c>
       <c r="D298" t="n">
-        <v>11683</v>
+        <v>11264</v>
       </c>
     </row>
     <row r="299">
@@ -9802,10 +9802,10 @@
         <v>4253</v>
       </c>
       <c r="C299" t="n">
-        <v>7429</v>
+        <v>6964</v>
       </c>
       <c r="D299" t="n">
-        <v>11682</v>
+        <v>11217</v>
       </c>
     </row>
     <row r="300">
@@ -9818,10 +9818,10 @@
         <v>1359</v>
       </c>
       <c r="C300" t="n">
-        <v>10321</v>
+        <v>9866</v>
       </c>
       <c r="D300" t="n">
-        <v>11680</v>
+        <v>11225</v>
       </c>
     </row>
     <row r="301">
@@ -9834,10 +9834,10 @@
         <v>410</v>
       </c>
       <c r="C301" t="n">
-        <v>11270</v>
+        <v>10815</v>
       </c>
       <c r="D301" t="n">
-        <v>11680</v>
+        <v>11225</v>
       </c>
     </row>
     <row r="302">
@@ -9850,10 +9850,10 @@
         <v>410</v>
       </c>
       <c r="C302" t="n">
-        <v>11270</v>
+        <v>10846</v>
       </c>
       <c r="D302" t="n">
-        <v>11680</v>
+        <v>11256</v>
       </c>
     </row>
     <row r="303">
@@ -9866,10 +9866,10 @@
         <v>410</v>
       </c>
       <c r="C303" t="n">
-        <v>11270</v>
+        <v>10726</v>
       </c>
       <c r="D303" t="n">
-        <v>11680</v>
+        <v>11136</v>
       </c>
     </row>
     <row r="304">
@@ -9882,10 +9882,10 @@
         <v>410</v>
       </c>
       <c r="C304" t="n">
-        <v>11270</v>
+        <v>10613</v>
       </c>
       <c r="D304" t="n">
-        <v>11680</v>
+        <v>11023</v>
       </c>
     </row>
     <row r="305">
@@ -9898,10 +9898,10 @@
         <v>410</v>
       </c>
       <c r="C305" t="n">
-        <v>11270</v>
+        <v>10775</v>
       </c>
       <c r="D305" t="n">
-        <v>11680</v>
+        <v>11185</v>
       </c>
     </row>
     <row r="306">
@@ -9914,10 +9914,10 @@
         <v>1079</v>
       </c>
       <c r="C306" t="n">
-        <v>10574</v>
+        <v>10032</v>
       </c>
       <c r="D306" t="n">
-        <v>11653</v>
+        <v>11111</v>
       </c>
     </row>
     <row r="307">
@@ -9930,10 +9930,10 @@
         <v>141</v>
       </c>
       <c r="C307" t="n">
-        <v>11511</v>
+        <v>10919</v>
       </c>
       <c r="D307" t="n">
-        <v>11652</v>
+        <v>11060</v>
       </c>
     </row>
     <row r="308">
@@ -9946,10 +9946,10 @@
         <v>141</v>
       </c>
       <c r="C308" t="n">
-        <v>11511</v>
+        <v>10839</v>
       </c>
       <c r="D308" t="n">
-        <v>11652</v>
+        <v>10980</v>
       </c>
     </row>
     <row r="309">
@@ -9962,10 +9962,10 @@
         <v>354</v>
       </c>
       <c r="C309" t="n">
-        <v>11287</v>
+        <v>10834</v>
       </c>
       <c r="D309" t="n">
-        <v>11641</v>
+        <v>11188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>